<commit_message>
smartmeters and eco measures update
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0875F3-FB44-4C93-83BC-C09C4F3AB6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018BF762-B680-47E5-85A9-6DFE9A433534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,13 +940,13 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1043397/table_252.xlsx</t>
   </si>
   <si>
-    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1047733/Headline_HEE_tables_20_JANUARY_2022.xlsx</t>
-  </si>
-  <si>
     <t>https://www.gov.uk/government/statistics/rhi-monthly-deployment-data-december-2021-annual-edition</t>
   </si>
   <si>
     <t>https://www.electralink.co.uk/2022/01/2021-smart-installations-increase-2020/</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1056549/Headline_HEE_tables_24_February_2022.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1599,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1705,14 +1705,14 @@
         <v>139</v>
       </c>
       <c r="E4" s="24">
-        <v>44531</v>
+        <v>44228</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>159</v>
       </c>
       <c r="G4" s="24">
         <f>DATE(YEAR(E4),MONTH(E4)+1,DAY(E4))</f>
-        <v>44562</v>
+        <v>44256</v>
       </c>
       <c r="H4" s="22" t="s">
         <v>220</v>
@@ -1799,43 +1799,43 @@
     </row>
     <row r="8" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>303</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>263</v>
+        <v>71</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>172</v>
       </c>
       <c r="E8" s="24">
-        <v>44562</v>
+        <v>44593</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>159</v>
       </c>
       <c r="G8" s="24">
         <f>DATE(YEAR(E8),MONTH(E8)+1,DAY(E8))</f>
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>305</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>172</v>
+        <v>52</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>143</v>
       </c>
       <c r="E9" s="24">
         <v>44562</v>
@@ -1848,30 +1848,30 @@
         <v>44593</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
-        <v>51</v>
+        <v>183</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>304</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>143</v>
+        <v>182</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>170</v>
       </c>
       <c r="E10" s="24">
-        <v>44562</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>159</v>
+        <v>44228</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="G10" s="24">
-        <f>DATE(YEAR(E10),MONTH(E10)+1,DAY(E10))</f>
+        <f>DATE(YEAR(E10)+1,MONTH(E10),DAY(E10))</f>
         <v>44593</v>
       </c>
       <c r="H10" s="22" t="s">
@@ -1880,25 +1880,25 @@
     </row>
     <row r="11" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
-        <v>183</v>
+        <v>49</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>170</v>
+        <v>50</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>142</v>
       </c>
       <c r="E11" s="24">
-        <v>44228</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>158</v>
+        <v>44501</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>157</v>
       </c>
       <c r="G11" s="24">
-        <f>DATE(YEAR(E11)+1,MONTH(E11),DAY(E11))</f>
+        <f>DATE(YEAR(E11),MONTH(E11)+3,DAY(E11))</f>
         <v>44593</v>
       </c>
       <c r="H11" s="22" t="s">
@@ -1906,52 +1906,52 @@
       </c>
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="24">
+      <c r="A12" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="E12" s="32">
         <v>44501</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="32">
         <f>DATE(YEAR(E12),MONTH(E12)+3,DAY(E12))</f>
         <v>44593</v>
       </c>
-      <c r="H12" s="22" t="s">
-        <v>220</v>
+      <c r="H12" s="30" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>213</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>265</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="E13" s="32">
+      <c r="A13" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13" s="24">
         <v>44501</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="24">
         <f>DATE(YEAR(E13),MONTH(E13)+3,DAY(E13))</f>
         <v>44593</v>
       </c>
@@ -1961,83 +1961,83 @@
     </row>
     <row r="14" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
       <c r="E14" s="24">
-        <v>44501</v>
+        <v>44409</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>157</v>
+        <v>288</v>
       </c>
       <c r="G14" s="24">
-        <f>DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
+        <f>DATE(YEAR(E14),MONTH(E14)+6,DAY(E14))</f>
         <v>44593</v>
       </c>
-      <c r="H14" s="30" t="s">
-        <v>222</v>
+      <c r="H14" s="22" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>201</v>
+        <v>117</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>249</v>
+        <v>118</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>261</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>203</v>
+        <v>261</v>
       </c>
       <c r="E15" s="24">
-        <v>44409</v>
+        <v>44501</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>288</v>
+        <v>157</v>
       </c>
       <c r="G15" s="24">
-        <f>DATE(YEAR(E15),MONTH(E15)+6,DAY(E15))</f>
+        <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
         <v>44593</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>261</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>263</v>
       </c>
       <c r="E16" s="24">
-        <v>44501</v>
+        <v>44593</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="G16" s="24">
-        <f t="shared" ref="G16:G34" si="0">DATE(YEAR(E16),MONTH(E16)+3,DAY(E16))</f>
-        <v>44593</v>
+        <f>DATE(YEAR(E16),MONTH(E16)+1,DAY(E16))</f>
+        <v>44621</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -2060,7 +2060,7 @@
         <v>157</v>
       </c>
       <c r="G17" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E17),MONTH(E17)+3,DAY(E17))</f>
         <v>44621</v>
       </c>
       <c r="H17" s="22" t="s">
@@ -2087,7 +2087,7 @@
         <v>157</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E18),MONTH(E18)+3,DAY(E18))</f>
         <v>44621</v>
       </c>
       <c r="H18" s="22" t="s">
@@ -2114,7 +2114,7 @@
         <v>157</v>
       </c>
       <c r="G19" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
         <v>44621</v>
       </c>
       <c r="H19" s="22" t="s">
@@ -2141,7 +2141,7 @@
         <v>157</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E20),MONTH(E20)+3,DAY(E20))</f>
         <v>44621</v>
       </c>
       <c r="H20" s="22" t="s">
@@ -2168,7 +2168,7 @@
         <v>157</v>
       </c>
       <c r="G21" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
         <v>44621</v>
       </c>
       <c r="H21" s="22" t="s">
@@ -2195,7 +2195,7 @@
         <v>157</v>
       </c>
       <c r="G22" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E22),MONTH(E22)+3,DAY(E22))</f>
         <v>44621</v>
       </c>
       <c r="H22" s="22" t="s">
@@ -2222,7 +2222,7 @@
         <v>157</v>
       </c>
       <c r="G23" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E23),MONTH(E23)+3,DAY(E23))</f>
         <v>44621</v>
       </c>
       <c r="H23" s="22" t="s">
@@ -2249,7 +2249,7 @@
         <v>157</v>
       </c>
       <c r="G24" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E24),MONTH(E24)+3,DAY(E24))</f>
         <v>44621</v>
       </c>
       <c r="H24" s="22" t="s">
@@ -2276,7 +2276,7 @@
         <v>157</v>
       </c>
       <c r="G25" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
         <v>44621</v>
       </c>
       <c r="H25" s="22" t="s">
@@ -2303,7 +2303,7 @@
         <v>157</v>
       </c>
       <c r="G26" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E26),MONTH(E26)+3,DAY(E26))</f>
         <v>44621</v>
       </c>
       <c r="H26" s="22" t="s">
@@ -2330,7 +2330,7 @@
         <v>157</v>
       </c>
       <c r="G27" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E27),MONTH(E27)+3,DAY(E27))</f>
         <v>44621</v>
       </c>
       <c r="H27" s="22" t="s">
@@ -2357,7 +2357,7 @@
         <v>157</v>
       </c>
       <c r="G28" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E28),MONTH(E28)+3,DAY(E28))</f>
         <v>44621</v>
       </c>
       <c r="H28" s="22" t="s">
@@ -2384,7 +2384,7 @@
         <v>157</v>
       </c>
       <c r="G29" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E29),MONTH(E29)+3,DAY(E29))</f>
         <v>44621</v>
       </c>
       <c r="H29" s="22" t="s">
@@ -2411,7 +2411,7 @@
         <v>157</v>
       </c>
       <c r="G30" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
         <v>44621</v>
       </c>
       <c r="H30" s="22" t="s">
@@ -2436,7 +2436,7 @@
         <v>157</v>
       </c>
       <c r="G31" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E31),MONTH(E31)+3,DAY(E31))</f>
         <v>44621</v>
       </c>
       <c r="H31" s="22" t="s">
@@ -2461,7 +2461,7 @@
         <v>157</v>
       </c>
       <c r="G32" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
         <v>44621</v>
       </c>
       <c r="H32" s="22" t="s">
@@ -2486,7 +2486,7 @@
         <v>157</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E33),MONTH(E33)+3,DAY(E33))</f>
         <v>44621</v>
       </c>
       <c r="H33" s="22" t="s">
@@ -2511,7 +2511,7 @@
         <v>157</v>
       </c>
       <c r="G34" s="24">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E34),MONTH(E34)+3,DAY(E34))</f>
         <v>44621</v>
       </c>
       <c r="H34" s="22" t="s">
@@ -2589,7 +2589,7 @@
         <v>158</v>
       </c>
       <c r="G37" s="24">
-        <f t="shared" ref="G37:G45" si="1">DATE(YEAR(E37)+1,MONTH(E37),DAY(E37))</f>
+        <f>DATE(YEAR(E37)+1,MONTH(E37),DAY(E37))</f>
         <v>44652</v>
       </c>
       <c r="H37" s="22" t="s">
@@ -2616,7 +2616,7 @@
         <v>158</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E38)+1,MONTH(E38),DAY(E38))</f>
         <v>44652</v>
       </c>
       <c r="H38" s="22" t="s">
@@ -2643,7 +2643,7 @@
         <v>158</v>
       </c>
       <c r="G39" s="24">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E39)+1,MONTH(E39),DAY(E39))</f>
         <v>44652</v>
       </c>
       <c r="H39" s="22" t="s">
@@ -2670,7 +2670,7 @@
         <v>158</v>
       </c>
       <c r="G40" s="32">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
         <v>44652</v>
       </c>
       <c r="H40" s="30" t="s">
@@ -2697,7 +2697,7 @@
         <v>158</v>
       </c>
       <c r="G41" s="32">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
         <v>44713</v>
       </c>
       <c r="H41" s="30" t="s">
@@ -2724,7 +2724,7 @@
         <v>158</v>
       </c>
       <c r="G42" s="32">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
         <v>44713</v>
       </c>
       <c r="H42" s="30" t="s">
@@ -2749,7 +2749,7 @@
         <v>158</v>
       </c>
       <c r="G43" s="29">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E43)+1,MONTH(E43),DAY(E43))</f>
         <v>44713</v>
       </c>
       <c r="H43" s="28" t="s">
@@ -2776,7 +2776,7 @@
         <v>158</v>
       </c>
       <c r="G44" s="29">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E44)+1,MONTH(E44),DAY(E44))</f>
         <v>44713</v>
       </c>
       <c r="H44" s="28" t="s">
@@ -2803,7 +2803,7 @@
         <v>158</v>
       </c>
       <c r="G45" s="24">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E45)+1,MONTH(E45),DAY(E45))</f>
         <v>44713</v>
       </c>
       <c r="H45" s="28" t="s">
@@ -2880,7 +2880,7 @@
         <v>158</v>
       </c>
       <c r="G48" s="24">
-        <f t="shared" ref="G48:G53" si="2">DATE(YEAR(E48)+1,MONTH(E48),DAY(E48))</f>
+        <f>DATE(YEAR(E48)+1,MONTH(E48),DAY(E48))</f>
         <v>44743</v>
       </c>
       <c r="H48" s="22" t="s">
@@ -2907,7 +2907,7 @@
         <v>158</v>
       </c>
       <c r="G49" s="24">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E49)+1,MONTH(E49),DAY(E49))</f>
         <v>44743</v>
       </c>
       <c r="H49" s="22" t="s">
@@ -2934,7 +2934,7 @@
         <v>158</v>
       </c>
       <c r="G50" s="24">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E50)+1,MONTH(E50),DAY(E50))</f>
         <v>44743</v>
       </c>
       <c r="H50" s="22" t="s">
@@ -2961,7 +2961,7 @@
         <v>158</v>
       </c>
       <c r="G51" s="24">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E51)+1,MONTH(E51),DAY(E51))</f>
         <v>44743</v>
       </c>
       <c r="H51" s="22" t="s">
@@ -2988,7 +2988,7 @@
         <v>158</v>
       </c>
       <c r="G52" s="24">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E52)+1,MONTH(E52),DAY(E52))</f>
         <v>44743</v>
       </c>
       <c r="H52" s="22" t="s">
@@ -3015,7 +3015,7 @@
         <v>158</v>
       </c>
       <c r="G53" s="24">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E53)+1,MONTH(E53),DAY(E53))</f>
         <v>44774</v>
       </c>
       <c r="H53" s="22" t="s">
@@ -3068,7 +3068,7 @@
         <v>158</v>
       </c>
       <c r="G55" s="24">
-        <f t="shared" ref="G55:G67" si="3">DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
+        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
         <v>44805</v>
       </c>
       <c r="H55" s="22" t="s">
@@ -3095,7 +3095,7 @@
         <v>158</v>
       </c>
       <c r="G56" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
         <v>44805</v>
       </c>
       <c r="H56" s="22" t="s">
@@ -3122,7 +3122,7 @@
         <v>158</v>
       </c>
       <c r="G57" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
         <v>44805</v>
       </c>
       <c r="H57" s="22" t="s">
@@ -3149,7 +3149,7 @@
         <v>158</v>
       </c>
       <c r="G58" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
         <v>44805</v>
       </c>
       <c r="H58" s="22" t="s">
@@ -3176,7 +3176,7 @@
         <v>158</v>
       </c>
       <c r="G59" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
         <v>44805</v>
       </c>
       <c r="H59" s="22" t="s">
@@ -3203,7 +3203,7 @@
         <v>158</v>
       </c>
       <c r="G60" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
         <v>44866</v>
       </c>
       <c r="H60" s="22" t="s">
@@ -3230,7 +3230,7 @@
         <v>158</v>
       </c>
       <c r="G61" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
         <v>44866</v>
       </c>
       <c r="H61" s="22" t="s">
@@ -3257,7 +3257,7 @@
         <v>158</v>
       </c>
       <c r="G62" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E62)+1,MONTH(E62),DAY(E62))</f>
         <v>44896</v>
       </c>
       <c r="H62" s="22" t="s">
@@ -3284,7 +3284,7 @@
         <v>158</v>
       </c>
       <c r="G63" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E63)+1,MONTH(E63),DAY(E63))</f>
         <v>44896</v>
       </c>
       <c r="H63" s="22" t="s">
@@ -3311,7 +3311,7 @@
         <v>158</v>
       </c>
       <c r="G64" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
         <v>44896</v>
       </c>
       <c r="H64" s="22" t="s">
@@ -3338,7 +3338,7 @@
         <v>158</v>
       </c>
       <c r="G65" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
         <v>44896</v>
       </c>
       <c r="H65" s="22" t="s">
@@ -3365,7 +3365,7 @@
         <v>158</v>
       </c>
       <c r="G66" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E66)+1,MONTH(E66),DAY(E66))</f>
         <v>44896</v>
       </c>
       <c r="H66" s="22" t="s">
@@ -3392,7 +3392,7 @@
         <v>158</v>
       </c>
       <c r="G67" s="24">
-        <f t="shared" si="3"/>
+        <f>DATE(YEAR(E67)+1,MONTH(E67),DAY(E67))</f>
         <v>44927</v>
       </c>
       <c r="H67" s="22" t="s">
@@ -3841,7 +3841,7 @@
     <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
     <hyperlink ref="D62" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
     <hyperlink ref="D30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D12" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D11" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
     <hyperlink ref="D65" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
     <hyperlink ref="D58" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
     <hyperlink ref="D59" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
@@ -3865,8 +3865,8 @@
     <hyperlink ref="D51" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
     <hyperlink ref="C24" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
     <hyperlink ref="D4" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="D14" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D9" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="D13" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D8" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
     <hyperlink ref="C68" r:id="rId49" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
     <hyperlink ref="D67" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
     <hyperlink ref="D42" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
@@ -3875,7 +3875,7 @@
     <hyperlink ref="D35" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
     <hyperlink ref="C70" r:id="rId55" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
     <hyperlink ref="C73" r:id="rId56" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
-    <hyperlink ref="D11" r:id="rId57" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
+    <hyperlink ref="D10" r:id="rId57" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
     <hyperlink ref="C34" r:id="rId58" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
     <hyperlink ref="D83" r:id="rId59" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
     <hyperlink ref="C83" r:id="rId60" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
@@ -3884,47 +3884,48 @@
     <hyperlink ref="C82" r:id="rId63" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
     <hyperlink ref="D57" r:id="rId64" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
     <hyperlink ref="D56" r:id="rId65" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
-    <hyperlink ref="D15" r:id="rId66" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
+    <hyperlink ref="D14" r:id="rId66" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
     <hyperlink ref="C76" r:id="rId67" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
     <hyperlink ref="C48" r:id="rId68" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
     <hyperlink ref="D29" r:id="rId69" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
     <hyperlink ref="D18" r:id="rId70" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
     <hyperlink ref="C54" r:id="rId71" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="C6" r:id="rId72" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="D10" r:id="rId73" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C35" r:id="rId74" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2021/03/oil-and-gas-production-statistics-2019/documents/oil-and-gas-production-statistics-2019---tables/oil-and-gas-production-statistics-2019---tables/govscot%3Adocument/Oil%2Band%2BGas%2BProduction%2B2019%2B-%2Bpublication%2Btables.xlsx?forceDownload=true" xr:uid="{EFFB3F7D-992D-403B-9018-45F56D2F9DE7}"/>
-    <hyperlink ref="C59" r:id="rId75" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D8" r:id="rId76" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
-    <hyperlink ref="C85" r:id="rId77" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
-    <hyperlink ref="C30" r:id="rId78" xr:uid="{2CD20F64-59CA-40E1-BDC9-2AE5808A14A7}"/>
-    <hyperlink ref="D64" r:id="rId79" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C23" r:id="rId80" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
-    <hyperlink ref="C63" r:id="rId81" xr:uid="{0452CD0A-EB9C-4B25-88AF-06E4876A2427}"/>
-    <hyperlink ref="D61" r:id="rId82" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
-    <hyperlink ref="C2" r:id="rId83" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D36" r:id="rId84" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
-    <hyperlink ref="C53" r:id="rId85" xr:uid="{E75D3585-4283-4149-B12A-500F1C77C046}"/>
-    <hyperlink ref="D76" r:id="rId86" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
-    <hyperlink ref="D3" r:id="rId87" xr:uid="{DC015219-0BD9-4A0B-AAA2-E97E313B87A6}"/>
-    <hyperlink ref="C3" r:id="rId88" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
-    <hyperlink ref="D81" r:id="rId89" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
-    <hyperlink ref="D85" r:id="rId90" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
-    <hyperlink ref="C74" r:id="rId91" xr:uid="{CCF6F9E7-8F70-4D1E-8597-F9646028F25D}"/>
-    <hyperlink ref="C36" r:id="rId92" xr:uid="{E2847BE0-806F-44DF-8C46-A67DFFC9BC0F}"/>
-    <hyperlink ref="C55" r:id="rId93" xr:uid="{2FE37BBE-E63B-4784-9429-160F41B36C00}"/>
-    <hyperlink ref="C62" r:id="rId94" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D25" r:id="rId95" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D26" r:id="rId96" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C25" r:id="rId97" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C28" r:id="rId98" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C20" r:id="rId99" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C4" r:id="rId100" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
-    <hyperlink ref="C9" r:id="rId101" xr:uid="{83E17A80-470B-4ECF-8B23-E05D4B48DAFC}"/>
+    <hyperlink ref="D9" r:id="rId72" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C35" r:id="rId73" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2021/03/oil-and-gas-production-statistics-2019/documents/oil-and-gas-production-statistics-2019---tables/oil-and-gas-production-statistics-2019---tables/govscot%3Adocument/Oil%2Band%2BGas%2BProduction%2B2019%2B-%2Bpublication%2Btables.xlsx?forceDownload=true" xr:uid="{EFFB3F7D-992D-403B-9018-45F56D2F9DE7}"/>
+    <hyperlink ref="C59" r:id="rId74" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
+    <hyperlink ref="D16" r:id="rId75" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="C85" r:id="rId76" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
+    <hyperlink ref="C30" r:id="rId77" xr:uid="{2CD20F64-59CA-40E1-BDC9-2AE5808A14A7}"/>
+    <hyperlink ref="D64" r:id="rId78" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
+    <hyperlink ref="C23" r:id="rId79" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="C63" r:id="rId80" xr:uid="{0452CD0A-EB9C-4B25-88AF-06E4876A2427}"/>
+    <hyperlink ref="D61" r:id="rId81" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
+    <hyperlink ref="C2" r:id="rId82" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
+    <hyperlink ref="D36" r:id="rId83" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="C53" r:id="rId84" xr:uid="{E75D3585-4283-4149-B12A-500F1C77C046}"/>
+    <hyperlink ref="D76" r:id="rId85" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
+    <hyperlink ref="D3" r:id="rId86" xr:uid="{DC015219-0BD9-4A0B-AAA2-E97E313B87A6}"/>
+    <hyperlink ref="C3" r:id="rId87" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
+    <hyperlink ref="D81" r:id="rId88" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
+    <hyperlink ref="D85" r:id="rId89" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
+    <hyperlink ref="C74" r:id="rId90" xr:uid="{CCF6F9E7-8F70-4D1E-8597-F9646028F25D}"/>
+    <hyperlink ref="C36" r:id="rId91" xr:uid="{E2847BE0-806F-44DF-8C46-A67DFFC9BC0F}"/>
+    <hyperlink ref="C55" r:id="rId92" xr:uid="{2FE37BBE-E63B-4784-9429-160F41B36C00}"/>
+    <hyperlink ref="C62" r:id="rId93" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
+    <hyperlink ref="D25" r:id="rId94" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D26" r:id="rId95" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C25" r:id="rId96" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C28" r:id="rId97" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C20" r:id="rId98" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C4" r:id="rId99" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C8" r:id="rId100" xr:uid="{83E17A80-470B-4ECF-8B23-E05D4B48DAFC}"/>
+    <hyperlink ref="C6" r:id="rId101" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
+    <hyperlink ref="C16" r:id="rId102" xr:uid="{E035FF6A-D6FD-4586-B36D-13C716E1E0D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId102"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId103"/>
   <tableParts count="1">
-    <tablePart r:id="rId103"/>
+    <tablePart r:id="rId104"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
smart meters, daily demand edits
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B49930-760E-4C4C-A7BE-BEF7A9E977B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5324E67F-4A37-459D-A96B-6421E3C346B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="307">
   <si>
     <t>Code</t>
   </si>
@@ -811,9 +811,6 @@
     <t>https://www.gov.uk/government/statistics/renewable-fuel-statistics-2020-final-report</t>
   </si>
   <si>
-    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2021/11/gdp-quarterly-national-accounts-2021-q2/documents/quarterly-national-accounts-2021-quarter-2---other-summary-tables/quarterly-national-accounts-2021-quarter-2---other-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2021%2BQ2%2B-%2BOther%2BSummary%2BTables.xlsx</t>
-  </si>
-  <si>
     <t>https://energysavingtrust.org.uk/wp-content/uploads/2021/10/Renewable-heat-in-Scotland-2020-report-version-2.pdf</t>
   </si>
   <si>
@@ -937,9 +934,6 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1043397/table_252.xlsx</t>
   </si>
   <si>
-    <t>https://www.electralink.co.uk/2022/01/2021-smart-installations-increase-2020/</t>
-  </si>
-  <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1056549/Headline_HEE_tables_24_February_2022.xlsx</t>
   </si>
   <si>
@@ -947,6 +941,15 @@
   </si>
   <si>
     <t>https://www.ofgem.gov.uk/sites/default/files/2022-02/Default_tarif_cap_level_v1.10.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.electralink.co.uk/2022/02/jan-smart-installs-increase-24-pc-yoy/</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/02/gdp-quarterly-national-accounts-2021-q3/documents/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/govscot%3Adocument/%25282%2529%2B-%2BQNAS%2B2021%2BQ3%2B-%2BOther%2BSummary%2BTables.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.scot/collections/economy-statistics/#quarterlygrossdomesticproduct(gdp)</t>
   </si>
 </sst>
 </file>
@@ -1702,20 +1705,20 @@
         <v>38</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>139</v>
       </c>
       <c r="E4" s="23">
-        <v>44228</v>
+        <v>44593</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>159</v>
       </c>
       <c r="G4" s="23">
         <f>DATE(YEAR(E4),MONTH(E4)+1,DAY(E4))</f>
-        <v>44256</v>
+        <v>44621</v>
       </c>
       <c r="H4" s="21" t="s">
         <v>220</v>
@@ -1808,7 +1811,7 @@
         <v>50</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>142</v>
@@ -1835,10 +1838,10 @@
         <v>213</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E9" s="31">
         <v>44501</v>
@@ -1888,21 +1891,21 @@
       <c r="B11" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>260</v>
+      <c r="C11" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>306</v>
       </c>
       <c r="E11" s="23">
-        <v>44501</v>
+        <v>44593</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>157</v>
       </c>
       <c r="G11" s="23">
         <f>DATE(YEAR(E11),MONTH(E11)+3,DAY(E11))</f>
-        <v>44593</v>
+        <v>44682</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>223</v>
@@ -1916,7 +1919,7 @@
         <v>71</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>172</v>
@@ -1943,7 +1946,7 @@
         <v>52</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>143</v>
@@ -1970,10 +1973,10 @@
         <v>28</v>
       </c>
       <c r="C14" s="40" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E14" s="23">
         <v>44593</v>
@@ -1997,7 +2000,7 @@
         <v>44</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>156</v>
@@ -2009,7 +2012,7 @@
         <v>157</v>
       </c>
       <c r="G15" s="23">
-        <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
+        <f t="shared" ref="G15:G32" si="0">DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
         <v>44621</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -2024,7 +2027,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>140</v>
@@ -2036,7 +2039,7 @@
         <v>157</v>
       </c>
       <c r="G16" s="23">
-        <f>DATE(YEAR(E16),MONTH(E16)+3,DAY(E16))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H16" s="21" t="s">
@@ -2045,13 +2048,13 @@
     </row>
     <row r="17" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D17" s="41" t="s">
         <v>140</v>
@@ -2063,7 +2066,7 @@
         <v>157</v>
       </c>
       <c r="G17" s="23">
-        <f>DATE(YEAR(E17),MONTH(E17)+3,DAY(E17))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -2072,13 +2075,13 @@
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D18" s="41" t="s">
         <v>140</v>
@@ -2090,7 +2093,7 @@
         <v>157</v>
       </c>
       <c r="G18" s="23">
-        <f>DATE(YEAR(E18),MONTH(E18)+3,DAY(E18))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -2105,7 +2108,7 @@
         <v>64</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>133</v>
@@ -2117,7 +2120,7 @@
         <v>157</v>
       </c>
       <c r="G19" s="23">
-        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H19" s="21" t="s">
@@ -2132,7 +2135,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>133</v>
@@ -2144,7 +2147,7 @@
         <v>157</v>
       </c>
       <c r="G20" s="23">
-        <f>DATE(YEAR(E20),MONTH(E20)+3,DAY(E20))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H20" s="21" t="s">
@@ -2159,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D21" s="22" t="s">
         <v>133</v>
@@ -2171,7 +2174,7 @@
         <v>157</v>
       </c>
       <c r="G21" s="23">
-        <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H21" s="21" t="s">
@@ -2186,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>133</v>
@@ -2198,7 +2201,7 @@
         <v>157</v>
       </c>
       <c r="G22" s="23">
-        <f>DATE(YEAR(E22),MONTH(E22)+3,DAY(E22))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H22" s="21" t="s">
@@ -2207,13 +2210,13 @@
     </row>
     <row r="23" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
+        <v>292</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>293</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>294</v>
       </c>
       <c r="D23" s="22" t="s">
         <v>133</v>
@@ -2225,7 +2228,7 @@
         <v>157</v>
       </c>
       <c r="G23" s="23">
-        <f>DATE(YEAR(E23),MONTH(E23)+3,DAY(E23))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H23" s="21" t="s">
@@ -2234,13 +2237,13 @@
     </row>
     <row r="24" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>133</v>
@@ -2252,7 +2255,7 @@
         <v>157</v>
       </c>
       <c r="G24" s="23">
-        <f>DATE(YEAR(E24),MONTH(E24)+3,DAY(E24))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H24" s="21" t="s">
@@ -2267,7 +2270,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>136</v>
@@ -2279,7 +2282,7 @@
         <v>157</v>
       </c>
       <c r="G25" s="23">
-        <f>DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H25" s="21" t="s">
@@ -2294,7 +2297,7 @@
         <v>40</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>140</v>
@@ -2306,7 +2309,7 @@
         <v>157</v>
       </c>
       <c r="G26" s="23">
-        <f>DATE(YEAR(E26),MONTH(E26)+3,DAY(E26))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H26" s="21" t="s">
@@ -2333,7 +2336,7 @@
         <v>157</v>
       </c>
       <c r="G27" s="23">
-        <f>DATE(YEAR(E27),MONTH(E27)+3,DAY(E27))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H27" s="21" t="s">
@@ -2348,7 +2351,7 @@
         <v>48</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>141</v>
@@ -2360,7 +2363,7 @@
         <v>157</v>
       </c>
       <c r="G28" s="23">
-        <f>DATE(YEAR(E28),MONTH(E28)+3,DAY(E28))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H28" s="21" t="s">
@@ -2385,7 +2388,7 @@
         <v>157</v>
       </c>
       <c r="G29" s="23">
-        <f>DATE(YEAR(E29),MONTH(E29)+3,DAY(E29))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H29" s="21" t="s">
@@ -2410,7 +2413,7 @@
         <v>157</v>
       </c>
       <c r="G30" s="23">
-        <f>DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H30" s="21" t="s">
@@ -2435,7 +2438,7 @@
         <v>157</v>
       </c>
       <c r="G31" s="23">
-        <f>DATE(YEAR(E31),MONTH(E31)+3,DAY(E31))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H31" s="21" t="s">
@@ -2460,7 +2463,7 @@
         <v>157</v>
       </c>
       <c r="G32" s="23">
-        <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
+        <f t="shared" si="0"/>
         <v>44621</v>
       </c>
       <c r="H32" s="21" t="s">
@@ -2501,10 +2504,10 @@
         <v>210</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E34" s="23">
         <v>44531</v>
@@ -2538,7 +2541,7 @@
         <v>158</v>
       </c>
       <c r="G35" s="23">
-        <f>DATE(YEAR(E35)+1,MONTH(E35),DAY(E35))</f>
+        <f t="shared" ref="G35:G43" si="1">DATE(YEAR(E35)+1,MONTH(E35),DAY(E35))</f>
         <v>44652</v>
       </c>
       <c r="H35" s="21" t="s">
@@ -2565,7 +2568,7 @@
         <v>158</v>
       </c>
       <c r="G36" s="23">
-        <f>DATE(YEAR(E36)+1,MONTH(E36),DAY(E36))</f>
+        <f t="shared" si="1"/>
         <v>44652</v>
       </c>
       <c r="H36" s="21" t="s">
@@ -2592,7 +2595,7 @@
         <v>158</v>
       </c>
       <c r="G37" s="23">
-        <f>DATE(YEAR(E37)+1,MONTH(E37),DAY(E37))</f>
+        <f t="shared" si="1"/>
         <v>44652</v>
       </c>
       <c r="H37" s="21" t="s">
@@ -2619,7 +2622,7 @@
         <v>158</v>
       </c>
       <c r="G38" s="31">
-        <f>DATE(YEAR(E38)+1,MONTH(E38),DAY(E38))</f>
+        <f t="shared" si="1"/>
         <v>44652</v>
       </c>
       <c r="H38" s="29" t="s">
@@ -2646,7 +2649,7 @@
         <v>158</v>
       </c>
       <c r="G39" s="31">
-        <f>DATE(YEAR(E39)+1,MONTH(E39),DAY(E39))</f>
+        <f t="shared" si="1"/>
         <v>44713</v>
       </c>
       <c r="H39" s="29" t="s">
@@ -2673,7 +2676,7 @@
         <v>158</v>
       </c>
       <c r="G40" s="31">
-        <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
+        <f t="shared" si="1"/>
         <v>44713</v>
       </c>
       <c r="H40" s="29" t="s">
@@ -2698,7 +2701,7 @@
         <v>158</v>
       </c>
       <c r="G41" s="31">
-        <f>DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
+        <f t="shared" si="1"/>
         <v>44713</v>
       </c>
       <c r="H41" s="29" t="s">
@@ -2725,7 +2728,7 @@
         <v>158</v>
       </c>
       <c r="G42" s="31">
-        <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
+        <f t="shared" si="1"/>
         <v>44713</v>
       </c>
       <c r="H42" s="29" t="s">
@@ -2752,7 +2755,7 @@
         <v>158</v>
       </c>
       <c r="G43" s="28">
-        <f>DATE(YEAR(E43)+1,MONTH(E43),DAY(E43))</f>
+        <f t="shared" si="1"/>
         <v>44713</v>
       </c>
       <c r="H43" s="27" t="s">
@@ -2952,7 +2955,7 @@
         <v>202</v>
       </c>
       <c r="C51" s="45" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D51" s="25" t="s">
         <v>203</v>
@@ -2961,7 +2964,7 @@
         <v>44593</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G51" s="23">
         <f>DATE(YEAR(E51),MONTH(E51)+6,DAY(E51))</f>
@@ -2979,7 +2982,7 @@
         <v>98</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>160</v>
@@ -3035,7 +3038,7 @@
         <v>255</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E54" s="31">
         <v>44440</v>
@@ -3044,7 +3047,7 @@
         <v>158</v>
       </c>
       <c r="G54" s="23">
-        <f>DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
+        <f t="shared" ref="G54:G66" si="2">DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
         <v>44805</v>
       </c>
       <c r="H54" s="21" t="s">
@@ -3071,7 +3074,7 @@
         <v>158</v>
       </c>
       <c r="G55" s="23">
-        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H55" s="21" t="s">
@@ -3098,7 +3101,7 @@
         <v>158</v>
       </c>
       <c r="G56" s="23">
-        <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H56" s="21" t="s">
@@ -3125,7 +3128,7 @@
         <v>158</v>
       </c>
       <c r="G57" s="23">
-        <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H57" s="21" t="s">
@@ -3152,7 +3155,7 @@
         <v>158</v>
       </c>
       <c r="G58" s="23">
-        <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H58" s="21" t="s">
@@ -3167,7 +3170,7 @@
         <v>62</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>148</v>
@@ -3179,7 +3182,7 @@
         <v>158</v>
       </c>
       <c r="G59" s="23">
-        <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
+        <f t="shared" si="2"/>
         <v>44866</v>
       </c>
       <c r="H59" s="21" t="s">
@@ -3194,10 +3197,10 @@
         <v>78</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E60" s="23">
         <v>44501</v>
@@ -3206,7 +3209,7 @@
         <v>158</v>
       </c>
       <c r="G60" s="23">
-        <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
+        <f t="shared" si="2"/>
         <v>44866</v>
       </c>
       <c r="H60" s="21" t="s">
@@ -3221,7 +3224,7 @@
         <v>36</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D61" s="22" t="s">
         <v>138</v>
@@ -3233,7 +3236,7 @@
         <v>158</v>
       </c>
       <c r="G61" s="23">
-        <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H61" s="21" t="s">
@@ -3248,7 +3251,7 @@
         <v>19</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>135</v>
@@ -3260,7 +3263,7 @@
         <v>158</v>
       </c>
       <c r="G62" s="23">
-        <f>DATE(YEAR(E62)+1,MONTH(E62),DAY(E62))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H62" s="21" t="s">
@@ -3275,7 +3278,7 @@
         <v>24</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D63" s="22" t="s">
         <v>147</v>
@@ -3287,7 +3290,7 @@
         <v>158</v>
       </c>
       <c r="G63" s="23">
-        <f>DATE(YEAR(E63)+1,MONTH(E63),DAY(E63))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H63" s="21" t="s">
@@ -3302,7 +3305,7 @@
         <v>54</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>144</v>
@@ -3314,7 +3317,7 @@
         <v>158</v>
       </c>
       <c r="G64" s="23">
-        <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H64" s="21" t="s">
@@ -3329,7 +3332,7 @@
         <v>60</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>147</v>
@@ -3341,7 +3344,7 @@
         <v>158</v>
       </c>
       <c r="G65" s="23">
-        <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H65" s="21" t="s">
@@ -3368,7 +3371,7 @@
         <v>158</v>
       </c>
       <c r="G66" s="23">
-        <f>DATE(YEAR(E66)+1,MONTH(E66),DAY(E66))</f>
+        <f t="shared" si="2"/>
         <v>44927</v>
       </c>
       <c r="H66" s="21" t="s">
@@ -3547,10 +3550,10 @@
         <v>76</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D74" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E74" s="23">
         <v>44256</v>
@@ -3598,7 +3601,7 @@
         <v>207</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E76" s="10">
         <v>44044</v>
@@ -3797,23 +3800,23 @@
     </row>
     <row r="85" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B85" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="C85" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="D85" s="9" t="s">
         <v>266</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>267</v>
       </c>
       <c r="E85" s="10">
         <v>44256</v>
       </c>
       <c r="G85" s="10"/>
       <c r="H85" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -3925,11 +3928,13 @@
     <hyperlink ref="C6" r:id="rId101" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
     <hyperlink ref="C14" r:id="rId102" xr:uid="{E035FF6A-D6FD-4586-B36D-13C716E1E0D1}"/>
     <hyperlink ref="C68" r:id="rId103" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
+    <hyperlink ref="C11" r:id="rId104" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/02/gdp-quarterly-national-accounts-2021-q3/documents/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/govscot%3Adocument/%25282%2529%2B-%2BQNAS%2B2021%2BQ3%2B-%2BOther%2BSummary%2BTables.xlsx" xr:uid="{759662E4-5376-4914-8A28-3408811A385D}"/>
+    <hyperlink ref="D11" r:id="rId105" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId104"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId106"/>
   <tableParts count="1">
-    <tablePart r:id="rId105"/>
+    <tablePart r:id="rId107"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
biofuels, energy cutomers, ficed tariffs
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CAAD53-E836-4B1E-82B7-384149EC9F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5C28EF-6EC9-4BB1-AD1B-004EF654C93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -868,9 +868,6 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1043396/table_251.xlsx</t>
   </si>
   <si>
-    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1031152/renewable-energy-planning-database-q3-september-2021.xlsx</t>
-  </si>
-  <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1043383/table_224.xlsx</t>
   </si>
   <si>
@@ -947,6 +944,9 @@
   </si>
   <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1048354/electric-vehicle-charging-device-statistics-january-2022.ods</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1051570/renewable-energy-planning-database-q4-december-2021.csv</t>
   </si>
 </sst>
 </file>
@@ -1116,12 +1116,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1603,7 +1603,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1722,136 +1722,135 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>258</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="E5" s="23">
-        <v>44531</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="23">
-        <f>DATE(YEAR(E5),MONTH(E5)+3,DAY(E5))</f>
+    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="16">
+        <v>44256</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="16">
         <v>44621</v>
       </c>
-      <c r="H5" s="29" t="s">
-        <v>221</v>
+      <c r="H5" s="13" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>138</v>
+        <v>127</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>170</v>
       </c>
       <c r="E6" s="23">
-        <v>44593</v>
+        <v>44256</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" s="23">
-        <f>DATE(YEAR(E6),MONTH(E6)+1,DAY(E6))</f>
-        <v>44621</v>
-      </c>
-      <c r="H6" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="31">
+        <f>DATE(YEAR(E6),MONTH(E6)+3,DAY(E6))</f>
+        <v>44348</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="23">
+        <v>44256</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="23">
+        <f>DATE(YEAR(E7),MONTH(E7)+3,DAY(E7))</f>
+        <v>44348</v>
+      </c>
+      <c r="H7" s="29" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>301</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="E7" s="23">
-        <v>44593</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="G7" s="23">
-        <f>DATE(YEAR(E7),MONTH(E7)+1,DAY(E7))</f>
-        <v>44621</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
     <row r="8" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>52</v>
+      <c r="A8" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8" s="23">
-        <v>44621</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>158</v>
+        <v>44256</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>156</v>
       </c>
       <c r="G8" s="23">
-        <f>DATE(YEAR(E8),MONTH(E8)+1,DAY(E8))</f>
-        <v>44652</v>
-      </c>
-      <c r="H8" s="21" t="s">
+        <f>DATE(YEAR(E8),MONTH(E8)+3,DAY(E8))</f>
+        <v>44348</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>298</v>
+        <v>294</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>293</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E9" s="23">
-        <v>44593</v>
+        <v>139</v>
+      </c>
+      <c r="E9" s="4">
+        <v>44256</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G9" s="23">
-        <f>DATE(YEAR(E9),MONTH(E9)+1,DAY(E9))</f>
-        <v>44621</v>
+        <f>DATE(YEAR(E9),MONTH(E9)+3,DAY(E9))</f>
+        <v>44348</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>219</v>
@@ -1859,26 +1858,26 @@
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="23">
-        <v>44531</v>
+        <v>295</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="4">
+        <v>44256</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G10" s="23">
-        <f t="shared" ref="G10:G27" si="0">DATE(YEAR(E10),MONTH(E10)+3,DAY(E10))</f>
-        <v>44621</v>
+        <f>DATE(YEAR(E10),MONTH(E10)+3,DAY(E10))</f>
+        <v>44348</v>
       </c>
       <c r="H10" s="21" t="s">
         <v>219</v>
@@ -1886,16 +1885,16 @@
     </row>
     <row r="11" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E11" s="23">
         <v>44531</v>
@@ -1904,7 +1903,7 @@
         <v>156</v>
       </c>
       <c r="G11" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E11),MONTH(E11)+3,DAY(E11))</f>
         <v>44621</v>
       </c>
       <c r="H11" s="21" t="s">
@@ -1913,25 +1912,25 @@
     </row>
     <row r="12" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>295</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>294</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="4">
+        <v>65</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="23">
         <v>44531</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G12" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E12),MONTH(E12)+3,DAY(E12))</f>
         <v>44621</v>
       </c>
       <c r="H12" s="21" t="s">
@@ -1940,25 +1939,25 @@
     </row>
     <row r="13" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>296</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="40" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E13" s="4">
+        <v>4</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="23">
         <v>44531</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G13" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E13),MONTH(E13)+3,DAY(E13))</f>
         <v>44621</v>
       </c>
       <c r="H13" s="21" t="s">
@@ -1967,13 +1966,13 @@
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D14" s="22" t="s">
         <v>132</v>
@@ -1985,7 +1984,7 @@
         <v>156</v>
       </c>
       <c r="G14" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
         <v>44621</v>
       </c>
       <c r="H14" s="21" t="s">
@@ -1994,13 +1993,13 @@
     </row>
     <row r="15" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
-        <v>65</v>
+        <v>288</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>66</v>
+        <v>292</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>132</v>
@@ -2012,7 +2011,7 @@
         <v>156</v>
       </c>
       <c r="G15" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
         <v>44621</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -2021,13 +2020,13 @@
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>4</v>
+        <v>287</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>5</v>
+        <v>291</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>132</v>
@@ -2039,7 +2038,7 @@
         <v>156</v>
       </c>
       <c r="G16" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E16),MONTH(E16)+3,DAY(E16))</f>
         <v>44621</v>
       </c>
       <c r="H16" s="21" t="s">
@@ -2048,16 +2047,16 @@
     </row>
     <row r="17" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>273</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>271</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E17" s="23">
         <v>44531</v>
@@ -2066,7 +2065,7 @@
         <v>156</v>
       </c>
       <c r="G17" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E17),MONTH(E17)+3,DAY(E17))</f>
         <v>44621</v>
       </c>
       <c r="H17" s="21" t="s">
@@ -2075,16 +2074,16 @@
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>289</v>
+        <v>39</v>
       </c>
       <c r="B18" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>290</v>
-      </c>
       <c r="D18" s="22" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E18" s="23">
         <v>44531</v>
@@ -2093,7 +2092,7 @@
         <v>156</v>
       </c>
       <c r="G18" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E18),MONTH(E18)+3,DAY(E18))</f>
         <v>44621</v>
       </c>
       <c r="H18" s="21" t="s">
@@ -2101,26 +2100,26 @@
       </c>
     </row>
     <row r="19" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>292</v>
+      <c r="A19" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="23">
+        <v>139</v>
+      </c>
+      <c r="E19" s="31">
         <v>44531</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="43" t="s">
         <v>156</v>
       </c>
       <c r="G19" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
         <v>44621</v>
       </c>
       <c r="H19" s="21" t="s">
@@ -2129,17 +2128,15 @@
     </row>
     <row r="20" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>135</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="26"/>
       <c r="E20" s="23">
         <v>44531</v>
       </c>
@@ -2147,26 +2144,24 @@
         <v>156</v>
       </c>
       <c r="G20" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E20),MONTH(E20)+3,DAY(E20))</f>
         <v>44621</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>139</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="26"/>
       <c r="E21" s="23">
         <v>44531</v>
       </c>
@@ -2174,61 +2169,59 @@
         <v>156</v>
       </c>
       <c r="G21" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
         <v>44621</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="E22" s="23">
+      <c r="A22" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="31">
         <v>44531</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="29" t="s">
         <v>156</v>
       </c>
       <c r="G22" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E22),MONTH(E22)+3,DAY(E22))</f>
         <v>44621</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>140</v>
+        <v>38</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>138</v>
       </c>
       <c r="E23" s="23">
-        <v>44531</v>
+        <v>44593</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G23" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E23),MONTH(E23)+1,DAY(E23))</f>
         <v>44621</v>
       </c>
       <c r="H23" s="21" t="s">
@@ -2237,193 +2230,200 @@
     </row>
     <row r="24" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="26"/>
+        <v>70</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>171</v>
+      </c>
       <c r="E24" s="23">
-        <v>44531</v>
+        <v>44593</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G24" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E24),MONTH(E24)+1,DAY(E24))</f>
         <v>44621</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="D25" s="26"/>
+        <v>28</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>260</v>
+      </c>
       <c r="E25" s="23">
-        <v>44531</v>
+        <v>44593</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G25" s="23">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E25),MONTH(E25)+1,DAY(E25))</f>
         <v>44621</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="26"/>
+        <v>164</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="25"/>
       <c r="E26" s="23">
-        <v>44531</v>
+        <v>44287</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G26" s="23">
-        <f t="shared" si="0"/>
-        <v>44621</v>
+        <f>DATE(YEAR(E26)+1,MONTH(E26),DAY(E26))</f>
+        <v>44652</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="31">
-        <v>44531</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>156</v>
+      <c r="A27" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="23">
+        <v>44287</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>157</v>
       </c>
       <c r="G27" s="23">
-        <f t="shared" si="0"/>
-        <v>44621</v>
+        <f>DATE(YEAR(E27)+1,MONTH(E27),DAY(E27))</f>
+        <v>44652</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>112</v>
+        <v>228</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>245</v>
+        <v>229</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>230</v>
       </c>
       <c r="D28" s="25" t="s">
-        <v>246</v>
+        <v>151</v>
       </c>
       <c r="E28" s="23">
-        <v>44256</v>
-      </c>
-      <c r="F28" s="24" t="s">
+        <v>44287</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>157</v>
       </c>
       <c r="G28" s="23">
-        <v>44621</v>
+        <f>DATE(YEAR(E28)+1,MONTH(E28),DAY(E28))</f>
+        <v>44652</v>
       </c>
       <c r="H28" s="21" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="40" t="s">
-        <v>279</v>
+      <c r="A29" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>210</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="E29" s="23">
-        <v>44562</v>
-      </c>
-      <c r="F29" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="31">
+        <v>44287</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="31">
+        <f>DATE(YEAR(E29)+1,MONTH(E29),DAY(E29))</f>
+        <v>44652</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="E30" s="23">
+        <v>44531</v>
+      </c>
+      <c r="F30" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G29" s="23">
-        <f>DATE(YEAR(E29),MONTH(E29)+3,DAY(E29))</f>
+      <c r="G30" s="23">
+        <f>DATE(YEAR(E30),MONTH(E30)+4,DAY(E30))</f>
         <v>44652</v>
       </c>
-      <c r="H29" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="16">
-        <v>44562</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="G30" s="23">
-        <f>DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
-        <v>44652</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>221</v>
+      <c r="H30" s="21" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>225</v>
+        <v>67</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>231</v>
+        <v>257</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>148</v>
@@ -2443,106 +2443,108 @@
       </c>
     </row>
     <row r="32" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>285</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="E32" s="23">
-        <v>44531</v>
-      </c>
-      <c r="F32" s="24" t="s">
+      <c r="A32" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="16">
+        <v>44562</v>
+      </c>
+      <c r="F32" s="13" t="s">
         <v>156</v>
       </c>
       <c r="G32" s="23">
-        <f>DATE(YEAR(E32),MONTH(E32)+4,DAY(E32))</f>
+        <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
         <v>44652</v>
       </c>
-      <c r="H32" s="21" t="s">
-        <v>224</v>
+      <c r="H32" s="13" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="D33" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>142</v>
+      </c>
       <c r="E33" s="23">
-        <v>44287</v>
+        <v>44621</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G33" s="23">
-        <f>DATE(YEAR(E33)+1,MONTH(E33),DAY(E33))</f>
+        <f>DATE(YEAR(E33),MONTH(E33)+1,DAY(E33))</f>
         <v>44652</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="E34" s="23">
-        <v>44287</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="G34" s="23">
-        <f>DATE(YEAR(E34)+1,MONTH(E34),DAY(E34))</f>
-        <v>44652</v>
-      </c>
-      <c r="H34" s="21" t="s">
-        <v>222</v>
+      <c r="A34" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>304</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>303</v>
+      </c>
+      <c r="E34" s="31">
+        <v>44593</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="31">
+        <f>DATE(YEAR(E34),MONTH(E34)+3,DAY(E34))</f>
+        <v>44682</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
-        <v>228</v>
+        <v>116</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>151</v>
+        <v>117</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>302</v>
       </c>
       <c r="E35" s="23">
-        <v>44287</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>157</v>
+        <v>44593</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>156</v>
       </c>
       <c r="G35" s="23">
-        <f>DATE(YEAR(E35)+1,MONTH(E35),DAY(E35))</f>
-        <v>44652</v>
+        <f>DATE(YEAR(E35),MONTH(E35)+3,DAY(E35))</f>
+        <v>44682</v>
       </c>
       <c r="H35" s="21" t="s">
         <v>222</v>
@@ -2550,97 +2552,95 @@
     </row>
     <row r="36" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>210</v>
+        <v>238</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E36" s="31">
-        <v>44287</v>
+        <v>44348</v>
       </c>
       <c r="F36" s="43" t="s">
         <v>157</v>
       </c>
       <c r="G36" s="31">
         <f>DATE(YEAR(E36)+1,MONTH(E36),DAY(E36))</f>
-        <v>44652</v>
+        <v>44713</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>305</v>
-      </c>
-      <c r="D37" s="49" t="s">
-        <v>304</v>
+        <v>92</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>174</v>
       </c>
       <c r="E37" s="31">
-        <v>44593</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>156</v>
+        <v>44348</v>
+      </c>
+      <c r="F37" s="43" t="s">
+        <v>157</v>
       </c>
       <c r="G37" s="31">
-        <f>DATE(YEAR(E37),MONTH(E37)+3,DAY(E37))</f>
-        <v>44682</v>
+        <f>DATE(YEAR(E37)+1,MONTH(E37),DAY(E37))</f>
+        <v>44713</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="D38" s="45" t="s">
-        <v>303</v>
-      </c>
-      <c r="E38" s="23">
-        <v>44593</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G38" s="23">
-        <f>DATE(YEAR(E38),MONTH(E38)+3,DAY(E38))</f>
-        <v>44682</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>222</v>
+      <c r="A38" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="26"/>
+      <c r="E38" s="31">
+        <v>44348</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" s="31">
+        <f>DATE(YEAR(E38)+1,MONTH(E38),DAY(E38))</f>
+        <v>44713</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>136</v>
+        <v>233</v>
       </c>
       <c r="E39" s="31">
         <v>44348</v>
@@ -2653,21 +2653,21 @@
         <v>44713</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="29" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="D40" s="30" t="s">
-        <v>174</v>
+        <v>103</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>233</v>
       </c>
       <c r="E40" s="31">
         <v>44348</v>
@@ -2680,20 +2680,22 @@
         <v>44713</v>
       </c>
       <c r="H40" s="29" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="29" t="s">
-        <v>93</v>
+        <v>234</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="26"/>
+        <v>235</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>237</v>
+      </c>
       <c r="E41" s="31">
         <v>44348</v>
       </c>
@@ -2701,116 +2703,114 @@
         <v>157</v>
       </c>
       <c r="G41" s="31">
-        <f>DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
         <v>44713</v>
       </c>
       <c r="H41" s="29" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="E42" s="31">
-        <v>44348</v>
-      </c>
-      <c r="F42" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="G42" s="31">
-        <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
-        <v>44713</v>
-      </c>
-      <c r="H42" s="29" t="s">
-        <v>222</v>
-      </c>
+      <c r="A42" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="E42" s="4">
+        <v>44646</v>
+      </c>
+      <c r="F42" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="G42" s="48">
+        <v>44738</v>
+      </c>
+      <c r="H42" s="45"/>
     </row>
     <row r="43" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="44" t="s">
-        <v>232</v>
+        <v>48</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>267</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>233</v>
+        <v>140</v>
       </c>
       <c r="E43" s="28">
-        <v>44348</v>
+        <v>44652</v>
       </c>
       <c r="F43" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G43" s="28">
-        <f>DATE(YEAR(E43)+1,MONTH(E43),DAY(E43))</f>
-        <v>44713</v>
+        <f>DATE(YEAR(E43),MONTH(E43)+3,DAY(E43))</f>
+        <v>44743</v>
       </c>
       <c r="H43" s="27" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C44" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>237</v>
-      </c>
+      <c r="A44" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="26"/>
       <c r="E44" s="23">
-        <v>44348</v>
-      </c>
-      <c r="F44" s="29" t="s">
-        <v>157</v>
+        <v>44652</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>156</v>
       </c>
       <c r="G44" s="28">
-        <v>44713</v>
+        <f>DATE(YEAR(E44),MONTH(E44)+3,DAY(E44))</f>
+        <v>44743</v>
       </c>
       <c r="H44" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" s="23">
+        <v>44652</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G45" s="23">
+        <f>DATE(YEAR(E45),MONTH(E45)+3,DAY(E45))</f>
+        <v>44743</v>
+      </c>
+      <c r="H45" s="27" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="B45" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="C45" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="D45" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="E45" s="4">
-        <v>44646</v>
-      </c>
-      <c r="F45" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="G45" s="4">
-        <v>44738</v>
-      </c>
-      <c r="H45" s="46"/>
     </row>
     <row r="46" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
@@ -2949,29 +2949,28 @@
     </row>
     <row r="51" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21" t="s">
-        <v>200</v>
+        <v>104</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51" s="45" t="s">
-        <v>300</v>
-      </c>
-      <c r="D51" s="25" t="s">
-        <v>202</v>
+        <v>105</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>151</v>
       </c>
       <c r="E51" s="23">
-        <v>44593</v>
+        <v>44287</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>283</v>
+        <v>193</v>
       </c>
       <c r="G51" s="23">
-        <f>DATE(YEAR(E51),MONTH(E51)+6,DAY(E51))</f>
         <v>44774</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -2982,7 +2981,7 @@
         <v>97</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D52" s="22" t="s">
         <v>159</v>
@@ -3003,28 +3002,29 @@
     </row>
     <row r="53" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
-        <v>104</v>
+        <v>200</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D53" s="22" t="s">
-        <v>151</v>
+        <v>201</v>
+      </c>
+      <c r="C53" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="E53" s="23">
-        <v>44287</v>
+        <v>44593</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>193</v>
+        <v>282</v>
       </c>
       <c r="G53" s="23">
+        <f>DATE(YEAR(E53),MONTH(E53)+6,DAY(E53))</f>
         <v>44774</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
@@ -3047,7 +3047,7 @@
         <v>157</v>
       </c>
       <c r="G54" s="23">
-        <f t="shared" ref="G54:G66" si="1">DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
+        <f>DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
         <v>44805</v>
       </c>
       <c r="H54" s="21" t="s">
@@ -3074,7 +3074,7 @@
         <v>157</v>
       </c>
       <c r="G55" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
         <v>44805</v>
       </c>
       <c r="H55" s="21" t="s">
@@ -3101,7 +3101,7 @@
         <v>157</v>
       </c>
       <c r="G56" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
         <v>44805</v>
       </c>
       <c r="H56" s="21" t="s">
@@ -3128,7 +3128,7 @@
         <v>157</v>
       </c>
       <c r="G57" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
         <v>44805</v>
       </c>
       <c r="H57" s="21" t="s">
@@ -3155,7 +3155,7 @@
         <v>157</v>
       </c>
       <c r="G58" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
         <v>44805</v>
       </c>
       <c r="H58" s="21" t="s">
@@ -3163,10 +3163,10 @@
       </c>
     </row>
     <row r="59" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="21" t="s">
+      <c r="A59" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="29" t="s">
         <v>62</v>
       </c>
       <c r="C59" s="22" t="s">
@@ -3175,17 +3175,17 @@
       <c r="D59" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E59" s="23">
+      <c r="E59" s="31">
         <v>44501</v>
       </c>
-      <c r="F59" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="G59" s="23">
-        <f t="shared" si="1"/>
+      <c r="F59" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="G59" s="31">
+        <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
         <v>44866</v>
       </c>
-      <c r="H59" s="21" t="s">
+      <c r="H59" s="29" t="s">
         <v>219</v>
       </c>
     </row>
@@ -3208,11 +3208,11 @@
       <c r="F60" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="G60" s="23">
-        <f t="shared" si="1"/>
+      <c r="G60" s="31">
+        <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
         <v>44866</v>
       </c>
-      <c r="H60" s="21" t="s">
+      <c r="H60" s="29" t="s">
         <v>220</v>
       </c>
     </row>
@@ -3236,7 +3236,7 @@
         <v>157</v>
       </c>
       <c r="G61" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
         <v>44896</v>
       </c>
       <c r="H61" s="21" t="s">
@@ -3263,7 +3263,7 @@
         <v>157</v>
       </c>
       <c r="G62" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E62)+1,MONTH(E62),DAY(E62))</f>
         <v>44896</v>
       </c>
       <c r="H62" s="21" t="s">
@@ -3290,7 +3290,7 @@
         <v>157</v>
       </c>
       <c r="G63" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E63)+1,MONTH(E63),DAY(E63))</f>
         <v>44896</v>
       </c>
       <c r="H63" s="21" t="s">
@@ -3317,7 +3317,7 @@
         <v>157</v>
       </c>
       <c r="G64" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
         <v>44896</v>
       </c>
       <c r="H64" s="21" t="s">
@@ -3344,7 +3344,7 @@
         <v>157</v>
       </c>
       <c r="G65" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
         <v>44896</v>
       </c>
       <c r="H65" s="21" t="s">
@@ -3371,7 +3371,7 @@
         <v>157</v>
       </c>
       <c r="G66" s="23">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E66)+1,MONTH(E66),DAY(E66))</f>
         <v>44927</v>
       </c>
       <c r="H66" s="21" t="s">
@@ -3412,7 +3412,7 @@
       <c r="B68" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="C68" s="45" t="s">
+      <c r="C68" s="44" t="s">
         <v>183</v>
       </c>
       <c r="D68" s="25" t="s">
@@ -3433,66 +3433,66 @@
       </c>
     </row>
     <row r="69" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C69" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="E69" s="20">
-        <v>43831</v>
-      </c>
-      <c r="F69" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="G69" s="20"/>
-      <c r="H69" s="2" t="s">
+      <c r="A69" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E69" s="23">
+        <v>43435</v>
+      </c>
+      <c r="F69" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G69" s="23"/>
+      <c r="H69" s="21" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="E70" s="10">
-        <v>44166</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="G70" s="10"/>
-      <c r="H70" s="6" t="s">
-        <v>219</v>
+      <c r="A70" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="E70" s="23">
+        <v>43447</v>
+      </c>
+      <c r="F70" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G70" s="23"/>
+      <c r="H70" s="21" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C71" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D71" s="6"/>
+      <c r="D71" s="12"/>
       <c r="E71" s="10">
-        <v>43916</v>
+        <v>43466</v>
       </c>
       <c r="F71" s="11" t="s">
         <v>157</v>
@@ -3503,320 +3503,321 @@
       </c>
     </row>
     <row r="72" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" s="12" t="s">
+      <c r="A72" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E72" s="20">
+        <v>43831</v>
+      </c>
+      <c r="F72" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="G72" s="20"/>
+      <c r="H72" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="10">
-        <v>43466</v>
-      </c>
-      <c r="F72" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="G72" s="10"/>
-      <c r="H72" s="6" t="s">
+      <c r="D73" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E73" s="23">
+        <v>43831</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="G73" s="23"/>
+      <c r="H73" s="21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D73" s="9"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="10"/>
-      <c r="H73" s="6" t="s">
+    <row r="74" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E74" s="20">
+        <v>43908</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G74" s="20"/>
+      <c r="H74" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D75" s="6"/>
+      <c r="E75" s="10">
+        <v>43916</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G75" s="10"/>
+      <c r="H75" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D76" s="25"/>
+      <c r="E76" s="23">
+        <v>43950</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="H76" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E77" s="23">
+        <v>43950</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="G77" s="23"/>
+      <c r="H77" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="E78" s="10">
+        <v>44044</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G78" s="10"/>
+      <c r="H78" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="74" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B74" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="D74" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="E74" s="23">
-        <v>44256</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="G74" s="23"/>
-      <c r="H74" s="21" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="B75" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="C75" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="D75" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="E75" s="23">
-        <v>43831</v>
-      </c>
-      <c r="F75" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="G75" s="23"/>
-      <c r="H75" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="E76" s="10">
-        <v>44044</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G76" s="10"/>
-      <c r="H76" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E77" s="10">
-        <v>44256</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="G77" s="10"/>
-      <c r="H77" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B78" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C78" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="D78" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="E78" s="23">
-        <v>43435</v>
-      </c>
-      <c r="F78" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G78" s="23"/>
-      <c r="H78" s="21" t="s">
-        <v>222</v>
-      </c>
-    </row>
     <row r="79" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B79" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="C79" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="D79" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="E79" s="23">
-        <v>43447</v>
-      </c>
-      <c r="F79" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="G79" s="23"/>
-      <c r="H79" s="21" t="s">
-        <v>222</v>
+      <c r="A79" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E79" s="10">
+        <v>44166</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G79" s="10"/>
+      <c r="H79" s="6" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="21" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="C80" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D80" s="25"/>
+        <v>121</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>213</v>
+      </c>
       <c r="E80" s="23">
-        <v>43950</v>
+        <v>44166</v>
       </c>
       <c r="F80" s="24" t="s">
         <v>157</v>
       </c>
       <c r="G80" s="23"/>
       <c r="H80" s="21" t="s">
-        <v>22</v>
+        <v>222</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="21" t="s">
-        <v>120</v>
+        <v>74</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="D81" s="22" t="s">
-        <v>213</v>
+        <v>281</v>
+      </c>
+      <c r="D81" s="25" t="s">
+        <v>281</v>
       </c>
       <c r="E81" s="23">
-        <v>44166</v>
+        <v>44256</v>
       </c>
       <c r="F81" s="24" t="s">
         <v>157</v>
       </c>
       <c r="G81" s="23"/>
       <c r="H81" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B82" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D82" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="E82" s="23">
-        <v>43950</v>
-      </c>
-      <c r="F82" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="G82" s="23"/>
-      <c r="H82" s="21" t="s">
-        <v>222</v>
+      <c r="A82" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="E82" s="10">
+        <v>44256</v>
+      </c>
+      <c r="F82" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G82" s="10"/>
+      <c r="H82" s="6" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="E83" s="20">
-        <v>43908</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G83" s="20"/>
-      <c r="H83" s="2" t="s">
-        <v>222</v>
+      <c r="A83" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E83" s="10">
+        <v>44256</v>
+      </c>
+      <c r="F83" s="6"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="6" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D84" s="19"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="2" t="s">
+      <c r="D85" s="19"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="D85" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E85" s="10">
-        <v>44256</v>
-      </c>
-      <c r="G85" s="10"/>
-      <c r="H85" s="6" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -3825,120 +3826,121 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="D67" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="C66" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C24" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C25" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C26" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C41" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C79" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C36" r:id="rId9" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-statistics-supplementary-tables-2018/documents/physical-commodity-balances-of-oil-gas-and-petroleum-products/physical-commodity-balances-of-oil-gas-and-petroleum-products/govscot%3Adocument/Commodity%2BBalances%2B-%2B1998-2018.xlsx" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C81" r:id="rId10" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D75" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C34" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C38" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C70" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C29" r:id="rId9" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-statistics-supplementary-tables-2018/documents/physical-commodity-balances-of-oil-gas-and-petroleum-products/physical-commodity-balances-of-oil-gas-and-petroleum-products/govscot%3Adocument/Commodity%2BBalances%2B-%2B1998-2018.xlsx" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C80" r:id="rId10" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D73" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C27" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
     <hyperlink ref="D54" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
     <hyperlink ref="D46" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="D10:D12" r:id="rId17" display="https://www.gov.uk/government/statistics/electricity-chapter-5-digest-of-united-kingdom-energy-statistics-dukes" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D39" r:id="rId19" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D36" r:id="rId19" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
     <hyperlink ref="D50" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
     <hyperlink ref="D61" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D29" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D43" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D45" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
     <hyperlink ref="D64" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
     <hyperlink ref="D57" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
     <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
     <hyperlink ref="D65" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
     <hyperlink ref="D59" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D14" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D15" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D30" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D31" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="D77" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="D79" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="D10" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D11" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D12" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D31" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="D32" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="D82" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="D70" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="D29" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="D7" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
     <hyperlink ref="D62" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D21" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D18" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
     <hyperlink ref="D52" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="D82" r:id="rId40" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="D78" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C78" r:id="rId42" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="D77" r:id="rId40" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="D69" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C69" r:id="rId42" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
     <hyperlink ref="D48" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
     <hyperlink ref="D49" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C17" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D6" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="D5" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D7" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C14" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D23" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="D6" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D24" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
     <hyperlink ref="C67" r:id="rId49" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
     <hyperlink ref="D66" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D40" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D34" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D53" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="D28" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="C70" r:id="rId55" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
-    <hyperlink ref="C73" r:id="rId56" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
+    <hyperlink ref="D37" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D27" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D51" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="D5" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="C79" r:id="rId55" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
+    <hyperlink ref="C84" r:id="rId56" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
     <hyperlink ref="D68" r:id="rId57" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
-    <hyperlink ref="C27" r:id="rId58" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
-    <hyperlink ref="D83" r:id="rId59" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
-    <hyperlink ref="C83" r:id="rId60" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
-    <hyperlink ref="D69" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C69" r:id="rId62" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
-    <hyperlink ref="C82" r:id="rId63" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
+    <hyperlink ref="C22" r:id="rId58" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
+    <hyperlink ref="D74" r:id="rId59" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
+    <hyperlink ref="C74" r:id="rId60" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
+    <hyperlink ref="D72" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C72" r:id="rId62" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
+    <hyperlink ref="C77" r:id="rId63" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
     <hyperlink ref="D56" r:id="rId64" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
     <hyperlink ref="D55" r:id="rId65" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
-    <hyperlink ref="D51" r:id="rId66" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
-    <hyperlink ref="C76" r:id="rId67" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
+    <hyperlink ref="D53" r:id="rId66" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
+    <hyperlink ref="C78" r:id="rId67" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
     <hyperlink ref="C46" r:id="rId68" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
-    <hyperlink ref="D22" r:id="rId69" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
-    <hyperlink ref="D11" r:id="rId70" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
-    <hyperlink ref="C53" r:id="rId71" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="D8" r:id="rId72" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C28" r:id="rId73" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2021/03/oil-and-gas-production-statistics-2019/documents/oil-and-gas-production-statistics-2019---tables/oil-and-gas-production-statistics-2019---tables/govscot%3Adocument/Oil%2Band%2BGas%2BProduction%2B2019%2B-%2Bpublication%2Btables.xlsx?forceDownload=true" xr:uid="{EFFB3F7D-992D-403B-9018-45F56D2F9DE7}"/>
+    <hyperlink ref="D19" r:id="rId69" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
+    <hyperlink ref="D8" r:id="rId70" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
+    <hyperlink ref="C51" r:id="rId71" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
+    <hyperlink ref="D33" r:id="rId72" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C5" r:id="rId73" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2021/03/oil-and-gas-production-statistics-2019/documents/oil-and-gas-production-statistics-2019---tables/oil-and-gas-production-statistics-2019---tables/govscot%3Adocument/Oil%2Band%2BGas%2BProduction%2B2019%2B-%2Bpublication%2Btables.xlsx?forceDownload=true" xr:uid="{EFFB3F7D-992D-403B-9018-45F56D2F9DE7}"/>
     <hyperlink ref="C58" r:id="rId74" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D9" r:id="rId75" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
-    <hyperlink ref="C85" r:id="rId76" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
-    <hyperlink ref="C23" r:id="rId77" xr:uid="{2CD20F64-59CA-40E1-BDC9-2AE5808A14A7}"/>
+    <hyperlink ref="D25" r:id="rId75" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="C83" r:id="rId76" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
+    <hyperlink ref="C43" r:id="rId77" xr:uid="{2CD20F64-59CA-40E1-BDC9-2AE5808A14A7}"/>
     <hyperlink ref="D63" r:id="rId78" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C16" r:id="rId79" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="C13" r:id="rId79" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
     <hyperlink ref="C62" r:id="rId80" xr:uid="{0452CD0A-EB9C-4B25-88AF-06E4876A2427}"/>
     <hyperlink ref="D60" r:id="rId81" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
     <hyperlink ref="C2" r:id="rId82" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D32" r:id="rId83" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="D30" r:id="rId83" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
     <hyperlink ref="C52" r:id="rId84" xr:uid="{E75D3585-4283-4149-B12A-500F1C77C046}"/>
-    <hyperlink ref="D76" r:id="rId85" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
+    <hyperlink ref="D78" r:id="rId85" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
     <hyperlink ref="D3" r:id="rId86" xr:uid="{DC015219-0BD9-4A0B-AAA2-E97E313B87A6}"/>
     <hyperlink ref="C3" r:id="rId87" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
-    <hyperlink ref="D81" r:id="rId88" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
-    <hyperlink ref="D85" r:id="rId89" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
-    <hyperlink ref="C74" r:id="rId90" xr:uid="{CCF6F9E7-8F70-4D1E-8597-F9646028F25D}"/>
-    <hyperlink ref="C32" r:id="rId91" xr:uid="{E2847BE0-806F-44DF-8C46-A67DFFC9BC0F}"/>
+    <hyperlink ref="D80" r:id="rId88" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
+    <hyperlink ref="D83" r:id="rId89" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
+    <hyperlink ref="C81" r:id="rId90" xr:uid="{CCF6F9E7-8F70-4D1E-8597-F9646028F25D}"/>
+    <hyperlink ref="C30" r:id="rId91" xr:uid="{E2847BE0-806F-44DF-8C46-A67DFFC9BC0F}"/>
     <hyperlink ref="C54" r:id="rId92" xr:uid="{2FE37BBE-E63B-4784-9429-160F41B36C00}"/>
     <hyperlink ref="C61" r:id="rId93" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D18" r:id="rId94" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D19" r:id="rId95" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C18" r:id="rId96" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C21" r:id="rId97" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C13" r:id="rId98" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C6" r:id="rId99" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
-    <hyperlink ref="C7" r:id="rId100" xr:uid="{83E17A80-470B-4ECF-8B23-E05D4B48DAFC}"/>
-    <hyperlink ref="C31" r:id="rId101" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="C9" r:id="rId102" xr:uid="{E035FF6A-D6FD-4586-B36D-13C716E1E0D1}"/>
+    <hyperlink ref="D15" r:id="rId94" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D16" r:id="rId95" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C15" r:id="rId96" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C18" r:id="rId97" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C10" r:id="rId98" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C23" r:id="rId99" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C24" r:id="rId100" xr:uid="{83E17A80-470B-4ECF-8B23-E05D4B48DAFC}"/>
+    <hyperlink ref="C32" r:id="rId101" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
+    <hyperlink ref="C25" r:id="rId102" xr:uid="{E035FF6A-D6FD-4586-B36D-13C716E1E0D1}"/>
     <hyperlink ref="C68" r:id="rId103" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
-    <hyperlink ref="C38" r:id="rId104" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/02/gdp-quarterly-national-accounts-2021-q3/documents/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/govscot%3Adocument/%25282%2529%2B-%2BQNAS%2B2021%2BQ3%2B-%2BOther%2BSummary%2BTables.xlsx" xr:uid="{759662E4-5376-4914-8A28-3408811A385D}"/>
-    <hyperlink ref="D38" r:id="rId105" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
-    <hyperlink ref="C37" r:id="rId106" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
-    <hyperlink ref="D37" r:id="rId107" xr:uid="{B20BE8F8-D156-4954-A6ED-104711E66619}"/>
-    <hyperlink ref="C29" r:id="rId108" xr:uid="{35F9E5E1-F98D-43CC-994E-2C1F79B3EBBC}"/>
-    <hyperlink ref="C5" r:id="rId109" xr:uid="{6826AFEE-F349-411C-9BBD-D6717F6FB1C2}"/>
+    <hyperlink ref="C35" r:id="rId104" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/02/gdp-quarterly-national-accounts-2021-q3/documents/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/govscot%3Adocument/%25282%2529%2B-%2BQNAS%2B2021%2BQ3%2B-%2BOther%2BSummary%2BTables.xlsx" xr:uid="{759662E4-5376-4914-8A28-3408811A385D}"/>
+    <hyperlink ref="D35" r:id="rId105" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
+    <hyperlink ref="C34" r:id="rId106" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
+    <hyperlink ref="D34" r:id="rId107" xr:uid="{B20BE8F8-D156-4954-A6ED-104711E66619}"/>
+    <hyperlink ref="C45" r:id="rId108" xr:uid="{35F9E5E1-F98D-43CC-994E-2C1F79B3EBBC}"/>
+    <hyperlink ref="C6" r:id="rId109" xr:uid="{6826AFEE-F349-411C-9BBD-D6717F6FB1C2}"/>
+    <hyperlink ref="D9" r:id="rId110" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId110"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId111"/>
   <tableParts count="1">
-    <tablePart r:id="rId111"/>
+    <tablePart r:id="rId112"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ecos measures, smart meters update
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154EAA07-3005-495F-9C50-3DE4CCFCAD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ABD095-6D0B-4082-B01D-755B9B008046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -922,18 +922,12 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1043397/table_252.xlsx</t>
   </si>
   <si>
-    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1056549/Headline_HEE_tables_24_February_2022.xlsx</t>
-  </si>
-  <si>
     <t>https://www.gov.uk/government/statistics/rhi-monthly-deployment-data-january-2022</t>
   </si>
   <si>
     <t>https://www.ofgem.gov.uk/sites/default/files/2022-02/Default_tarif_cap_level_v1.10.xlsx</t>
   </si>
   <si>
-    <t>https://www.electralink.co.uk/2022/02/jan-smart-installs-increase-24-pc-yoy/</t>
-  </si>
-  <si>
     <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/02/gdp-quarterly-national-accounts-2021-q3/documents/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/govscot%3Adocument/%25282%2529%2B-%2BQNAS%2B2021%2BQ3%2B-%2BOther%2BSummary%2BTables.xlsx</t>
   </si>
   <si>
@@ -947,6 +941,12 @@
   </si>
   <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1051570/renewable-energy-planning-database-q4-december-2021.csv</t>
+  </si>
+  <si>
+    <t>https://www.electralink.co.uk/2022/06/may-smart-installs-increase-11pc/</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/statistics/household-energy-efficiency-statistics-headline-release-june-2022</t>
   </si>
 </sst>
 </file>
@@ -1602,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1696,373 +1696,373 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>185</v>
+      <c r="A4" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="31">
+        <v>217</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" s="33">
+        <v>44197</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="23">
+        <f>DATE(YEAR(E4)+1,MONTH(E4),DAY(E4))</f>
+        <v>44562</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="16">
         <v>44256</v>
       </c>
-      <c r="F4" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="G4" s="23">
-        <f>DATE(YEAR(E4),MONTH(E4)+3,DAY(E4))</f>
-        <v>44348</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="23">
-        <v>44256</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="23">
-        <f>DATE(YEAR(E5),MONTH(E5)+3,DAY(E5))</f>
-        <v>44348</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>219</v>
+      <c r="F5" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="16">
+        <v>44621</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="E6" s="33">
-        <v>44197</v>
-      </c>
-      <c r="F6" s="32" t="s">
+      <c r="A6" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="23">
+        <v>44287</v>
+      </c>
+      <c r="F6" s="24" t="s">
         <v>157</v>
       </c>
       <c r="G6" s="23">
         <f>DATE(YEAR(E6)+1,MONTH(E6),DAY(E6))</f>
-        <v>44562</v>
+        <v>44652</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="E7" s="16">
-        <v>44256</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="16">
-        <v>44621</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="A7" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" s="23">
+        <v>44287</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="23">
+        <f>DATE(YEAR(E7)+1,MONTH(E7),DAY(E7))</f>
+        <v>44652</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>69</v>
+        <v>228</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>300</v>
+        <v>229</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>230</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="E8" s="23">
-        <v>44593</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>158</v>
+        <v>44287</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>157</v>
       </c>
       <c r="G8" s="23">
-        <f>DATE(YEAR(E8),MONTH(E8)+1,DAY(E8))</f>
-        <v>44621</v>
+        <f>DATE(YEAR(E8)+1,MONTH(E8),DAY(E8))</f>
+        <v>44652</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>297</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E9" s="23">
-        <v>44593</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="G9" s="23">
-        <f>DATE(YEAR(E9),MONTH(E9)+1,DAY(E9))</f>
-        <v>44621</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>219</v>
+      <c r="A9" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="31">
+        <v>44287</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="31">
+        <f>DATE(YEAR(E9)+1,MONTH(E9),DAY(E9))</f>
+        <v>44652</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="25"/>
+        <v>284</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>283</v>
+      </c>
       <c r="E10" s="23">
-        <v>44287</v>
+        <v>44531</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G10" s="23">
-        <f>DATE(YEAR(E10)+1,MONTH(E10),DAY(E10))</f>
+        <f>DATE(YEAR(E10),MONTH(E10)+4,DAY(E10))</f>
         <v>44652</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="E11" s="23">
-        <v>44287</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>157</v>
+      <c r="A11" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="16">
+        <v>44562</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="G11" s="23">
-        <f>DATE(YEAR(E11)+1,MONTH(E11),DAY(E11))</f>
+        <f>DATE(YEAR(E11),MONTH(E11)+3,DAY(E11))</f>
         <v>44652</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="16">
+        <v>44562</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="23">
+        <f>DATE(YEAR(E12),MONTH(E12)+3,DAY(E12))</f>
+        <v>44652</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="E13" s="23">
+        <v>44621</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G13" s="23">
+        <f>DATE(YEAR(E13),MONTH(E13)+1,DAY(E13))</f>
+        <v>44652</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>302</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>301</v>
+      </c>
+      <c r="E14" s="31">
+        <v>44593</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="31">
+        <f t="shared" ref="G14:G24" si="0">DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
+        <v>44682</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="E15" s="23">
+        <v>44593</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="0"/>
+        <v>44682</v>
+      </c>
+      <c r="H15" s="21" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="E12" s="23">
-        <v>44287</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="G12" s="23">
-        <f>DATE(YEAR(E12)+1,MONTH(E12),DAY(E12))</f>
-        <v>44652</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="E13" s="31">
-        <v>44287</v>
-      </c>
-      <c r="F13" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="G13" s="31">
-        <f>DATE(YEAR(E13)+1,MONTH(E13),DAY(E13))</f>
-        <v>44652</v>
-      </c>
-      <c r="H13" s="29" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>283</v>
-      </c>
-      <c r="E14" s="23">
-        <v>44531</v>
-      </c>
-      <c r="F14" s="24" t="s">
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="31">
+        <v>44621</v>
+      </c>
+      <c r="F16" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="G14" s="23">
-        <f>DATE(YEAR(E14),MONTH(E14)+4,DAY(E14))</f>
-        <v>44652</v>
-      </c>
-      <c r="H14" s="21" t="s">
+      <c r="G16" s="23">
+        <f t="shared" si="0"/>
+        <v>44713</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E15" s="16">
-        <v>44562</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="G15" s="23">
-        <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
-        <v>44652</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E16" s="16">
-        <v>44562</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="G16" s="23">
-        <f>DATE(YEAR(E16),MONTH(E16)+3,DAY(E16))</f>
-        <v>44652</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>298</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>271</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E17" s="23">
         <v>44621</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G17" s="23">
-        <f>DATE(YEAR(E17),MONTH(E17)+1,DAY(E17))</f>
-        <v>44652</v>
+        <f t="shared" si="0"/>
+        <v>44713</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>219</v>
@@ -2070,282 +2070,280 @@
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>38</v>
+        <v>295</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="E18" s="23">
-        <v>44652</v>
+        <v>296</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="4">
+        <v>44621</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G18" s="23">
-        <f>DATE(YEAR(E18),MONTH(E18)+1,DAY(E18))</f>
-        <v>44682</v>
+        <f t="shared" si="0"/>
+        <v>44713</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
-        <v>211</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>304</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>303</v>
-      </c>
-      <c r="E19" s="31">
-        <v>44593</v>
-      </c>
-      <c r="F19" s="29" t="s">
+      <c r="A19" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19" s="23">
+        <v>44621</v>
+      </c>
+      <c r="F19" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G19" s="31">
-        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
-        <v>44682</v>
+        <f t="shared" si="0"/>
+        <v>44713</v>
       </c>
       <c r="H19" s="29" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>301</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>302</v>
+      <c r="A20" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="E20" s="23">
-        <v>44593</v>
-      </c>
-      <c r="F20" s="24" t="s">
+        <v>44621</v>
+      </c>
+      <c r="F20" s="43" t="s">
         <v>156</v>
       </c>
       <c r="G20" s="23">
-        <f>DATE(YEAR(E20),MONTH(E20)+3,DAY(E20))</f>
-        <v>44682</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>222</v>
+        <f t="shared" si="0"/>
+        <v>44713</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
-        <v>295</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>296</v>
-      </c>
-      <c r="D21" s="41" t="s">
+      <c r="A21" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="23">
         <v>44621</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="43" t="s">
         <v>156</v>
       </c>
       <c r="G21" s="23">
-        <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
+        <f t="shared" si="0"/>
         <v>44713</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H21" s="29" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>258</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="E22" s="23">
+        <v>294</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>293</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" s="4">
         <v>44621</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="G22" s="31">
-        <f>DATE(YEAR(E22),MONTH(E22)+3,DAY(E22))</f>
+      <c r="G22" s="23">
+        <f t="shared" si="0"/>
         <v>44713</v>
       </c>
-      <c r="H22" s="29" t="s">
-        <v>221</v>
+      <c r="H22" s="21" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>44</v>
+      <c r="A23" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>87</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>155</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="D23" s="26"/>
       <c r="E23" s="23">
         <v>44621</v>
       </c>
-      <c r="F23" s="43" t="s">
+      <c r="F23" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G23" s="23">
-        <f>DATE(YEAR(E23),MONTH(E23)+3,DAY(E23))</f>
+        <f t="shared" si="0"/>
         <v>44713</v>
       </c>
-      <c r="H23" s="29" t="s">
-        <v>219</v>
+      <c r="H23" s="21" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>139</v>
-      </c>
+      <c r="A24" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="26"/>
       <c r="E24" s="23">
         <v>44621</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G24" s="23">
-        <f>DATE(YEAR(E24),MONTH(E24)+3,DAY(E24))</f>
+        <f t="shared" si="0"/>
         <v>44713</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="H24" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="31">
+        <v>44348</v>
+      </c>
+      <c r="F25" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="31">
+        <f>DATE(YEAR(E25)+1,MONTH(E25),DAY(E25))</f>
+        <v>44713</v>
+      </c>
+      <c r="H25" s="29" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
-        <v>294</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>293</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="E25" s="4">
-        <v>44621</v>
-      </c>
-      <c r="F25" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G25" s="23">
-        <f>DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="31">
+        <v>44348</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="31">
+        <f>DATE(YEAR(E26)+1,MONTH(E26),DAY(E26))</f>
         <v>44713</v>
       </c>
-      <c r="H25" s="21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="23">
-        <v>44621</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G26" s="23">
-        <f>DATE(YEAR(E26),MONTH(E26)+3,DAY(E26))</f>
+      <c r="H26" s="29" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="31">
+        <v>44348</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="31">
+        <f>DATE(YEAR(E27)+1,MONTH(E27),DAY(E27))</f>
         <v>44713</v>
       </c>
-      <c r="H26" s="21" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="26"/>
-      <c r="E27" s="23">
-        <v>44621</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G27" s="23">
-        <f>DATE(YEAR(E27),MONTH(E27)+3,DAY(E27))</f>
-        <v>44713</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>223</v>
+      <c r="H27" s="29" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="29" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>136</v>
+        <v>233</v>
       </c>
       <c r="E28" s="31">
         <v>44348</v>
@@ -2358,21 +2356,21 @@
         <v>44713</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="29" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>174</v>
+        <v>103</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>233</v>
       </c>
       <c r="E29" s="31">
         <v>44348</v>
@@ -2385,20 +2383,22 @@
         <v>44713</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="29" t="s">
-        <v>93</v>
+        <v>234</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="26"/>
+        <v>235</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>237</v>
+      </c>
       <c r="E30" s="31">
         <v>44348</v>
       </c>
@@ -2406,142 +2406,142 @@
         <v>157</v>
       </c>
       <c r="G30" s="31">
-        <f>DATE(YEAR(E30)+1,MONTH(E30),DAY(E30))</f>
         <v>44713</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>232</v>
+      <c r="A31" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>279</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="E31" s="31">
-        <v>44348</v>
-      </c>
-      <c r="F31" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="G31" s="31">
-        <f>DATE(YEAR(E31)+1,MONTH(E31),DAY(E31))</f>
-        <v>44713</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>222</v>
+        <v>132</v>
+      </c>
+      <c r="E31" s="4">
+        <v>44622</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="23">
+        <f t="shared" ref="G31:G38" si="1">DATE(YEAR(E31),MONTH(E31)+3,DAY(E31))</f>
+        <v>44714</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>232</v>
+      <c r="A32" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>280</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="E32" s="31">
-        <v>44348</v>
-      </c>
-      <c r="F32" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="G32" s="31">
-        <f>DATE(YEAR(E32)+1,MONTH(E32),DAY(E32))</f>
-        <v>44713</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>222</v>
+        <v>132</v>
+      </c>
+      <c r="E32" s="4">
+        <v>44623</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" s="23">
+        <f t="shared" si="1"/>
+        <v>44715</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="E33" s="31">
-        <v>44348</v>
-      </c>
-      <c r="F33" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="G33" s="31">
-        <v>44713</v>
-      </c>
-      <c r="H33" s="29" t="s">
+      <c r="A33" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="4">
+        <v>44624</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="G33" s="23">
+        <f t="shared" si="1"/>
+        <v>44716</v>
+      </c>
+      <c r="H33" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="40" t="s">
-        <v>279</v>
+        <v>40</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>293</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E34" s="4">
-        <v>44622</v>
+        <v>44625</v>
       </c>
       <c r="F34" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G34" s="23">
-        <f>DATE(YEAR(E34),MONTH(E34)+3,DAY(E34))</f>
-        <v>44714</v>
+        <f t="shared" si="1"/>
+        <v>44717</v>
       </c>
       <c r="H34" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>280</v>
+      <c r="A35" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="40" t="s">
+        <v>255</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E35" s="4">
-        <v>44623</v>
-      </c>
-      <c r="F35" s="24" t="s">
+        <v>44626</v>
+      </c>
+      <c r="F35" s="43" t="s">
         <v>156</v>
       </c>
       <c r="G35" s="23">
-        <f>DATE(YEAR(E35),MONTH(E35)+3,DAY(E35))</f>
-        <v>44715</v>
+        <f t="shared" si="1"/>
+        <v>44718</v>
       </c>
       <c r="H35" s="21" t="s">
         <v>219</v>
@@ -2549,26 +2549,26 @@
     </row>
     <row r="36" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>132</v>
       </c>
       <c r="E36" s="4">
-        <v>44624</v>
+        <v>44627</v>
       </c>
       <c r="F36" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G36" s="23">
-        <f>DATE(YEAR(E36),MONTH(E36)+3,DAY(E36))</f>
-        <v>44716</v>
+        <f t="shared" si="1"/>
+        <v>44719</v>
       </c>
       <c r="H36" s="21" t="s">
         <v>219</v>
@@ -2576,162 +2576,162 @@
     </row>
     <row r="37" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
-        <v>39</v>
+        <v>288</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>40</v>
+        <v>292</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E37" s="4">
-        <v>44625</v>
+        <v>44628</v>
       </c>
       <c r="F37" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G37" s="23">
-        <f>DATE(YEAR(E37),MONTH(E37)+3,DAY(E37))</f>
-        <v>44717</v>
+        <f t="shared" si="1"/>
+        <v>44720</v>
       </c>
       <c r="H37" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>255</v>
+      <c r="A38" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>290</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E38" s="4">
-        <v>44626</v>
-      </c>
-      <c r="F38" s="43" t="s">
+        <v>44629</v>
+      </c>
+      <c r="F38" s="24" t="s">
         <v>156</v>
       </c>
       <c r="G38" s="23">
-        <f>DATE(YEAR(E38),MONTH(E38)+3,DAY(E38))</f>
-        <v>44718</v>
+        <f t="shared" si="1"/>
+        <v>44721</v>
       </c>
       <c r="H38" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="D39" s="22" t="s">
-        <v>132</v>
+      <c r="A39" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="B39" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>187</v>
       </c>
       <c r="E39" s="4">
-        <v>44627</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G39" s="23">
-        <f>DATE(YEAR(E39),MONTH(E39)+3,DAY(E39))</f>
-        <v>44719</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>219</v>
-      </c>
+        <v>44646</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="48">
+        <v>44738</v>
+      </c>
+      <c r="H39" s="45"/>
     </row>
     <row r="40" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="s">
-        <v>288</v>
+        <v>69</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="D40" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" s="4">
-        <v>44628</v>
+        <v>70</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="23">
+        <v>44713</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G40" s="23">
-        <f>DATE(YEAR(E40),MONTH(E40)+3,DAY(E40))</f>
-        <v>44720</v>
+        <f>DATE(YEAR(E40),MONTH(E40)+1,DAY(E40))</f>
+        <v>44743</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21" t="s">
-        <v>287</v>
+        <v>27</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" s="4">
-        <v>44629</v>
+        <v>28</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E41" s="23">
+        <v>44713</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G41" s="23">
-        <f>DATE(YEAR(E41),MONTH(E41)+3,DAY(E41))</f>
-        <v>44721</v>
+        <f>DATE(YEAR(E41),MONTH(E41)+1,DAY(E41))</f>
+        <v>44743</v>
       </c>
       <c r="H41" s="21" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="B42" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="C42" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="D42" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="E42" s="4">
-        <v>44646</v>
-      </c>
-      <c r="F42" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="G42" s="48">
-        <v>44738</v>
-      </c>
-      <c r="H42" s="45"/>
+      <c r="A42" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="23">
+        <v>44713</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G42" s="23">
+        <f>DATE(YEAR(E42),MONTH(E42)+1,DAY(E42))</f>
+        <v>44743</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="43" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
@@ -2793,7 +2793,7 @@
         <v>50</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>141</v>
@@ -3008,7 +3008,7 @@
         <v>201</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D53" s="25" t="s">
         <v>202</v>
@@ -3047,7 +3047,7 @@
         <v>157</v>
       </c>
       <c r="G54" s="23">
-        <f>DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
+        <f t="shared" ref="G54:G66" si="2">DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
         <v>44805</v>
       </c>
       <c r="H54" s="21" t="s">
@@ -3074,7 +3074,7 @@
         <v>157</v>
       </c>
       <c r="G55" s="23">
-        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H55" s="21" t="s">
@@ -3101,7 +3101,7 @@
         <v>157</v>
       </c>
       <c r="G56" s="23">
-        <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H56" s="21" t="s">
@@ -3128,7 +3128,7 @@
         <v>157</v>
       </c>
       <c r="G57" s="23">
-        <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H57" s="21" t="s">
@@ -3155,7 +3155,7 @@
         <v>157</v>
       </c>
       <c r="G58" s="23">
-        <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
+        <f t="shared" si="2"/>
         <v>44805</v>
       </c>
       <c r="H58" s="21" t="s">
@@ -3182,7 +3182,7 @@
         <v>157</v>
       </c>
       <c r="G59" s="31">
-        <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
+        <f t="shared" si="2"/>
         <v>44866</v>
       </c>
       <c r="H59" s="29" t="s">
@@ -3209,7 +3209,7 @@
         <v>157</v>
       </c>
       <c r="G60" s="31">
-        <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
+        <f t="shared" si="2"/>
         <v>44866</v>
       </c>
       <c r="H60" s="29" t="s">
@@ -3236,7 +3236,7 @@
         <v>157</v>
       </c>
       <c r="G61" s="23">
-        <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H61" s="21" t="s">
@@ -3263,7 +3263,7 @@
         <v>157</v>
       </c>
       <c r="G62" s="23">
-        <f>DATE(YEAR(E62)+1,MONTH(E62),DAY(E62))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H62" s="21" t="s">
@@ -3290,7 +3290,7 @@
         <v>157</v>
       </c>
       <c r="G63" s="23">
-        <f>DATE(YEAR(E63)+1,MONTH(E63),DAY(E63))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H63" s="21" t="s">
@@ -3317,7 +3317,7 @@
         <v>157</v>
       </c>
       <c r="G64" s="23">
-        <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H64" s="21" t="s">
@@ -3344,7 +3344,7 @@
         <v>157</v>
       </c>
       <c r="G65" s="23">
-        <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
+        <f t="shared" si="2"/>
         <v>44896</v>
       </c>
       <c r="H65" s="21" t="s">
@@ -3371,7 +3371,7 @@
         <v>157</v>
       </c>
       <c r="G66" s="23">
-        <f>DATE(YEAR(E66)+1,MONTH(E66),DAY(E66))</f>
+        <f t="shared" si="2"/>
         <v>44927</v>
       </c>
       <c r="H66" s="21" t="s">
@@ -3826,25 +3826,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C25" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="D67" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="C66" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="C44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C26" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C27" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C30" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C27" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="C70" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C13" r:id="rId9" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-statistics-supplementary-tables-2018/documents/physical-commodity-balances-of-oil-gas-and-petroleum-products/physical-commodity-balances-of-oil-gas-and-petroleum-products/govscot%3Adocument/Commodity%2BBalances%2B-%2B1998-2018.xlsx" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C9" r:id="rId9" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-statistics-supplementary-tables-2018/documents/physical-commodity-balances-of-oil-gas-and-petroleum-products/physical-commodity-balances-of-oil-gas-and-petroleum-products/govscot%3Adocument/Commodity%2BBalances%2B-%2B1998-2018.xlsx" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
     <hyperlink ref="C80" r:id="rId10" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="D73" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D36" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D39" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D33" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D36" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
     <hyperlink ref="D54" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
     <hyperlink ref="D46" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="D10:D12" r:id="rId17" display="https://www.gov.uk/government/statistics/electricity-chapter-5-digest-of-united-kingdom-energy-statistics-dukes" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="D5" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="D17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D25" r:id="rId19" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
     <hyperlink ref="D50" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
     <hyperlink ref="D61" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
     <hyperlink ref="D43" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
@@ -3854,36 +3854,36 @@
     <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
     <hyperlink ref="D65" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
     <hyperlink ref="D59" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D34" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D35" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D15" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D16" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="D31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D11" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="D12" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
     <hyperlink ref="D82" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
     <hyperlink ref="D70" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D13" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="D23" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D9" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="D20" r:id="rId36" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
     <hyperlink ref="D62" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D37" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D34" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
     <hyperlink ref="D52" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
     <hyperlink ref="D77" r:id="rId40" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
     <hyperlink ref="D69" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
     <hyperlink ref="C69" r:id="rId42" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
     <hyperlink ref="D48" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
     <hyperlink ref="D49" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C39" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D18" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="D22" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D8" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C36" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D42" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="D19" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D40" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
     <hyperlink ref="C67" r:id="rId49" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
     <hyperlink ref="D66" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D29" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D11" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D26" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D7" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
     <hyperlink ref="D51" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="D7" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="D5" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
     <hyperlink ref="C79" r:id="rId55" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
     <hyperlink ref="C84" r:id="rId56" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
     <hyperlink ref="D68" r:id="rId57" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
-    <hyperlink ref="C4" r:id="rId58" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
+    <hyperlink ref="C16" r:id="rId58" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
     <hyperlink ref="D74" r:id="rId59" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
     <hyperlink ref="C74" r:id="rId60" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
     <hyperlink ref="D72" r:id="rId61" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
@@ -3894,21 +3894,21 @@
     <hyperlink ref="D53" r:id="rId66" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
     <hyperlink ref="C78" r:id="rId67" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
     <hyperlink ref="C46" r:id="rId68" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
-    <hyperlink ref="D38" r:id="rId69" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
-    <hyperlink ref="D24" r:id="rId70" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
+    <hyperlink ref="D35" r:id="rId69" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
+    <hyperlink ref="D21" r:id="rId70" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
     <hyperlink ref="C51" r:id="rId71" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="D17" r:id="rId72" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C7" r:id="rId73" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2021/03/oil-and-gas-production-statistics-2019/documents/oil-and-gas-production-statistics-2019---tables/oil-and-gas-production-statistics-2019---tables/govscot%3Adocument/Oil%2Band%2BGas%2BProduction%2B2019%2B-%2Bpublication%2Btables.xlsx?forceDownload=true" xr:uid="{EFFB3F7D-992D-403B-9018-45F56D2F9DE7}"/>
+    <hyperlink ref="D13" r:id="rId72" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C5" r:id="rId73" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2021/03/oil-and-gas-production-statistics-2019/documents/oil-and-gas-production-statistics-2019---tables/oil-and-gas-production-statistics-2019---tables/govscot%3Adocument/Oil%2Band%2BGas%2BProduction%2B2019%2B-%2Bpublication%2Btables.xlsx?forceDownload=true" xr:uid="{EFFB3F7D-992D-403B-9018-45F56D2F9DE7}"/>
     <hyperlink ref="C58" r:id="rId74" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D9" r:id="rId75" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="D41" r:id="rId75" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
     <hyperlink ref="C83" r:id="rId76" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
     <hyperlink ref="C43" r:id="rId77" xr:uid="{2CD20F64-59CA-40E1-BDC9-2AE5808A14A7}"/>
     <hyperlink ref="D63" r:id="rId78" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C36" r:id="rId79" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="C33" r:id="rId79" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
     <hyperlink ref="C62" r:id="rId80" xr:uid="{0452CD0A-EB9C-4B25-88AF-06E4876A2427}"/>
     <hyperlink ref="D60" r:id="rId81" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
     <hyperlink ref="C2" r:id="rId82" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D14" r:id="rId83" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="D10" r:id="rId83" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
     <hyperlink ref="C52" r:id="rId84" xr:uid="{E75D3585-4283-4149-B12A-500F1C77C046}"/>
     <hyperlink ref="D78" r:id="rId85" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
     <hyperlink ref="D3" r:id="rId86" xr:uid="{DC015219-0BD9-4A0B-AAA2-E97E313B87A6}"/>
@@ -3916,34 +3916,32 @@
     <hyperlink ref="D80" r:id="rId88" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
     <hyperlink ref="D83" r:id="rId89" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
     <hyperlink ref="C81" r:id="rId90" xr:uid="{CCF6F9E7-8F70-4D1E-8597-F9646028F25D}"/>
-    <hyperlink ref="C14" r:id="rId91" xr:uid="{E2847BE0-806F-44DF-8C46-A67DFFC9BC0F}"/>
+    <hyperlink ref="C10" r:id="rId91" xr:uid="{E2847BE0-806F-44DF-8C46-A67DFFC9BC0F}"/>
     <hyperlink ref="C54" r:id="rId92" xr:uid="{2FE37BBE-E63B-4784-9429-160F41B36C00}"/>
     <hyperlink ref="C61" r:id="rId93" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D40" r:id="rId94" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D41" r:id="rId95" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C40" r:id="rId96" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C37" r:id="rId97" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C21" r:id="rId98" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C18" r:id="rId99" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
-    <hyperlink ref="C8" r:id="rId100" xr:uid="{83E17A80-470B-4ECF-8B23-E05D4B48DAFC}"/>
-    <hyperlink ref="C16" r:id="rId101" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="C9" r:id="rId102" xr:uid="{E035FF6A-D6FD-4586-B36D-13C716E1E0D1}"/>
-    <hyperlink ref="C68" r:id="rId103" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
-    <hyperlink ref="C20" r:id="rId104" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/02/gdp-quarterly-national-accounts-2021-q3/documents/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/govscot%3Adocument/%25282%2529%2B-%2BQNAS%2B2021%2BQ3%2B-%2BOther%2BSummary%2BTables.xlsx" xr:uid="{759662E4-5376-4914-8A28-3408811A385D}"/>
-    <hyperlink ref="D20" r:id="rId105" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
-    <hyperlink ref="C19" r:id="rId106" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
-    <hyperlink ref="D19" r:id="rId107" xr:uid="{B20BE8F8-D156-4954-A6ED-104711E66619}"/>
-    <hyperlink ref="C45" r:id="rId108" xr:uid="{35F9E5E1-F98D-43CC-994E-2C1F79B3EBBC}"/>
-    <hyperlink ref="C22" r:id="rId109" xr:uid="{6826AFEE-F349-411C-9BBD-D6717F6FB1C2}"/>
-    <hyperlink ref="D25" r:id="rId110" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
-    <hyperlink ref="C38" r:id="rId111" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
-    <hyperlink ref="C34" r:id="rId112" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
-    <hyperlink ref="C5" r:id="rId113" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
+    <hyperlink ref="D37" r:id="rId94" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D38" r:id="rId95" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C37" r:id="rId96" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C34" r:id="rId97" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C18" r:id="rId98" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C42" r:id="rId99" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C12" r:id="rId100" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
+    <hyperlink ref="C68" r:id="rId101" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
+    <hyperlink ref="C15" r:id="rId102" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/02/gdp-quarterly-national-accounts-2021-q3/documents/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/gdp-quarterly-national-accounts-2021-q3---other-summary-tables/govscot%3Adocument/%25282%2529%2B-%2BQNAS%2B2021%2BQ3%2B-%2BOther%2BSummary%2BTables.xlsx" xr:uid="{759662E4-5376-4914-8A28-3408811A385D}"/>
+    <hyperlink ref="D15" r:id="rId103" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
+    <hyperlink ref="C14" r:id="rId104" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
+    <hyperlink ref="D14" r:id="rId105" xr:uid="{B20BE8F8-D156-4954-A6ED-104711E66619}"/>
+    <hyperlink ref="C45" r:id="rId106" xr:uid="{35F9E5E1-F98D-43CC-994E-2C1F79B3EBBC}"/>
+    <hyperlink ref="C19" r:id="rId107" xr:uid="{6826AFEE-F349-411C-9BBD-D6717F6FB1C2}"/>
+    <hyperlink ref="D22" r:id="rId108" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
+    <hyperlink ref="C35" r:id="rId109" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
+    <hyperlink ref="C31" r:id="rId110" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
+    <hyperlink ref="C17" r:id="rId111" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId114"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId112"/>
   <tableParts count="1">
-    <tablePart r:id="rId115"/>
+    <tablePart r:id="rId113"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
industry productivity, eco measures update
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E76A97D-B5BB-4CFD-BAAF-947945F1E4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB53CFB-C4F0-4515-9AC5-50C56EA94D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1095,6 +1095,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1565,7 +1568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1575,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,25 +1754,25 @@
     </row>
     <row r="7" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>255</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" s="18">
-        <v>44805</v>
+        <v>66</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44743</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G7" s="18">
-        <f>DATE(YEAR(E7),MONTH(E7)+1,DAY(E7))</f>
+        <f>DATE(YEAR(E7),MONTH(E7)+3,DAY(E7))</f>
         <v>44835</v>
       </c>
       <c r="H7" s="16" t="s">
@@ -1778,18 +1781,18 @@
     </row>
     <row r="8" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="1">
+        <v>127</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="18">
         <v>44743</v>
       </c>
       <c r="F8" s="19" t="s">
@@ -1800,111 +1803,109 @@
         <v>44835</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>284</v>
+        <v>70</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>289</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E9" s="18">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G9" s="18">
-        <f>DATE(YEAR(E9),MONTH(E9)+3,DAY(E9))</f>
-        <v>44835</v>
+        <f>DATE(YEAR(E9),MONTH(E9)+1,DAY(E9))</f>
+        <v>44866</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>69</v>
+        <v>192</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>289</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>170</v>
+        <v>194</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>193</v>
       </c>
       <c r="E10" s="18">
-        <v>44835</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>157</v>
+        <v>44531</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="G10" s="18">
-        <f>DATE(YEAR(E10),MONTH(E10)+1,DAY(E10))</f>
-        <v>44866</v>
+        <f>DATE(YEAR(E10)+1,MONTH(E10),DAY(E10))</f>
+        <v>44896</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>27</v>
+        <v>183</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>293</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>243</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="17"/>
       <c r="E11" s="18">
-        <v>44835</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>157</v>
+        <v>44805</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="G11" s="18">
-        <f>DATE(YEAR(E11),MONTH(E11)+1,DAY(E11))</f>
-        <v>44866</v>
+        <f>DATE(YEAR(E11),MONTH(E11)+3,DAY(E11))</f>
+        <v>44896</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>192</v>
+        <v>63</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="E12" s="18">
-        <v>44531</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>156</v>
+        <v>64</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44805</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>155</v>
       </c>
       <c r="G12" s="18">
-        <f>DATE(YEAR(E12)+1,MONTH(E12),DAY(E12))</f>
+        <f>DATE(YEAR(E12),MONTH(E12)+3,DAY(E12))</f>
         <v>44896</v>
       </c>
       <c r="H12" s="16" t="s">
@@ -1913,101 +1914,107 @@
     </row>
     <row r="13" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>183</v>
+        <v>35</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" s="17"/>
+        <v>36</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>136</v>
+      </c>
       <c r="E13" s="18">
-        <v>44805</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>155</v>
+        <v>44531</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>156</v>
       </c>
       <c r="G13" s="18">
-        <f>DATE(YEAR(E13),MONTH(E13)+3,DAY(E13))</f>
+        <f>DATE(YEAR(E13)+1,MONTH(E13),DAY(E13))</f>
         <v>44896</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>234</v>
-      </c>
-      <c r="D14" s="17"/>
+        <v>250</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>145</v>
+      </c>
       <c r="E14" s="18">
-        <v>44805</v>
+        <v>44531</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G14" s="18">
-        <f>DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
+        <f>DATE(YEAR(E14)+1,MONTH(E14),DAY(E14))</f>
         <v>44896</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="17"/>
+        <v>80</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>172</v>
+      </c>
       <c r="E15" s="18">
-        <v>44805</v>
+        <v>44562</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G15" s="18">
-        <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
-        <v>44896</v>
+        <f>DATE(YEAR(E15)+1,MONTH(E15),DAY(E15))</f>
+        <v>44927</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>258</v>
+        <v>298</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E16" s="1">
-        <v>44805</v>
+        <v>141</v>
+      </c>
+      <c r="E16" s="18">
+        <v>44835</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G16" s="18">
-        <f>DATE(YEAR(E16),MONTH(E16)+3,DAY(E16))</f>
-        <v>44896</v>
+        <f>DATE(YEAR(E16),MONTH(E16)+4,DAY(E16))</f>
+        <v>44958</v>
       </c>
       <c r="H16" s="16" t="s">
         <v>216</v>
@@ -2015,51 +2022,53 @@
     </row>
     <row r="17" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="17"/>
+        <v>198</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>199</v>
+      </c>
       <c r="E17" s="18">
-        <v>44805</v>
+        <v>44774</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>155</v>
+        <v>260</v>
       </c>
       <c r="G17" s="18">
-        <f>DATE(YEAR(E17),MONTH(E17)+3,DAY(E17))</f>
-        <v>44896</v>
+        <f>DATE(YEAR(E17),MONTH(E17)+6,DAY(E17))</f>
+        <v>44958</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>35</v>
+        <v>181</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>136</v>
+        <v>180</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="E18" s="18">
-        <v>44531</v>
-      </c>
-      <c r="F18" s="19" t="s">
+        <v>44593</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>156</v>
       </c>
       <c r="G18" s="18">
         <f>DATE(YEAR(E18)+1,MONTH(E18),DAY(E18))</f>
-        <v>44896</v>
+        <v>44958</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>216</v>
@@ -2067,107 +2076,105 @@
     </row>
     <row r="19" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>145</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D19" s="17"/>
       <c r="E19" s="18">
-        <v>44531</v>
+        <v>44896</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G19" s="18">
-        <f>DATE(YEAR(E19)+1,MONTH(E19),DAY(E19))</f>
-        <v>44896</v>
+        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
+        <v>44986</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>172</v>
+        <v>28</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>243</v>
       </c>
       <c r="E20" s="18">
-        <v>44562</v>
+        <v>44958</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G20" s="18">
-        <f>DATE(YEAR(E20)+1,MONTH(E20),DAY(E20))</f>
-        <v>44927</v>
+        <f>DATE(YEAR(E20),MONTH(E20)+1,DAY(E20))</f>
+        <v>44986</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>73</v>
+        <v>38</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>137</v>
       </c>
       <c r="E21" s="18">
-        <v>44562</v>
+        <v>44958</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G21" s="18">
-        <f>DATE(YEAR(E21),MONTH(E21)+12,DAY(E21))</f>
-        <v>44927</v>
+        <f>DATE(YEAR(E21),MONTH(E21)+1,DAY(E21))</f>
+        <v>44986</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>52</v>
+        <v>271</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>298</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>141</v>
+        <v>272</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>138</v>
       </c>
       <c r="E22" s="18">
-        <v>44835</v>
+        <v>44896</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G22" s="18">
-        <f>DATE(YEAR(E22),MONTH(E22)+4,DAY(E22))</f>
-        <v>44958</v>
+        <f>DATE(YEAR(E22),MONTH(E22)+3,DAY(E22))</f>
+        <v>44986</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>216</v>
@@ -2175,53 +2182,53 @@
     </row>
     <row r="23" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>197</v>
+        <v>264</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="E23" s="18">
-        <v>44774</v>
+        <v>268</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" s="1">
+        <v>44896</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>260</v>
+        <v>155</v>
       </c>
       <c r="G23" s="18">
-        <f>DATE(YEAR(E23),MONTH(E23)+6,DAY(E23))</f>
-        <v>44958</v>
+        <f>DATE(YEAR(E23),MONTH(E23)+3,DAY(E23))</f>
+        <v>44986</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="C24" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="E24" s="18">
-        <v>44593</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>156</v>
+        <v>267</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" s="1">
+        <v>44896</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>155</v>
       </c>
       <c r="G24" s="18">
-        <f>DATE(YEAR(E24)+1,MONTH(E24),DAY(E24))</f>
-        <v>44958</v>
+        <f>DATE(YEAR(E24),MONTH(E24)+3,DAY(E24))</f>
+        <v>44986</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>216</v>
@@ -2229,25 +2236,25 @@
     </row>
     <row r="25" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>272</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" s="18">
+        <v>4</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="1">
         <v>44896</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G25" s="18">
-        <f t="shared" ref="G25:G31" si="0">DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
+        <f>DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
         <v>44986</v>
       </c>
       <c r="H25" s="16" t="s">
@@ -2256,13 +2263,13 @@
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>264</v>
+        <v>6</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>268</v>
+        <v>7</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>132</v>
@@ -2274,7 +2281,7 @@
         <v>155</v>
       </c>
       <c r="G26" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E26),MONTH(E26)+3,DAY(E26))</f>
         <v>44986</v>
       </c>
       <c r="H26" s="16" t="s">
@@ -2283,25 +2290,25 @@
     </row>
     <row r="27" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>263</v>
+        <v>43</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>267</v>
+        <v>44</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E27" s="1">
+        <v>154</v>
+      </c>
+      <c r="E27" s="18">
         <v>44896</v>
       </c>
       <c r="F27" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G27" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E27),MONTH(E27)+3,DAY(E27))</f>
         <v>44986</v>
       </c>
       <c r="H27" s="16" t="s">
@@ -2310,25 +2317,25 @@
     </row>
     <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="1">
+        <v>138</v>
+      </c>
+      <c r="E28" s="18">
         <v>44896</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G28" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E28),MONTH(E28)+3,DAY(E28))</f>
         <v>44986</v>
       </c>
       <c r="H28" s="16" t="s">
@@ -2337,43 +2344,43 @@
     </row>
     <row r="29" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>6</v>
+        <v>205</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E29" s="1">
-        <v>44896</v>
+        <v>206</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="E29" s="18">
+        <v>44866</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G29" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E29),MONTH(E29)+4,DAY(E29))</f>
         <v>44986</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>256</v>
+        <v>30</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>251</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="E30" s="18">
         <v>44896</v>
@@ -2382,7 +2389,7 @@
         <v>155</v>
       </c>
       <c r="G30" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
         <v>44986</v>
       </c>
       <c r="H30" s="16" t="s">
@@ -2391,16 +2398,16 @@
     </row>
     <row r="31" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E31" s="18">
         <v>44896</v>
@@ -2409,7 +2416,7 @@
         <v>155</v>
       </c>
       <c r="G31" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E31),MONTH(E31)+3,DAY(E31))</f>
         <v>44986</v>
       </c>
       <c r="H31" s="16" t="s">
@@ -2418,43 +2425,43 @@
     </row>
     <row r="32" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>205</v>
+        <v>49</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>261</v>
+        <v>50</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>280</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>140</v>
       </c>
       <c r="E32" s="18">
-        <v>44866</v>
+        <v>44896</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G32" s="18">
-        <f>DATE(YEAR(E32),MONTH(E32)+4,DAY(E32))</f>
+        <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
         <v>44986</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>135</v>
+        <v>285</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>273</v>
       </c>
       <c r="E33" s="18">
         <v>44896</v>
@@ -2467,58 +2474,58 @@
         <v>44986</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>139</v>
+        <v>295</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>294</v>
       </c>
       <c r="E34" s="18">
-        <v>44896</v>
+        <v>44621</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G34" s="18">
-        <f>DATE(YEAR(E34),MONTH(E34)+3,DAY(E34))</f>
+        <f>DATE(YEAR(E34)+1,MONTH(E34),DAY(E34))</f>
         <v>44986</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>50</v>
+        <v>270</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>280</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>140</v>
+        <v>269</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>138</v>
       </c>
       <c r="E35" s="18">
-        <v>44896</v>
+        <v>44897</v>
       </c>
       <c r="F35" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G35" s="18">
         <f>DATE(YEAR(E35),MONTH(E35)+3,DAY(E35))</f>
-        <v>44986</v>
+        <v>44987</v>
       </c>
       <c r="H35" s="16" t="s">
         <v>216</v>
@@ -2526,203 +2533,203 @@
     </row>
     <row r="36" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>285</v>
-      </c>
-      <c r="D36" s="33" t="s">
-        <v>273</v>
+        <v>40</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="E36" s="18">
-        <v>44896</v>
+        <v>44898</v>
       </c>
       <c r="F36" s="19" t="s">
         <v>155</v>
       </c>
       <c r="G36" s="18">
         <f>DATE(YEAR(E36),MONTH(E36)+3,DAY(E36))</f>
-        <v>44986</v>
+        <v>44988</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>294</v>
+        <v>42</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>138</v>
       </c>
       <c r="E37" s="18">
-        <v>44621</v>
+        <v>44899</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G37" s="18">
-        <f>DATE(YEAR(E37)+1,MONTH(E37),DAY(E37))</f>
-        <v>44986</v>
+        <f>DATE(YEAR(E37),MONTH(E37)+3,DAY(E37))</f>
+        <v>44989</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>269</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>138</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="20"/>
       <c r="E38" s="18">
-        <v>44897</v>
+        <v>44652</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G38" s="18">
-        <f>DATE(YEAR(E38),MONTH(E38)+3,DAY(E38))</f>
-        <v>44987</v>
+        <f>DATE(YEAR(E38)+1,MONTH(E38),DAY(E38))</f>
+        <v>45017</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>269</v>
+        <v>129</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="E39" s="18">
-        <v>44898</v>
+        <v>44652</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G39" s="18">
-        <f>DATE(YEAR(E39),MONTH(E39)+3,DAY(E39))</f>
-        <v>44988</v>
+        <f>DATE(YEAR(E39)+1,MONTH(E39),DAY(E39))</f>
+        <v>45017</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>240</v>
+      <c r="A40" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>207</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="18">
-        <v>44899</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="G40" s="18">
-        <f>DATE(YEAR(E40),MONTH(E40)+3,DAY(E40))</f>
-        <v>44989</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>216</v>
+        <v>151</v>
+      </c>
+      <c r="E40" s="36">
+        <v>44652</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="G40" s="36">
+        <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
+        <v>45017</v>
+      </c>
+      <c r="H40" s="35" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="18">
+        <v>176</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="E41" s="34">
         <v>44652</v>
       </c>
-      <c r="F41" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="G41" s="18">
-        <f t="shared" ref="G41:G46" si="1">DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
+      <c r="F41" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G41" s="36">
+        <f>DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
         <v>45017</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="35" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="18">
+      <c r="A42" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="36">
         <v>44652</v>
       </c>
-      <c r="F42" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="G42" s="18">
-        <f t="shared" si="1"/>
+      <c r="F42" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="G42" s="36">
+        <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
         <v>45017</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="35" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E43" s="22">
         <v>44652</v>
@@ -2731,7 +2738,7 @@
         <v>156</v>
       </c>
       <c r="G43" s="22">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E43)+1,MONTH(E43),DAY(E43))</f>
         <v>45017</v>
       </c>
       <c r="H43" s="21" t="s">
@@ -2740,148 +2747,144 @@
     </row>
     <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>175</v>
+        <v>86</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="D44" s="23" t="s">
-        <v>299</v>
-      </c>
-      <c r="E44" s="34">
-        <v>44652</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>156</v>
+        <v>87</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18">
+        <v>44958</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>155</v>
       </c>
       <c r="G44" s="22">
-        <f t="shared" si="1"/>
-        <v>45017</v>
+        <f>DATE(YEAR(E44),MONTH(E44)+3,DAY(E44))</f>
+        <v>45047</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>150</v>
-      </c>
+      <c r="A45" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="17"/>
       <c r="E45" s="18">
-        <v>44652</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>156</v>
+        <v>44958</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>155</v>
       </c>
       <c r="G45" s="18">
-        <f t="shared" si="1"/>
-        <v>45017</v>
+        <f>DATE(YEAR(E45),MONTH(E45)+3,DAY(E45))</f>
+        <v>45047</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="E46" s="18">
-        <v>44652</v>
+        <v>44501</v>
       </c>
       <c r="F46" s="27" t="s">
         <v>156</v>
       </c>
       <c r="G46" s="18">
-        <f t="shared" si="1"/>
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>242</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D47" s="17"/>
       <c r="E47" s="18">
-        <v>44501</v>
-      </c>
-      <c r="F47" s="19" t="s">
+        <v>44713</v>
+      </c>
+      <c r="F47" s="16" t="s">
         <v>156</v>
       </c>
       <c r="G47" s="18">
-        <v>45047</v>
+        <f>DATE(YEAR(E47)+1,MONTH(E47),DAY(E47))</f>
+        <v>45078</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="17"/>
+        <v>235</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>173</v>
+      </c>
       <c r="E48" s="18">
         <v>44713</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="F48" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G48" s="18">
-        <f t="shared" ref="G48:G68" si="2">DATE(YEAR(E48)+1,MONTH(E48),DAY(E48))</f>
+        <f>DATE(YEAR(E48)+1,MONTH(E48),DAY(E48))</f>
         <v>45078</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="D49" s="23" t="s">
-        <v>173</v>
+        <v>101</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>277</v>
       </c>
       <c r="E49" s="18">
         <v>44713</v>
@@ -2890,21 +2893,21 @@
         <v>156</v>
       </c>
       <c r="G49" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E49)+1,MONTH(E49),DAY(E49))</f>
         <v>45078</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>278</v>
       </c>
       <c r="D50" s="17" t="s">
@@ -2917,7 +2920,7 @@
         <v>156</v>
       </c>
       <c r="G50" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E50)+1,MONTH(E50),DAY(E50))</f>
         <v>45078</v>
       </c>
       <c r="H50" s="16" t="s">
@@ -2926,53 +2929,53 @@
     </row>
     <row r="51" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>102</v>
+        <v>229</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>277</v>
+        <v>230</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>275</v>
       </c>
       <c r="E51" s="18">
         <v>44713</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="F51" s="16" t="s">
         <v>156</v>
       </c>
       <c r="G51" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E51)+1,MONTH(E51),DAY(E51))</f>
         <v>45078</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>229</v>
+        <v>10</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="C52" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="D52" s="33" t="s">
-        <v>275</v>
+        <v>11</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="E52" s="18">
-        <v>44713</v>
-      </c>
-      <c r="F52" s="16" t="s">
+        <v>44743</v>
+      </c>
+      <c r="F52" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G52" s="18">
-        <f t="shared" si="2"/>
-        <v>45078</v>
+        <f>DATE(YEAR(E52)+1,MONTH(E52),DAY(E52))</f>
+        <v>45108</v>
       </c>
       <c r="H52" s="16" t="s">
         <v>216</v>
@@ -2980,16 +2983,16 @@
     </row>
     <row r="53" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>236</v>
+        <v>34</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>231</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>133</v>
+        <v>232</v>
       </c>
       <c r="E53" s="18">
         <v>44743</v>
@@ -2998,7 +3001,7 @@
         <v>156</v>
       </c>
       <c r="G53" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E53)+1,MONTH(E53),DAY(E53))</f>
         <v>45108</v>
       </c>
       <c r="H53" s="16" t="s">
@@ -3007,16 +3010,16 @@
     </row>
     <row r="54" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>232</v>
+        <v>133</v>
       </c>
       <c r="E54" s="18">
         <v>44743</v>
@@ -3025,7 +3028,7 @@
         <v>156</v>
       </c>
       <c r="G54" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
         <v>45108</v>
       </c>
       <c r="H54" s="16" t="s">
@@ -3034,13 +3037,13 @@
     </row>
     <row r="55" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D55" s="17" t="s">
         <v>133</v>
@@ -3052,7 +3055,7 @@
         <v>156</v>
       </c>
       <c r="G55" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
         <v>45108</v>
       </c>
       <c r="H55" s="16" t="s">
@@ -3061,13 +3064,13 @@
     </row>
     <row r="56" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>133</v>
@@ -3079,7 +3082,7 @@
         <v>156</v>
       </c>
       <c r="G56" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
         <v>45108</v>
       </c>
       <c r="H56" s="16" t="s">
@@ -3087,27 +3090,27 @@
       </c>
     </row>
     <row r="57" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>17</v>
+      <c r="A57" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>9</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>233</v>
+        <v>291</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E57" s="18">
-        <v>44743</v>
-      </c>
-      <c r="F57" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="E57" s="36">
+        <v>44805</v>
+      </c>
+      <c r="F57" s="37" t="s">
         <v>156</v>
       </c>
       <c r="G57" s="18">
-        <f t="shared" si="2"/>
-        <v>45108</v>
+        <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
+        <v>45170</v>
       </c>
       <c r="H57" s="16" t="s">
         <v>216</v>
@@ -3115,16 +3118,16 @@
     </row>
     <row r="58" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>292</v>
+        <v>144</v>
       </c>
       <c r="E58" s="22">
         <v>44805</v>
@@ -3133,7 +3136,7 @@
         <v>156</v>
       </c>
       <c r="G58" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
         <v>45170</v>
       </c>
       <c r="H58" s="16" t="s">
@@ -3142,16 +3145,16 @@
     </row>
     <row r="59" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>239</v>
+        <v>282</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>144</v>
+        <v>281</v>
       </c>
       <c r="E59" s="18">
         <v>44805</v>
@@ -3160,7 +3163,7 @@
         <v>156</v>
       </c>
       <c r="G59" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
         <v>45170</v>
       </c>
       <c r="H59" s="16" t="s">
@@ -3169,25 +3172,25 @@
     </row>
     <row r="60" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>31</v>
+        <v>195</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>282</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>281</v>
+        <v>196</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>193</v>
       </c>
       <c r="E60" s="18">
         <v>44805</v>
       </c>
-      <c r="F60" s="19" t="s">
+      <c r="F60" s="16" t="s">
         <v>156</v>
       </c>
       <c r="G60" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
         <v>45170</v>
       </c>
       <c r="H60" s="16" t="s">
@@ -3196,25 +3199,25 @@
     </row>
     <row r="61" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>195</v>
+        <v>55</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>196</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>286</v>
-      </c>
-      <c r="D61" s="23" t="s">
-        <v>193</v>
+        <v>56</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>143</v>
       </c>
       <c r="E61" s="18">
         <v>44805</v>
       </c>
-      <c r="F61" s="16" t="s">
+      <c r="F61" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G61" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
         <v>45170</v>
       </c>
       <c r="H61" s="16" t="s">
@@ -3223,43 +3226,43 @@
     </row>
     <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="E62" s="18">
-        <v>44805</v>
+        <v>44866</v>
       </c>
       <c r="F62" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G62" s="18">
-        <f t="shared" si="2"/>
-        <v>45170</v>
+        <f>DATE(YEAR(E62)+1,MONTH(E62),DAY(E62))</f>
+        <v>45231</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>301</v>
+        <v>244</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E63" s="18">
         <v>44866</v>
@@ -3268,35 +3271,35 @@
         <v>156</v>
       </c>
       <c r="G63" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E63)+1,MONTH(E63),DAY(E63))</f>
         <v>45231</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>244</v>
+        <v>304</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E64" s="18">
-        <v>44866</v>
+        <v>44896</v>
       </c>
       <c r="F64" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G64" s="18">
-        <f t="shared" si="2"/>
-        <v>45231</v>
+        <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
+        <v>45261</v>
       </c>
       <c r="H64" s="16" t="s">
         <v>216</v>
@@ -3304,16 +3307,16 @@
     </row>
     <row r="65" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>304</v>
+        <v>54</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>296</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E65" s="18">
         <v>44896</v>
@@ -3322,7 +3325,7 @@
         <v>156</v>
       </c>
       <c r="G65" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
         <v>45261</v>
       </c>
       <c r="H65" s="16" t="s">
@@ -3331,16 +3334,16 @@
     </row>
     <row r="66" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C66" s="31" t="s">
-        <v>296</v>
+        <v>60</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>250</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E66" s="18">
         <v>44896</v>
@@ -3349,7 +3352,7 @@
         <v>156</v>
       </c>
       <c r="G66" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E66)+1,MONTH(E66),DAY(E66))</f>
         <v>45261</v>
       </c>
       <c r="H66" s="16" t="s">
@@ -3358,29 +3361,29 @@
     </row>
     <row r="67" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>250</v>
+        <v>72</v>
+      </c>
+      <c r="C67" s="23" t="s">
+        <v>171</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
       <c r="E67" s="18">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="F67" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G67" s="18">
-        <f t="shared" si="2"/>
-        <v>45261</v>
+        <f>DATE(YEAR(E67),MONTH(E67)+12,DAY(E67))</f>
+        <v>45292</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3403,7 +3406,7 @@
         <v>156</v>
       </c>
       <c r="G68" s="18">
-        <f t="shared" si="2"/>
+        <f>DATE(YEAR(E68)+1,MONTH(E68),DAY(E68))</f>
         <v>45292</v>
       </c>
       <c r="H68" s="16" t="s">
@@ -3790,107 +3793,107 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D67" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C45" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C47" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="C71" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C43" r:id="rId8" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-statistics-supplementary-tables-2018/documents/physical-commodity-balances-of-oil-gas-and-petroleum-products/physical-commodity-balances-of-oil-gas-and-petroleum-products/govscot%3Adocument/Commodity%2BBalances%2B-%2B1998-2018.xlsx" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C40" r:id="rId8" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/09/oil-and-gas-statistics-supplementary-tables-2018/documents/physical-commodity-balances-of-oil-gas-and-petroleum-products/physical-commodity-balances-of-oil-gas-and-petroleum-products/govscot%3Adocument/Commodity%2BBalances%2B-%2B1998-2018.xlsx" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
     <hyperlink ref="C81" r:id="rId9" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="D74" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C42" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D29" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D53" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="D33" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D54" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D34" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D35" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D66" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D62" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D59" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="D67" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D64" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D16" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D8" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C39" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D25" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D26" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="D52" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="D30" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D53" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="D31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D32" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D65" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D61" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D58" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="D66" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="D63" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="D12" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D7" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
     <hyperlink ref="D4" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
     <hyperlink ref="D5" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
     <hyperlink ref="D82" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
     <hyperlink ref="D71" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D43" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="D30" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="D65" r:id="rId33" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D39" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="D63" r:id="rId35" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D40" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="D27" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D64" r:id="rId33" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D62" r:id="rId35" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
     <hyperlink ref="D78" r:id="rId36" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
     <hyperlink ref="D70" r:id="rId37" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
     <hyperlink ref="C70" r:id="rId38" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="D56" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D57" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C29" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D7" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="D9" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D10" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C21" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="D20" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D49" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D42" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D46" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="D55" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D56" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C26" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D21" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="D8" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D9" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C67" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D15" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="D48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D39" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D43" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
     <hyperlink ref="C80" r:id="rId50" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
     <hyperlink ref="C84" r:id="rId51" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
-    <hyperlink ref="D24" r:id="rId52" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
-    <hyperlink ref="C13" r:id="rId53" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
+    <hyperlink ref="D18" r:id="rId52" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
+    <hyperlink ref="C11" r:id="rId53" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
     <hyperlink ref="D75" r:id="rId54" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
     <hyperlink ref="C75" r:id="rId55" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
     <hyperlink ref="D73" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
     <hyperlink ref="C73" r:id="rId57" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
     <hyperlink ref="C78" r:id="rId58" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
-    <hyperlink ref="D12" r:id="rId59" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
-    <hyperlink ref="D61" r:id="rId60" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
-    <hyperlink ref="D23" r:id="rId61" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
+    <hyperlink ref="D10" r:id="rId59" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
+    <hyperlink ref="D60" r:id="rId60" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
+    <hyperlink ref="D17" r:id="rId61" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
     <hyperlink ref="C79" r:id="rId62" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
-    <hyperlink ref="C53" r:id="rId63" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
-    <hyperlink ref="D40" r:id="rId64" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
-    <hyperlink ref="D31" r:id="rId65" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
-    <hyperlink ref="C46" r:id="rId66" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="D22" r:id="rId67" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C59" r:id="rId68" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D11" r:id="rId69" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="C52" r:id="rId63" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
+    <hyperlink ref="D37" r:id="rId64" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
+    <hyperlink ref="D28" r:id="rId65" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
+    <hyperlink ref="C43" r:id="rId66" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
+    <hyperlink ref="D16" r:id="rId67" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C58" r:id="rId68" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
+    <hyperlink ref="D20" r:id="rId69" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
     <hyperlink ref="C83" r:id="rId70" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
-    <hyperlink ref="D19" r:id="rId71" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C28" r:id="rId72" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
-    <hyperlink ref="D47" r:id="rId73" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
+    <hyperlink ref="D14" r:id="rId71" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
+    <hyperlink ref="C25" r:id="rId72" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="D46" r:id="rId73" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
     <hyperlink ref="C2" r:id="rId74" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D32" r:id="rId75" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="D29" r:id="rId75" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
     <hyperlink ref="D79" r:id="rId76" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
-    <hyperlink ref="C44" r:id="rId77" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/04/scottish-natural-capital-accounts-2022/documents/scottish-natural-capital-accounts-2022-reference-tables/scottish-natural-capital-accounts-2022-reference-tables/govscot%3Adocument/scottish-natural-capital-accounts-2022-reference-tables.xlsx" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
+    <hyperlink ref="C41" r:id="rId77" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/04/scottish-natural-capital-accounts-2022/documents/scottish-natural-capital-accounts-2022-reference-tables/scottish-natural-capital-accounts-2022-reference-tables/govscot%3Adocument/scottish-natural-capital-accounts-2022-reference-tables.xlsx" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
     <hyperlink ref="D81" r:id="rId78" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
     <hyperlink ref="D83" r:id="rId79" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
-    <hyperlink ref="C18" r:id="rId80" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D26" r:id="rId81" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D27" r:id="rId82" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C26" r:id="rId83" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C39" r:id="rId84" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C25" r:id="rId85" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C7" r:id="rId86" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C13" r:id="rId80" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
+    <hyperlink ref="D23" r:id="rId81" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D24" r:id="rId82" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C23" r:id="rId83" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C36" r:id="rId84" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C22" r:id="rId85" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C21" r:id="rId86" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
     <hyperlink ref="C5" r:id="rId87" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="C24" r:id="rId88" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
-    <hyperlink ref="D36" r:id="rId89" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
+    <hyperlink ref="C18" r:id="rId88" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
+    <hyperlink ref="D33" r:id="rId89" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
     <hyperlink ref="C6" r:id="rId90" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
-    <hyperlink ref="D38" r:id="rId91" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
-    <hyperlink ref="C40" r:id="rId92" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
-    <hyperlink ref="C16" r:id="rId93" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
-    <hyperlink ref="C33" r:id="rId94" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
-    <hyperlink ref="D52" r:id="rId95" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
-    <hyperlink ref="C52" r:id="rId96" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
-    <hyperlink ref="C50" r:id="rId97" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
-    <hyperlink ref="C22" r:id="rId98" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
-    <hyperlink ref="C11" r:id="rId99" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
-    <hyperlink ref="C66" r:id="rId100" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
-    <hyperlink ref="C32" r:id="rId101" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
+    <hyperlink ref="D35" r:id="rId91" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
+    <hyperlink ref="C37" r:id="rId92" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
+    <hyperlink ref="C12" r:id="rId93" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
+    <hyperlink ref="C30" r:id="rId94" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
+    <hyperlink ref="D51" r:id="rId95" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
+    <hyperlink ref="C51" r:id="rId96" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
+    <hyperlink ref="C49" r:id="rId97" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
+    <hyperlink ref="C16" r:id="rId98" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
+    <hyperlink ref="C20" r:id="rId99" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
+    <hyperlink ref="C65" r:id="rId100" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
+    <hyperlink ref="C29" r:id="rId101" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId102"/>

</xml_diff>

<commit_message>
lcree and system security
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FE87B9-63E5-4330-8CB9-FDE16A0FA52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D21E95A-6250-496E-9172-ADFB4EE4385A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,9 +193,6 @@
     <t>National Grid: Data Item Explorer</t>
   </si>
   <si>
-    <t>https://www.nationalgrideso.com/balancing-data/data-finder-and-explorer</t>
-  </si>
-  <si>
     <t>NGElecDemand</t>
   </si>
   <si>
@@ -754,9 +751,6 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1086684/sub-national-road-transport-fuel-consumption-statistics-2005-2020.xlsx</t>
   </si>
   <si>
-    <t>https://www.ons.gov.uk/file?uri=/economy/environmentalaccounts/datasets/lowcarbonandrenewableenergyeconomyfirstestimatesdataset/current/lcreedataset202016022022143552.xlsx</t>
-  </si>
-  <si>
     <t>https://www.gov.uk/government/statistics/renewable-fuel-statistics-2021-fourth-provisional-report</t>
   </si>
   <si>
@@ -935,6 +929,12 @@
   </si>
   <si>
     <t>https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx</t>
+  </si>
+  <si>
+    <t>https://data.nationalgrideso.com/data-groups/demand</t>
+  </si>
+  <si>
+    <t>https://www.ons.gov.uk/file?uri=/economy/environmentalaccounts/datasets/lowcarbonandrenewableenergyeconomyfirstestimatesdataset/current/lcreedataset2021.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1095,9 +1095,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1579,7 +1576,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,10 +1598,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>99</v>
-      </c>
-      <c r="D1" t="s">
-        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1613,10 +1610,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1627,48 +1624,48 @@
         <v>51</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="15">
         <v>43862</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G2" s="15">
         <f>DATE(YEAR(E2)+1,MONTH(E2),DAY(E2))</f>
         <v>44228</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>178</v>
-      </c>
       <c r="D3" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E3" s="25">
         <v>44197</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" s="18">
         <f>DATE(YEAR(E3)+1,MONTH(E3),DAY(E3))</f>
         <v>44562</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1676,26 +1673,26 @@
         <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" s="8">
         <v>44562</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="18">
         <f>DATE(YEAR(E4),MONTH(E4)+3,DAY(E4))</f>
         <v>44652</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1703,80 +1700,80 @@
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" s="8">
         <v>44562</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G5" s="18">
         <f>DATE(YEAR(E5),MONTH(E5)+3,DAY(E5))</f>
         <v>44652</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>173</v>
-      </c>
       <c r="C6" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E6" s="18">
         <v>44743</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" s="18">
         <f>DATE(YEAR(E6),MONTH(E6)+3,DAY(E6))</f>
         <v>44835</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>96</v>
-      </c>
       <c r="C7" s="32" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="18">
         <v>44743</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" s="18">
         <f>DATE(YEAR(E7),MONTH(E7)+3,DAY(E7))</f>
         <v>44835</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1787,48 +1784,48 @@
         <v>39</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="18">
         <v>44835</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" s="18">
         <f>DATE(YEAR(E8),MONTH(E8)+1,DAY(E8))</f>
         <v>44866</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="C9" s="23" t="s">
         <v>151</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>152</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="18">
         <v>44805</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G9" s="18">
         <f>DATE(YEAR(E9),MONTH(E9)+3,DAY(E9))</f>
         <v>44896</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1836,26 +1833,26 @@
         <v>20</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="18">
         <v>44531</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" s="18">
         <f>DATE(YEAR(E10)+1,MONTH(E10),DAY(E10))</f>
         <v>44896</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1863,26 +1860,26 @@
         <v>14</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="18">
         <v>44531</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G11" s="18">
         <f>DATE(YEAR(E11)+1,MONTH(E11),DAY(E11))</f>
         <v>44896</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1896,20 +1893,20 @@
         <v>49</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="18">
         <v>44562</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" s="18">
         <f>DATE(YEAR(E12)+1,MONTH(E12),DAY(E12))</f>
         <v>44927</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1917,53 +1914,53 @@
         <v>28</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" s="18">
         <v>44835</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G13" s="18">
         <f>DATE(YEAR(E13),MONTH(E13)+4,DAY(E13))</f>
         <v>44958</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>149</v>
-      </c>
       <c r="D14" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E14" s="18">
         <v>44593</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G14" s="18">
         <f>DATE(YEAR(E14)+1,MONTH(E14),DAY(E14))</f>
         <v>44958</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1981,14 +1978,14 @@
         <v>44896</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G15" s="18">
         <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
         <v>44986</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1996,26 +1993,26 @@
         <v>16</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E16" s="18">
         <v>44958</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G16" s="18">
         <f>DATE(YEAR(E16),MONTH(E16)+1,DAY(E16))</f>
         <v>44986</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2023,26 +2020,26 @@
         <v>21</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E17" s="18">
         <v>44958</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G17" s="18">
         <f>DATE(YEAR(E17),MONTH(E17)+1,DAY(E17))</f>
         <v>44986</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2050,26 +2047,26 @@
         <v>24</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18" s="18">
         <v>44896</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G18" s="18">
         <f>DATE(YEAR(E18),MONTH(E18)+3,DAY(E18))</f>
         <v>44986</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2077,80 +2074,80 @@
         <v>25</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E19" s="18">
         <v>44896</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="18">
         <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
         <v>44986</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>171</v>
-      </c>
       <c r="C20" s="32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E20" s="18">
         <v>44866</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G20" s="18">
         <f>DATE(YEAR(E20),MONTH(E20)+4,DAY(E20))</f>
         <v>44986</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>86</v>
-      </c>
       <c r="C21" s="31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E21" s="18">
         <v>44896</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G21" s="18">
         <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
         <v>44986</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2161,129 +2158,129 @@
         <v>44</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E22" s="18">
         <v>44621</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G22" s="18">
         <f>DATE(YEAR(E22)+1,MONTH(E22),DAY(E22))</f>
         <v>44986</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="C23" s="20" t="s">
         <v>132</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>133</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="18">
         <v>44652</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G23" s="18">
         <f>DATE(YEAR(E23)+1,MONTH(E23),DAY(E23))</f>
         <v>45017</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>144</v>
-      </c>
       <c r="C24" s="33" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E24" s="34">
         <v>44652</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G24" s="18">
         <f>DATE(YEAR(E24)+1,MONTH(E24),DAY(E24))</f>
         <v>45017</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="C25" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="23" t="s">
-        <v>191</v>
-      </c>
       <c r="D25" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E25" s="18">
         <v>44652</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G25" s="18">
         <f>DATE(YEAR(E25)+1,MONTH(E25),DAY(E25))</f>
         <v>45017</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>74</v>
-      </c>
       <c r="C26" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E26" s="18">
         <v>44652</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G26" s="18">
         <f>DATE(YEAR(E26)+1,MONTH(E26),DAY(E26))</f>
         <v>45017</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2294,126 +2291,126 @@
         <v>56</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="18">
-        <v>44958</v>
+        <v>45017</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G27" s="18">
         <f>DATE(YEAR(E27),MONTH(E27)+3,DAY(E27))</f>
-        <v>45047</v>
+        <v>45108</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="C28" s="17" t="s">
-        <v>57</v>
+        <v>303</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="18">
-        <v>44958</v>
+        <v>45017</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G28" s="18">
         <f>DATE(YEAR(E28),MONTH(E28)+3,DAY(E28))</f>
+        <v>45108</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E29" s="18">
+        <v>44501</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="18">
         <v>45047</v>
       </c>
-      <c r="H28" s="16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="E29" s="36">
-        <v>44501</v>
-      </c>
-      <c r="F29" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="G29" s="36">
-        <v>45047</v>
-      </c>
-      <c r="H29" s="35" t="s">
-        <v>181</v>
+      <c r="H29" s="16" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" t="s">
+        <v>276</v>
+      </c>
+      <c r="C30" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="B30" t="s">
-        <v>278</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>233</v>
-      </c>
       <c r="D30" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" s="18">
         <v>44986</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G30" s="18">
-        <f>DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
+        <f t="shared" ref="G30:G39" si="0">DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
         <v>45078</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>228</v>
-      </c>
       <c r="D31" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E31" s="1">
         <v>44986</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G31" s="18">
-        <f>DATE(YEAR(E31),MONTH(E31)+3,DAY(E31))</f>
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2421,26 +2418,26 @@
         <v>35</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="1">
         <v>44986</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G32" s="18">
-        <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2448,53 +2445,53 @@
         <v>34</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E33" s="1">
         <v>44986</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G33" s="18">
-        <f>DATE(YEAR(E33),MONTH(E33)+3,DAY(E33))</f>
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B34" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E34" s="18">
         <v>44986</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G34" s="18">
-        <f>DATE(YEAR(E34),MONTH(E34)+3,DAY(E34))</f>
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2502,26 +2499,26 @@
         <v>22</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E35" s="18">
         <v>44986</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G35" s="18">
-        <f>DATE(YEAR(E35),MONTH(E35)+3,DAY(E35))</f>
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2529,26 +2526,26 @@
         <v>23</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E36" s="18">
         <v>44986</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G36" s="18">
-        <f>DATE(YEAR(E36),MONTH(E36)+3,DAY(E36))</f>
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2556,26 +2553,26 @@
         <v>17</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E37" s="18">
         <v>44986</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="G37" s="36">
-        <f>DATE(YEAR(E37),MONTH(E37)+3,DAY(E37))</f>
+        <v>123</v>
+      </c>
+      <c r="G37" s="18">
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
-      <c r="H37" s="35" t="s">
-        <v>180</v>
+      <c r="H37" s="16" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2583,213 +2580,213 @@
         <v>26</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E38" s="18">
         <v>44986</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G38" s="18">
-        <f>DATE(YEAR(E38),MONTH(E38)+3,DAY(E38))</f>
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
-      <c r="H38" s="35" t="s">
-        <v>180</v>
+      <c r="H38" s="16" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="35" t="s">
-        <v>268</v>
+      <c r="B39" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" s="36">
+        <v>108</v>
+      </c>
+      <c r="E39" s="18">
         <v>44986</v>
       </c>
-      <c r="F39" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="G39" s="36">
-        <f>DATE(YEAR(E39),MONTH(E39)+3,DAY(E39))</f>
+      <c r="F39" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" s="18">
+        <f t="shared" si="0"/>
         <v>45078</v>
       </c>
-      <c r="H39" s="35" t="s">
-        <v>180</v>
+      <c r="H39" s="16" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="C40" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="18">
         <v>44713</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="G40" s="36">
+        <v>124</v>
+      </c>
+      <c r="G40" s="18">
         <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
         <v>45078</v>
       </c>
-      <c r="H40" s="35" t="s">
-        <v>185</v>
+      <c r="H40" s="16" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="16" t="s">
-        <v>61</v>
-      </c>
       <c r="C41" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E41" s="18">
         <v>44713</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G41" s="18">
         <f>DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
         <v>45078</v>
       </c>
-      <c r="H41" s="35" t="s">
-        <v>181</v>
+      <c r="H41" s="16" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="35" t="s">
-        <v>70</v>
-      </c>
       <c r="C42" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E42" s="18">
         <v>44713</v>
       </c>
-      <c r="F42" s="37" t="s">
-        <v>125</v>
+      <c r="F42" s="19" t="s">
+        <v>124</v>
       </c>
       <c r="G42" s="18">
         <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
         <v>45078</v>
       </c>
-      <c r="H42" s="35" t="s">
-        <v>183</v>
+      <c r="H42" s="16" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B43" s="21" t="s">
-        <v>72</v>
-      </c>
       <c r="C43" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E43" s="22">
         <v>44713</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G43" s="22">
         <f>DATE(YEAR(E43)+1,MONTH(E43),DAY(E43))</f>
         <v>45078</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C44" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D44" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E44" s="18">
         <v>44713</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G44" s="22">
         <f>DATE(YEAR(E44)+1,MONTH(E44),DAY(E44))</f>
         <v>45078</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E45" s="1">
         <v>44987</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G45" s="18">
         <f>DATE(YEAR(E45),MONTH(E45)+3,DAY(E45))</f>
         <v>45079</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2797,26 +2794,26 @@
         <v>4</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E46" s="1">
         <v>44988</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G46" s="18">
         <f>DATE(YEAR(E46),MONTH(E46)+3,DAY(E46))</f>
         <v>45080</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2824,26 +2821,26 @@
         <v>5</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E47" s="1">
         <v>44989</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G47" s="18">
         <f>DATE(YEAR(E47),MONTH(E47)+3,DAY(E47))</f>
         <v>45081</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2851,26 +2848,26 @@
         <v>7</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E48" s="18">
         <v>44743</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G48" s="18">
         <f>DATE(YEAR(E48)+1,MONTH(E48),DAY(E48))</f>
         <v>45108</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2878,26 +2875,26 @@
         <v>19</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C49" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D49" s="17" t="s">
         <v>194</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>195</v>
       </c>
       <c r="E49" s="18">
         <v>44743</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G49" s="18">
         <f>DATE(YEAR(E49)+1,MONTH(E49),DAY(E49))</f>
         <v>45108</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2905,26 +2902,26 @@
         <v>8</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E50" s="18">
         <v>44743</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G50" s="18">
         <f>DATE(YEAR(E50)+1,MONTH(E50),DAY(E50))</f>
         <v>45108</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2932,26 +2929,26 @@
         <v>9</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E51" s="18">
         <v>44743</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G51" s="18">
         <f>DATE(YEAR(E51)+1,MONTH(E51),DAY(E51))</f>
         <v>45108</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2959,53 +2956,53 @@
         <v>10</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E52" s="18">
         <v>44743</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G52" s="18">
         <f>DATE(YEAR(E52)+1,MONTH(E52),DAY(E52))</f>
         <v>45108</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="C53" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D53" s="23" t="s">
         <v>163</v>
-      </c>
-      <c r="C53" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>164</v>
       </c>
       <c r="E53" s="18">
         <v>44958</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G53" s="18">
         <f>DATE(YEAR(E53),MONTH(E53)+6,DAY(E53))</f>
         <v>45139</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3013,53 +3010,53 @@
         <v>6</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E54" s="18">
         <v>44805</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G54" s="18">
-        <f>DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
+        <f t="shared" ref="G54:G65" si="1">DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
         <v>45170</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="35" t="s">
-        <v>293</v>
+      <c r="B55" s="16" t="s">
+        <v>291</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="E55" s="36">
+        <v>112</v>
+      </c>
+      <c r="E55" s="18">
         <v>44805</v>
       </c>
-      <c r="F55" s="37" t="s">
-        <v>125</v>
+      <c r="F55" s="19" t="s">
+        <v>124</v>
       </c>
       <c r="G55" s="18">
-        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
+        <f t="shared" si="1"/>
         <v>45170</v>
       </c>
       <c r="H55" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3067,53 +3064,53 @@
         <v>18</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E56" s="18">
         <v>44805</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G56" s="18">
-        <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
+        <f t="shared" si="1"/>
         <v>45170</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E57" s="18">
         <v>44805</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G57" s="18">
-        <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
+        <f t="shared" si="1"/>
         <v>45170</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -3121,53 +3118,53 @@
         <v>30</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E58" s="22">
         <v>44805</v>
       </c>
       <c r="F58" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G58" s="18">
-        <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
+        <f t="shared" si="1"/>
         <v>45170</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="16" t="s">
-        <v>66</v>
-      </c>
       <c r="C59" s="17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E59" s="18">
         <v>44866</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G59" s="18">
-        <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
+        <f t="shared" si="1"/>
         <v>45231</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3175,53 +3172,53 @@
         <v>33</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E60" s="18">
         <v>44866</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G60" s="18">
-        <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
+        <f t="shared" si="1"/>
         <v>45231</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" s="23" t="s">
         <v>159</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="C61" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="D61" s="23" t="s">
-        <v>160</v>
       </c>
       <c r="E61" s="18">
         <v>44896</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G61" s="18">
-        <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
+        <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3229,26 +3226,26 @@
         <v>11</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E62" s="18">
         <v>44896</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G62" s="18">
-        <f>DATE(YEAR(E62)+1,MONTH(E62),DAY(E62))</f>
+        <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3256,26 +3253,26 @@
         <v>29</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E63" s="18">
         <v>44896</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G63" s="18">
-        <f>DATE(YEAR(E63)+1,MONTH(E63),DAY(E63))</f>
+        <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3283,53 +3280,53 @@
         <v>32</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E64" s="18">
         <v>44896</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G64" s="18">
-        <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
+        <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="16" t="s">
-        <v>79</v>
-      </c>
       <c r="C65" s="31" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E65" s="18">
         <v>44927</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G65" s="18">
-        <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
+        <f t="shared" si="1"/>
         <v>45292</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3340,7 +3337,7 @@
         <v>41</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D66" s="17" t="s">
         <v>42</v>
@@ -3349,68 +3346,68 @@
         <v>44927</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G66" s="18">
         <f>DATE(YEAR(E66),MONTH(E66)+12,DAY(E66))</f>
         <v>45292</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="C67" s="17" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E67" s="18">
         <v>44927</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G67" s="18">
         <f>DATE(YEAR(E67)+1,MONTH(E67),DAY(E67))</f>
         <v>45292</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>98</v>
-      </c>
       <c r="C68" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E68" s="18">
         <v>45017</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G68" s="18">
         <f>DATE(YEAR(E68)+1,MONTH(E68),DAY(E68))</f>
         <v>45383</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3425,50 +3422,50 @@
     </row>
     <row r="70" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D70" s="20" t="s">
         <v>128</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C70" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>129</v>
       </c>
       <c r="E70" s="18">
         <v>43435</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G70" s="18"/>
       <c r="H70" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="C71" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C71" s="17" t="s">
-        <v>77</v>
-      </c>
       <c r="D71" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E71" s="18">
         <v>43447</v>
       </c>
       <c r="F71" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3476,7 +3473,7 @@
         <v>15</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
@@ -3486,7 +3483,7 @@
         <v>43466</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G72" s="8"/>
       <c r="H72" s="4" t="s">
@@ -3495,46 +3492,46 @@
     </row>
     <row r="73" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="C73" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E73" s="15">
         <v>43831</v>
       </c>
       <c r="F73" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C74" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E74" s="18">
         <v>43831</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="16" t="s">
@@ -3543,26 +3540,26 @@
     </row>
     <row r="75" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D75" s="14" t="s">
         <v>154</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>155</v>
       </c>
       <c r="E75" s="15">
         <v>43908</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3570,7 +3567,7 @@
         <v>12</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>13</v>
@@ -3580,7 +3577,7 @@
         <v>43916</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="4" t="s">
@@ -3589,10 +3586,10 @@
     </row>
     <row r="77" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" s="16" t="s">
         <v>87</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>88</v>
       </c>
       <c r="C77" s="17" t="s">
         <v>13</v>
@@ -3602,7 +3599,7 @@
         <v>43950</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G77" s="18"/>
       <c r="H77" s="16" t="s">
@@ -3611,136 +3608,136 @@
     </row>
     <row r="78" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>92</v>
-      </c>
       <c r="C78" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E78" s="18">
         <v>43950</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G78" s="18"/>
       <c r="H78" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="C79" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>168</v>
-      </c>
       <c r="D79" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E79" s="8">
         <v>44044</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G79" s="8"/>
       <c r="H79" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E80" s="8">
         <v>44166</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G80" s="8"/>
       <c r="H80" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B81" s="16" t="s">
-        <v>90</v>
-      </c>
       <c r="C81" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E81" s="18">
         <v>44166</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G81" s="18"/>
       <c r="H81" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>68</v>
-      </c>
       <c r="C82" s="17" t="s">
-        <v>244</v>
+        <v>304</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E82" s="18">
         <v>44986</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G82" s="18"/>
       <c r="H82" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="C83" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D83" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="E83" s="8">
         <v>44256</v>
@@ -3748,33 +3745,33 @@
       <c r="F83" s="4"/>
       <c r="G83" s="8"/>
       <c r="H83" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8"/>
       <c r="F84" s="4"/>
       <c r="G84" s="8"/>
       <c r="H84" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>13</v>
@@ -3797,109 +3794,108 @@
     <hyperlink ref="C12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="C15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="C27" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C40" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C71" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C81" r:id="rId8" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D74" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C68" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D46" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D47" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D48" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="D37" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D49" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D38" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D39" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D63" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D58" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D55" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="D64" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D60" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D33" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D32" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D4" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D5" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="D82" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="D71" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D18" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="D62" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="D59" r:id="rId33" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="D78" r:id="rId34" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="D70" r:id="rId35" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C70" r:id="rId36" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="D51" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D52" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C47" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D17" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="D7" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D8" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C66" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="D12" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D41" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D68" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D26" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="C80" r:id="rId48" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
-    <hyperlink ref="C84" r:id="rId49" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
-    <hyperlink ref="D14" r:id="rId50" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
-    <hyperlink ref="C9" r:id="rId51" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
-    <hyperlink ref="D75" r:id="rId52" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
-    <hyperlink ref="C75" r:id="rId53" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
-    <hyperlink ref="D73" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C73" r:id="rId55" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
-    <hyperlink ref="C78" r:id="rId56" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
-    <hyperlink ref="D61" r:id="rId57" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
-    <hyperlink ref="D57" r:id="rId58" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
-    <hyperlink ref="D53" r:id="rId59" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
-    <hyperlink ref="C79" r:id="rId60" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
-    <hyperlink ref="C48" r:id="rId61" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
-    <hyperlink ref="D36" r:id="rId62" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
-    <hyperlink ref="D19" r:id="rId63" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
-    <hyperlink ref="C26" r:id="rId64" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="D13" r:id="rId65" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C55" r:id="rId66" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D16" r:id="rId67" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
-    <hyperlink ref="C83" r:id="rId68" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
-    <hyperlink ref="D11" r:id="rId69" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C46" r:id="rId70" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
-    <hyperlink ref="D29" r:id="rId71" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
-    <hyperlink ref="C2" r:id="rId72" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D20" r:id="rId73" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
-    <hyperlink ref="D79" r:id="rId74" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
-    <hyperlink ref="C24" r:id="rId75" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/04/scottish-natural-capital-accounts-2022/documents/scottish-natural-capital-accounts-2022-reference-tables/scottish-natural-capital-accounts-2022-reference-tables/govscot%3Adocument/scottish-natural-capital-accounts-2022-reference-tables.xlsx" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
-    <hyperlink ref="D81" r:id="rId76" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
-    <hyperlink ref="D83" r:id="rId77" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
-    <hyperlink ref="C10" r:id="rId78" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D31" r:id="rId79" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D45" r:id="rId80" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C31" r:id="rId81" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C35" r:id="rId82" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C30" r:id="rId83" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C17" r:id="rId84" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
-    <hyperlink ref="C5" r:id="rId85" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="C14" r:id="rId86" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
-    <hyperlink ref="D21" r:id="rId87" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
-    <hyperlink ref="C6" r:id="rId88" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
-    <hyperlink ref="D34" r:id="rId89" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
-    <hyperlink ref="C36" r:id="rId90" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
-    <hyperlink ref="C33" r:id="rId91" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
-    <hyperlink ref="C37" r:id="rId92" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
-    <hyperlink ref="D44" r:id="rId93" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
-    <hyperlink ref="C44" r:id="rId94" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
-    <hyperlink ref="C42" r:id="rId95" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
-    <hyperlink ref="C13" r:id="rId96" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
-    <hyperlink ref="C16" r:id="rId97" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
-    <hyperlink ref="C63" r:id="rId98" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
-    <hyperlink ref="C20" r:id="rId99" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
-    <hyperlink ref="C61" r:id="rId100" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
-    <hyperlink ref="C65" r:id="rId101" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
-    <hyperlink ref="D24" r:id="rId102" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
+    <hyperlink ref="C40" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C71" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C81" r:id="rId7" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D74" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C68" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D46" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D47" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="D48" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="D37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D49" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="D38" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D63" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D58" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D55" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="D64" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="D60" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="D33" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D4" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="D5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="D82" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="D71" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="D18" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D35" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D59" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D78" r:id="rId33" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="D70" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C70" r:id="rId35" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="D51" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D52" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C47" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D17" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="D7" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D8" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C66" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D12" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="D41" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D68" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D26" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="C80" r:id="rId47" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
+    <hyperlink ref="C84" r:id="rId48" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
+    <hyperlink ref="D14" r:id="rId49" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
+    <hyperlink ref="C9" r:id="rId50" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
+    <hyperlink ref="D75" r:id="rId51" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
+    <hyperlink ref="C75" r:id="rId52" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
+    <hyperlink ref="D73" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C73" r:id="rId54" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
+    <hyperlink ref="C78" r:id="rId55" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
+    <hyperlink ref="D61" r:id="rId56" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
+    <hyperlink ref="D57" r:id="rId57" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
+    <hyperlink ref="D53" r:id="rId58" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
+    <hyperlink ref="C79" r:id="rId59" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
+    <hyperlink ref="C48" r:id="rId60" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
+    <hyperlink ref="D36" r:id="rId61" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
+    <hyperlink ref="D19" r:id="rId62" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
+    <hyperlink ref="C26" r:id="rId63" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
+    <hyperlink ref="D13" r:id="rId64" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C55" r:id="rId65" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
+    <hyperlink ref="D16" r:id="rId66" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="C83" r:id="rId67" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
+    <hyperlink ref="D11" r:id="rId68" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
+    <hyperlink ref="C46" r:id="rId69" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="D29" r:id="rId70" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
+    <hyperlink ref="C2" r:id="rId71" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
+    <hyperlink ref="D20" r:id="rId72" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="D79" r:id="rId73" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
+    <hyperlink ref="C24" r:id="rId74" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/04/scottish-natural-capital-accounts-2022/documents/scottish-natural-capital-accounts-2022-reference-tables/scottish-natural-capital-accounts-2022-reference-tables/govscot%3Adocument/scottish-natural-capital-accounts-2022-reference-tables.xlsx" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
+    <hyperlink ref="D81" r:id="rId75" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
+    <hyperlink ref="D83" r:id="rId76" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
+    <hyperlink ref="C10" r:id="rId77" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
+    <hyperlink ref="D31" r:id="rId78" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D45" r:id="rId79" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C31" r:id="rId80" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C35" r:id="rId81" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C30" r:id="rId82" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C17" r:id="rId83" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C5" r:id="rId84" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
+    <hyperlink ref="C14" r:id="rId85" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
+    <hyperlink ref="D21" r:id="rId86" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
+    <hyperlink ref="C6" r:id="rId87" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
+    <hyperlink ref="D34" r:id="rId88" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
+    <hyperlink ref="C36" r:id="rId89" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
+    <hyperlink ref="C33" r:id="rId90" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
+    <hyperlink ref="C37" r:id="rId91" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
+    <hyperlink ref="D44" r:id="rId92" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
+    <hyperlink ref="C44" r:id="rId93" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
+    <hyperlink ref="C42" r:id="rId94" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
+    <hyperlink ref="C13" r:id="rId95" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
+    <hyperlink ref="C16" r:id="rId96" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
+    <hyperlink ref="C63" r:id="rId97" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
+    <hyperlink ref="C20" r:id="rId98" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
+    <hyperlink ref="C61" r:id="rId99" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
+    <hyperlink ref="C65" r:id="rId100" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
+    <hyperlink ref="D24" r:id="rId101" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId103"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId102"/>
   <tableParts count="1">
-    <tablePart r:id="rId104"/>
+    <tablePart r:id="rId103"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Renewable heat report 2023 update
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D21E95A-6250-496E-9172-ADFB4EE4385A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01587EB-D9B7-444B-A671-8A48F529CEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25455" yWindow="2115" windowWidth="19200" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -784,9 +784,6 @@
     <t>https://energysavingtrust.org.uk/report/community-and-locally-owned-energy-in-scotland-2021-report/</t>
   </si>
   <si>
-    <t>https://energysavingtrust.org.uk/wp-content/uploads/2022/03/Community-and-locally-owned-energy-report-2021.pdf</t>
-  </si>
-  <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1115149/subnational_electricity_consumption_statistics_2005-2020.xlsx</t>
   </si>
   <si>
@@ -935,6 +932,9 @@
   </si>
   <si>
     <t>https://www.ons.gov.uk/file?uri=/economy/environmentalaccounts/datasets/lowcarbonandrenewableenergyeconomyfirstestimatesdataset/current/lcreedataset2021.xlsx</t>
+  </si>
+  <si>
+    <t>https://energysavingtrust.org.uk/wp-content/uploads/2023/03/Community-and-Locally-Owned-Energy-report-2022.pdf</t>
   </si>
 </sst>
 </file>
@@ -1575,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,7 +1833,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>216</v>
@@ -1842,14 +1842,14 @@
         <v>104</v>
       </c>
       <c r="E10" s="18">
-        <v>44531</v>
+        <v>44896</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G10" s="18">
         <f>DATE(YEAR(E10)+1,MONTH(E10),DAY(E10))</f>
-        <v>44896</v>
+        <v>45261</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>179</v>
@@ -1860,7 +1860,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>212</v>
@@ -1914,10 +1914,10 @@
         <v>28</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>109</v>
@@ -1941,7 +1941,7 @@
         <v>147</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>148</v>
@@ -1993,7 +1993,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>252</v>
@@ -2020,7 +2020,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>217</v>
@@ -2047,7 +2047,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>218</v>
@@ -2074,7 +2074,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>219</v>
@@ -2104,7 +2104,7 @@
         <v>170</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>223</v>
@@ -2157,21 +2157,21 @@
       <c r="B22" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>254</v>
+      <c r="C22" s="31" t="s">
+        <v>304</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>253</v>
       </c>
       <c r="E22" s="18">
-        <v>44621</v>
+        <v>44986</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G22" s="18">
         <f>DATE(YEAR(E22)+1,MONTH(E22),DAY(E22))</f>
-        <v>44986</v>
+        <v>45352</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>180</v>
@@ -2210,10 +2210,10 @@
         <v>143</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E24" s="34">
         <v>44652</v>
@@ -2316,7 +2316,7 @@
         <v>58</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="18">
@@ -2347,13 +2347,14 @@
         <v>204</v>
       </c>
       <c r="E29" s="18">
-        <v>44501</v>
+        <v>45047</v>
       </c>
       <c r="F29" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G29" s="18">
-        <v>45047</v>
+        <f>DATE(YEAR(E29)+1,MONTH(E29),DAY(E29))</f>
+        <v>45413</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>180</v>
@@ -2364,7 +2365,7 @@
         <v>231</v>
       </c>
       <c r="B30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" s="31" t="s">
         <v>232</v>
@@ -2391,7 +2392,7 @@
         <v>226</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>227</v>
@@ -2418,7 +2419,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>221</v>
@@ -2445,7 +2446,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C33" s="31" t="s">
         <v>220</v>
@@ -2472,7 +2473,7 @@
         <v>230</v>
       </c>
       <c r="B34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>229</v>
@@ -2499,7 +2500,7 @@
         <v>22</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>229</v>
@@ -2526,7 +2527,7 @@
         <v>23</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C36" s="31" t="s">
         <v>202</v>
@@ -2553,7 +2554,7 @@
         <v>17</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>213</v>
@@ -2580,7 +2581,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>239</v>
@@ -2607,7 +2608,7 @@
         <v>27</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C39" s="31" t="s">
         <v>240</v>
@@ -2740,7 +2741,7 @@
         <v>192</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>236</v>
@@ -2767,7 +2768,7 @@
         <v>225</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>228</v>
@@ -2794,7 +2795,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>214</v>
@@ -2821,7 +2822,7 @@
         <v>5</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>215</v>
@@ -2848,7 +2849,7 @@
         <v>7</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>198</v>
@@ -2875,7 +2876,7 @@
         <v>19</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>193</v>
@@ -2902,7 +2903,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C50" s="17" t="s">
         <v>199</v>
@@ -2929,7 +2930,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>200</v>
@@ -2956,7 +2957,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>195</v>
@@ -3010,7 +3011,7 @@
         <v>6</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>250</v>
@@ -3037,7 +3038,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>201</v>
@@ -3064,7 +3065,7 @@
         <v>18</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C56" s="17" t="s">
         <v>242</v>
@@ -3091,7 +3092,7 @@
         <v>160</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C57" s="23" t="s">
         <v>245</v>
@@ -3118,7 +3119,7 @@
         <v>30</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C58" s="26" t="s">
         <v>246</v>
@@ -3148,7 +3149,7 @@
         <v>65</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>126</v>
@@ -3172,7 +3173,7 @@
         <v>33</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>206</v>
@@ -3199,7 +3200,7 @@
         <v>158</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C61" s="33" t="s">
         <v>168</v>
@@ -3226,10 +3227,10 @@
         <v>11</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D62" s="17" t="s">
         <v>102</v>
@@ -3253,10 +3254,10 @@
         <v>29</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D63" s="17" t="s">
         <v>110</v>
@@ -3280,7 +3281,7 @@
         <v>32</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C64" s="17" t="s">
         <v>212</v>
@@ -3310,10 +3311,10 @@
         <v>78</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E65" s="18">
         <v>44927</v>
@@ -3364,10 +3365,10 @@
         <v>81</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E67" s="18">
         <v>44927</v>
@@ -3473,7 +3474,7 @@
         <v>15</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
@@ -3567,7 +3568,7 @@
         <v>12</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>13</v>
@@ -3659,7 +3660,7 @@
         <v>141</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>135</v>
@@ -3710,7 +3711,7 @@
         <v>67</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D82" s="17" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
June 2023 quarterly update
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01587EB-D9B7-444B-A671-8A48F529CEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE903EB-6494-46D9-9FFC-AC69C8090B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25455" yWindow="2115" windowWidth="19200" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1059,7 +1059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1095,6 +1095,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1575,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,26 +1833,26 @@
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E10" s="18">
-        <v>44896</v>
+        <v>44531</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G10" s="18">
         <f>DATE(YEAR(E10)+1,MONTH(E10),DAY(E10))</f>
-        <v>45261</v>
+        <v>44896</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>179</v>
@@ -1857,79 +1860,79 @@
     </row>
     <row r="11" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>270</v>
+        <v>48</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>113</v>
+        <v>49</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>139</v>
       </c>
       <c r="E11" s="18">
-        <v>44531</v>
+        <v>44562</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G11" s="18">
         <f>DATE(YEAR(E11)+1,MONTH(E11),DAY(E11))</f>
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>139</v>
+        <v>271</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>109</v>
       </c>
       <c r="E12" s="18">
-        <v>44562</v>
+        <v>44835</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G12" s="18">
-        <f>DATE(YEAR(E12)+1,MONTH(E12),DAY(E12))</f>
-        <v>44927</v>
+        <f>DATE(YEAR(E12),MONTH(E12)+4,DAY(E12))</f>
+        <v>44958</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>256</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>109</v>
+        <v>272</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="E13" s="18">
-        <v>44835</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>123</v>
+        <v>44593</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="G13" s="18">
-        <f>DATE(YEAR(E13),MONTH(E13)+4,DAY(E13))</f>
+        <f>DATE(YEAR(E13)+1,MONTH(E13),DAY(E13))</f>
         <v>44958</v>
       </c>
       <c r="H13" s="16" t="s">
@@ -1938,68 +1941,68 @@
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>147</v>
+        <v>52</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>135</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="17"/>
       <c r="E14" s="18">
-        <v>44593</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>124</v>
+        <v>44896</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="G14" s="18">
-        <f>DATE(YEAR(E14)+1,MONTH(E14),DAY(E14))</f>
-        <v>44958</v>
+        <f>DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
+        <v>44986</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="17"/>
+        <v>273</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>205</v>
+      </c>
       <c r="E15" s="18">
-        <v>44896</v>
+        <v>44958</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G15" s="18">
-        <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
+        <f>DATE(YEAR(E15),MONTH(E15)+1,DAY(E15))</f>
         <v>44986</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
       <c r="E16" s="18">
         <v>44958</v>
@@ -2017,25 +2020,25 @@
     </row>
     <row r="17" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>217</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>105</v>
+        <v>280</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="E17" s="18">
-        <v>44958</v>
+        <v>44896</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G17" s="18">
-        <f>DATE(YEAR(E17),MONTH(E17)+1,DAY(E17))</f>
+        <f>DATE(YEAR(E17),MONTH(E17)+3,DAY(E17))</f>
         <v>44986</v>
       </c>
       <c r="H17" s="16" t="s">
@@ -2044,16 +2047,16 @@
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="E18" s="18">
         <v>44896</v>
@@ -2071,107 +2074,105 @@
     </row>
     <row r="19" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>106</v>
+        <v>170</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>223</v>
       </c>
       <c r="E19" s="18">
-        <v>44896</v>
+        <v>44866</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G19" s="18">
-        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
+        <f>DATE(YEAR(E19),MONTH(E19)+4,DAY(E19))</f>
         <v>44986</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>169</v>
+        <v>84</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>223</v>
+        <v>85</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>233</v>
       </c>
       <c r="E20" s="18">
-        <v>44866</v>
+        <v>44896</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G20" s="18">
-        <f>DATE(YEAR(E20),MONTH(E20)+4,DAY(E20))</f>
+        <f>DATE(YEAR(E20),MONTH(E20)+3,DAY(E20))</f>
         <v>44986</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>233</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="20"/>
       <c r="E21" s="18">
-        <v>44896</v>
+        <v>44652</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G21" s="18">
-        <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
-        <v>44986</v>
+        <f>DATE(YEAR(E21)+1,MONTH(E21),DAY(E21))</f>
+        <v>45017</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>304</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="E22" s="18">
-        <v>44986</v>
-      </c>
-      <c r="F22" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="E22" s="34">
+        <v>44652</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G22" s="18">
         <f>DATE(YEAR(E22)+1,MONTH(E22),DAY(E22))</f>
-        <v>45352</v>
+        <v>45017</v>
       </c>
       <c r="H22" s="16" t="s">
         <v>180</v>
@@ -2179,19 +2180,21 @@
     </row>
     <row r="23" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" s="20"/>
+        <v>189</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>118</v>
+      </c>
       <c r="E23" s="18">
         <v>44652</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G23" s="18">
@@ -2199,26 +2202,26 @@
         <v>45017</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>258</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>257</v>
-      </c>
-      <c r="E24" s="34">
+        <v>73</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="18">
         <v>44652</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G24" s="18">
@@ -2226,151 +2229,155 @@
         <v>45017</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>118</v>
+        <v>231</v>
+      </c>
+      <c r="B25" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>106</v>
       </c>
       <c r="E25" s="18">
-        <v>44652</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>124</v>
+        <v>44986</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="G25" s="18">
-        <f>DATE(YEAR(E25)+1,MONTH(E25),DAY(E25))</f>
-        <v>45017</v>
+        <f>DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
+        <v>45078</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>72</v>
+        <v>226</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>73</v>
+        <v>276</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="18">
-        <v>44652</v>
+        <v>100</v>
+      </c>
+      <c r="E26" s="1">
+        <v>44986</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G26" s="18">
-        <f>DATE(YEAR(E26)+1,MONTH(E26),DAY(E26))</f>
-        <v>45017</v>
+        <f>DATE(YEAR(E26),MONTH(E26)+3,DAY(E26))</f>
+        <v>45078</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>56</v>
+        <v>266</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="18">
-        <v>45017</v>
+        <v>221</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1">
+        <v>44986</v>
       </c>
       <c r="F27" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G27" s="18">
         <f>DATE(YEAR(E27),MONTH(E27)+3,DAY(E27))</f>
-        <v>45108</v>
+        <v>45078</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="18">
-        <v>45017</v>
+        <v>268</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="1">
+        <v>44986</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G28" s="18">
         <f>DATE(YEAR(E28),MONTH(E28)+3,DAY(E28))</f>
-        <v>45108</v>
+        <v>45078</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>204</v>
+        <v>230</v>
+      </c>
+      <c r="B29" t="s">
+        <v>282</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>106</v>
       </c>
       <c r="E29" s="18">
-        <v>45047</v>
+        <v>44986</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G29" s="18">
-        <f>DATE(YEAR(E29)+1,MONTH(E29),DAY(E29))</f>
-        <v>45413</v>
+        <f>DATE(YEAR(E29),MONTH(E29)+3,DAY(E29))</f>
+        <v>45078</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="B30" t="s">
-        <v>275</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="D30" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>106</v>
       </c>
       <c r="E30" s="18">
@@ -2380,7 +2387,7 @@
         <v>123</v>
       </c>
       <c r="G30" s="18">
-        <f t="shared" ref="G30:G39" si="0">DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
+        <f>DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
         <v>45078</v>
       </c>
       <c r="H30" s="16" t="s">
@@ -2389,25 +2396,25 @@
     </row>
     <row r="31" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>226</v>
+        <v>23</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>227</v>
+        <v>275</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>202</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="1">
+        <v>106</v>
+      </c>
+      <c r="E31" s="18">
         <v>44986</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G31" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E31),MONTH(E31)+3,DAY(E31))</f>
         <v>45078</v>
       </c>
       <c r="H31" s="16" t="s">
@@ -2416,348 +2423,344 @@
     </row>
     <row r="32" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>266</v>
+        <v>62</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="1">
-        <v>44986</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>123</v>
+        <v>63</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18">
+        <v>44713</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="G32" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E32)+1,MONTH(E32),DAY(E32))</f>
         <v>45078</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>220</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="1">
-        <v>44986</v>
+        <v>60</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="18">
+        <v>44713</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G33" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E33)+1,MONTH(E33),DAY(E33))</f>
         <v>45078</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="B34" t="s">
-        <v>282</v>
+        <v>68</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>106</v>
+        <v>238</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>237</v>
       </c>
       <c r="E34" s="18">
-        <v>44986</v>
+        <v>44713</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G34" s="18">
-        <f t="shared" si="0"/>
+        <f>DATE(YEAR(E34)+1,MONTH(E34),DAY(E34))</f>
         <v>45078</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>282</v>
+      <c r="A35" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>71</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E35" s="18">
-        <v>44986</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="G35" s="18">
-        <f t="shared" si="0"/>
+        <v>237</v>
+      </c>
+      <c r="E35" s="36">
+        <v>44713</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="G35" s="36">
+        <f>DATE(YEAR(E35)+1,MONTH(E35),DAY(E35))</f>
         <v>45078</v>
       </c>
-      <c r="H35" s="16" t="s">
-        <v>179</v>
+      <c r="H35" s="35" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>23</v>
+        <v>192</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="C36" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>106</v>
+        <v>283</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>235</v>
       </c>
       <c r="E36" s="18">
-        <v>44986</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="G36" s="18">
-        <f t="shared" si="0"/>
+        <v>44713</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G36" s="36">
+        <f>DATE(YEAR(E36)+1,MONTH(E36),DAY(E36))</f>
         <v>45078</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="35" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>17</v>
+        <v>225</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>213</v>
+        <v>277</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>228</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="E37" s="18">
-        <v>44986</v>
+        <v>100</v>
+      </c>
+      <c r="E37" s="1">
+        <v>44987</v>
       </c>
       <c r="F37" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G37" s="18">
-        <f t="shared" si="0"/>
-        <v>45078</v>
-      </c>
-      <c r="H37" s="16" t="s">
+        <f>DATE(YEAR(E37),MONTH(E37)+3,DAY(E37))</f>
+        <v>45079</v>
+      </c>
+      <c r="H37" s="35" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>264</v>
+      <c r="A38" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>278</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="18">
-        <v>44986</v>
-      </c>
-      <c r="F38" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="1">
+        <v>44988</v>
+      </c>
+      <c r="F38" s="37" t="s">
         <v>123</v>
       </c>
       <c r="G38" s="18">
-        <f t="shared" si="0"/>
-        <v>45078</v>
-      </c>
-      <c r="H38" s="16" t="s">
+        <f>DATE(YEAR(E38),MONTH(E38)+3,DAY(E38))</f>
+        <v>45080</v>
+      </c>
+      <c r="H38" s="35" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="C39" s="31" t="s">
-        <v>240</v>
+        <v>279</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>215</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="E39" s="18">
-        <v>44986</v>
+        <v>100</v>
+      </c>
+      <c r="E39" s="1">
+        <v>44989</v>
       </c>
       <c r="F39" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G39" s="18">
-        <f t="shared" si="0"/>
-        <v>45078</v>
+        <f>DATE(YEAR(E39),MONTH(E39)+3,DAY(E39))</f>
+        <v>45081</v>
       </c>
       <c r="H39" s="16" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>62</v>
+      <c r="A40" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>56</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="D40" s="17"/>
-      <c r="E40" s="18">
-        <v>44713</v>
-      </c>
-      <c r="F40" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="G40" s="18">
-        <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
-        <v>45078</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>184</v>
+      <c r="E40" s="36">
+        <v>45017</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="36">
+        <f>DATE(YEAR(E40),MONTH(E40)+3,DAY(E40))</f>
+        <v>45108</v>
+      </c>
+      <c r="H40" s="35" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>140</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="D41" s="17"/>
       <c r="E41" s="18">
-        <v>44713</v>
+        <v>45017</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="G41" s="18">
-        <f>DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
-        <v>45078</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>180</v>
+        <v>123</v>
+      </c>
+      <c r="G41" s="36">
+        <f>DATE(YEAR(E41),MONTH(E41)+3,DAY(E41))</f>
+        <v>45108</v>
+      </c>
+      <c r="H41" s="35" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="31" t="s">
-        <v>238</v>
+        <v>284</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>198</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>237</v>
+        <v>101</v>
       </c>
       <c r="E42" s="18">
-        <v>44713</v>
+        <v>44743</v>
       </c>
       <c r="F42" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G42" s="18">
         <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
-        <v>45078</v>
-      </c>
-      <c r="H42" s="16" t="s">
-        <v>182</v>
+        <v>45108</v>
+      </c>
+      <c r="H42" s="35" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>71</v>
+        <v>285</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="E43" s="22">
-        <v>44713</v>
+        <v>44743</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>124</v>
       </c>
       <c r="G43" s="22">
         <f>DATE(YEAR(E43)+1,MONTH(E43),DAY(E43))</f>
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
-        <v>192</v>
+        <v>8</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>236</v>
-      </c>
-      <c r="D44" s="33" t="s">
-        <v>235</v>
+        <v>286</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="E44" s="18">
-        <v>44713</v>
-      </c>
-      <c r="F44" s="16" t="s">
+        <v>44743</v>
+      </c>
+      <c r="F44" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G44" s="22">
         <f>DATE(YEAR(E44)+1,MONTH(E44),DAY(E44))</f>
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="H44" s="21" t="s">
         <v>179</v>
@@ -2765,26 +2768,26 @@
     </row>
     <row r="45" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>225</v>
+        <v>9</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E45" s="1">
-        <v>44987</v>
+        <v>101</v>
+      </c>
+      <c r="E45" s="18">
+        <v>44743</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G45" s="18">
-        <f>DATE(YEAR(E45),MONTH(E45)+3,DAY(E45))</f>
-        <v>45079</v>
+        <f>DATE(YEAR(E45)+1,MONTH(E45),DAY(E45))</f>
+        <v>45108</v>
       </c>
       <c r="H45" s="21" t="s">
         <v>179</v>
@@ -2792,26 +2795,26 @@
     </row>
     <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E46" s="1">
-        <v>44988</v>
+        <v>101</v>
+      </c>
+      <c r="E46" s="18">
+        <v>44743</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G46" s="18">
-        <f>DATE(YEAR(E46),MONTH(E46)+3,DAY(E46))</f>
-        <v>45080</v>
+        <f>DATE(YEAR(E46)+1,MONTH(E46),DAY(E46))</f>
+        <v>45108</v>
       </c>
       <c r="H46" s="21" t="s">
         <v>179</v>
@@ -2819,53 +2822,53 @@
     </row>
     <row r="47" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47" s="1">
-        <v>44989</v>
+        <v>162</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="E47" s="18">
+        <v>44958</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>123</v>
+        <v>222</v>
       </c>
       <c r="G47" s="18">
-        <f>DATE(YEAR(E47),MONTH(E47)+3,DAY(E47))</f>
-        <v>45081</v>
+        <f>DATE(YEAR(E47),MONTH(E47)+6,DAY(E47))</f>
+        <v>45139</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>198</v>
+        <v>263</v>
+      </c>
+      <c r="C48" s="31" t="s">
+        <v>213</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E48" s="18">
-        <v>44743</v>
+        <v>45078</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G48" s="18">
-        <f>DATE(YEAR(E48)+1,MONTH(E48),DAY(E48))</f>
-        <v>45108</v>
+        <f>DATE(YEAR(E48),MONTH(E48)+3,DAY(E48))</f>
+        <v>45170</v>
       </c>
       <c r="H48" s="16" t="s">
         <v>179</v>
@@ -2873,26 +2876,26 @@
     </row>
     <row r="49" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>193</v>
+        <v>239</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>194</v>
+        <v>107</v>
       </c>
       <c r="E49" s="18">
-        <v>44743</v>
+        <v>45078</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G49" s="18">
-        <f>DATE(YEAR(E49)+1,MONTH(E49),DAY(E49))</f>
-        <v>45108</v>
+        <f>DATE(YEAR(E49),MONTH(E49)+3,DAY(E49))</f>
+        <v>45170</v>
       </c>
       <c r="H49" s="16" t="s">
         <v>179</v>
@@ -2900,26 +2903,26 @@
     </row>
     <row r="50" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>199</v>
+        <v>265</v>
+      </c>
+      <c r="C50" s="31" t="s">
+        <v>240</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E50" s="18">
-        <v>44743</v>
+        <v>45078</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G50" s="18">
-        <f>DATE(YEAR(E50)+1,MONTH(E50),DAY(E50))</f>
-        <v>45108</v>
+        <f>DATE(YEAR(E50),MONTH(E50)+3,DAY(E50))</f>
+        <v>45170</v>
       </c>
       <c r="H50" s="16" t="s">
         <v>179</v>
@@ -2927,26 +2930,26 @@
     </row>
     <row r="51" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>101</v>
+        <v>251</v>
       </c>
       <c r="E51" s="18">
-        <v>44743</v>
+        <v>44805</v>
       </c>
       <c r="F51" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G51" s="18">
         <f>DATE(YEAR(E51)+1,MONTH(E51),DAY(E51))</f>
-        <v>45108</v>
+        <v>45170</v>
       </c>
       <c r="H51" s="16" t="s">
         <v>179</v>
@@ -2954,26 +2957,26 @@
     </row>
     <row r="52" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="E52" s="18">
-        <v>44743</v>
+        <v>44805</v>
       </c>
       <c r="F52" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G52" s="18">
         <f>DATE(YEAR(E52)+1,MONTH(E52),DAY(E52))</f>
-        <v>45108</v>
+        <v>45170</v>
       </c>
       <c r="H52" s="16" t="s">
         <v>179</v>
@@ -2981,52 +2984,52 @@
     </row>
     <row r="53" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>161</v>
+        <v>18</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C53" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>163</v>
+        <v>291</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>241</v>
       </c>
       <c r="E53" s="18">
-        <v>44958</v>
+        <v>44805</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>222</v>
+        <v>124</v>
       </c>
       <c r="G53" s="18">
-        <f>DATE(YEAR(E53),MONTH(E53)+6,DAY(E53))</f>
-        <v>45139</v>
+        <f>DATE(YEAR(E53)+1,MONTH(E53),DAY(E53))</f>
+        <v>45170</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>6</v>
+        <v>160</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>251</v>
+        <v>292</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="E54" s="18">
         <v>44805</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G54" s="18">
-        <f t="shared" ref="G54:G65" si="1">DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
+        <f>DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
         <v>45170</v>
       </c>
       <c r="H54" s="16" t="s">
@@ -3034,26 +3037,26 @@
       </c>
     </row>
     <row r="55" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>290</v>
+      <c r="A55" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>293</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>201</v>
+        <v>246</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E55" s="18">
+        <v>111</v>
+      </c>
+      <c r="E55" s="36">
         <v>44805</v>
       </c>
-      <c r="F55" s="19" t="s">
+      <c r="F55" s="37" t="s">
         <v>124</v>
       </c>
       <c r="G55" s="18">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
         <v>45170</v>
       </c>
       <c r="H55" s="16" t="s">
@@ -3062,53 +3065,53 @@
     </row>
     <row r="56" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>291</v>
+        <v>65</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>241</v>
+        <v>126</v>
       </c>
       <c r="E56" s="18">
-        <v>44805</v>
+        <v>44866</v>
       </c>
       <c r="F56" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G56" s="18">
-        <f t="shared" si="1"/>
-        <v>45170</v>
+        <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
+        <v>45231</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="C57" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="D57" s="23" t="s">
-        <v>159</v>
+        <v>294</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>114</v>
       </c>
       <c r="E57" s="18">
-        <v>44805</v>
-      </c>
-      <c r="F57" s="16" t="s">
+        <v>44866</v>
+      </c>
+      <c r="F57" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G57" s="18">
-        <f t="shared" si="1"/>
-        <v>45170</v>
+        <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
+        <v>45231</v>
       </c>
       <c r="H57" s="16" t="s">
         <v>179</v>
@@ -3116,26 +3119,26 @@
     </row>
     <row r="58" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E58" s="22">
-        <v>44805</v>
+        <v>44896</v>
       </c>
       <c r="F58" s="27" t="s">
         <v>124</v>
       </c>
       <c r="G58" s="18">
-        <f t="shared" si="1"/>
-        <v>45170</v>
+        <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
+        <v>45261</v>
       </c>
       <c r="H58" s="16" t="s">
         <v>179</v>
@@ -3143,53 +3146,53 @@
     </row>
     <row r="59" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>64</v>
+        <v>158</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>126</v>
+        <v>267</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="E59" s="18">
-        <v>44866</v>
-      </c>
-      <c r="F59" s="19" t="s">
+        <v>44896</v>
+      </c>
+      <c r="F59" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G59" s="18">
-        <f t="shared" si="1"/>
-        <v>45231</v>
+        <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
+        <v>45261</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>206</v>
+        <v>262</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="E60" s="18">
-        <v>44866</v>
+        <v>44896</v>
       </c>
       <c r="F60" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G60" s="18">
-        <f t="shared" si="1"/>
-        <v>45231</v>
+        <f>DATE(YEAR(E60)+1,MONTH(E60),DAY(E60))</f>
+        <v>45261</v>
       </c>
       <c r="H60" s="16" t="s">
         <v>179</v>
@@ -3197,25 +3200,25 @@
     </row>
     <row r="61" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>158</v>
+        <v>29</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="C61" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="D61" s="23" t="s">
-        <v>159</v>
+        <v>296</v>
+      </c>
+      <c r="C61" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="E61" s="18">
         <v>44896</v>
       </c>
-      <c r="F61" s="16" t="s">
+      <c r="F61" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G61" s="18">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E61)+1,MONTH(E61),DAY(E61))</f>
         <v>45261</v>
       </c>
       <c r="H61" s="16" t="s">
@@ -3224,16 +3227,16 @@
     </row>
     <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="E62" s="18">
         <v>44896</v>
@@ -3242,7 +3245,7 @@
         <v>124</v>
       </c>
       <c r="G62" s="18">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E62)+1,MONTH(E62),DAY(E62))</f>
         <v>45261</v>
       </c>
       <c r="H62" s="16" t="s">
@@ -3251,69 +3254,69 @@
     </row>
     <row r="63" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>296</v>
+        <v>78</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>254</v>
+        <v>301</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>110</v>
+        <v>260</v>
       </c>
       <c r="E63" s="18">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="F63" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G63" s="18">
-        <f t="shared" si="1"/>
-        <v>45261</v>
+        <f>DATE(YEAR(E63)+1,MONTH(E63),DAY(E63))</f>
+        <v>45292</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>212</v>
+        <v>41</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="E64" s="18">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="F64" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G64" s="18">
-        <f t="shared" si="1"/>
-        <v>45261</v>
+        <f>DATE(YEAR(E64),MONTH(E64)+12,DAY(E64))</f>
+        <v>45292</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C65" s="31" t="s">
-        <v>301</v>
-      </c>
-      <c r="D65" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D65" s="23" t="s">
         <v>260</v>
       </c>
       <c r="E65" s="18">
@@ -3323,7 +3326,7 @@
         <v>124</v>
       </c>
       <c r="G65" s="18">
-        <f t="shared" si="1"/>
+        <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
         <v>45292</v>
       </c>
       <c r="H65" s="16" t="s">
@@ -3332,26 +3335,26 @@
     </row>
     <row r="66" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C66" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="C66" s="31" t="s">
+        <v>304</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>253</v>
       </c>
       <c r="E66" s="18">
-        <v>44927</v>
+        <v>44986</v>
       </c>
       <c r="F66" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G66" s="18">
-        <f>DATE(YEAR(E66),MONTH(E66)+12,DAY(E66))</f>
-        <v>45292</v>
+        <f>DATE(YEAR(E66)+1,MONTH(E66),DAY(E66))</f>
+        <v>45352</v>
       </c>
       <c r="H66" s="16" t="s">
         <v>180</v>
@@ -3359,26 +3362,26 @@
     </row>
     <row r="67" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="D67" s="23" t="s">
-        <v>260</v>
+        <v>97</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="E67" s="18">
-        <v>44927</v>
+        <v>45017</v>
       </c>
       <c r="F67" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G67" s="18">
         <f>DATE(YEAR(E67)+1,MONTH(E67),DAY(E67))</f>
-        <v>45292</v>
+        <v>45383</v>
       </c>
       <c r="H67" s="16" t="s">
         <v>182</v>
@@ -3386,29 +3389,29 @@
     </row>
     <row r="68" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>79</v>
+        <v>46</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>204</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="E68" s="18">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="F68" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G68" s="18">
         <f>DATE(YEAR(E68)+1,MONTH(E68),DAY(E68))</f>
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3791,107 +3794,107 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D66" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C27" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C40" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D64" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C40" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C32" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="C71" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
     <hyperlink ref="C81" r:id="rId7" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="D74" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C68" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D46" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D47" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D48" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="D37" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D49" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D38" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D63" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D58" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D55" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="D64" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D60" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D33" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D32" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C67" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D38" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D39" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="D42" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="D48" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D43" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D58" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="D49" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D50" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D61" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D55" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="D62" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="D57" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="D28" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
     <hyperlink ref="D4" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
     <hyperlink ref="D5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
     <hyperlink ref="D82" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
     <hyperlink ref="D71" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D18" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D35" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="D59" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D17" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D60" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D30" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D56" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
     <hyperlink ref="D78" r:id="rId33" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
     <hyperlink ref="D70" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
     <hyperlink ref="C70" r:id="rId35" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="D51" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D52" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C47" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D17" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="D45" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D46" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D16" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
     <hyperlink ref="D7" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
     <hyperlink ref="D8" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C66" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="D12" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D41" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D68" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D26" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="C64" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D11" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="D33" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D67" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D24" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
     <hyperlink ref="C80" r:id="rId47" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
     <hyperlink ref="C84" r:id="rId48" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
-    <hyperlink ref="D14" r:id="rId49" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
+    <hyperlink ref="D13" r:id="rId49" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
     <hyperlink ref="C9" r:id="rId50" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
     <hyperlink ref="D75" r:id="rId51" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
     <hyperlink ref="C75" r:id="rId52" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
     <hyperlink ref="D73" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
     <hyperlink ref="C73" r:id="rId54" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
     <hyperlink ref="C78" r:id="rId55" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
-    <hyperlink ref="D61" r:id="rId56" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
-    <hyperlink ref="D57" r:id="rId57" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
-    <hyperlink ref="D53" r:id="rId58" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
+    <hyperlink ref="D59" r:id="rId56" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
+    <hyperlink ref="D54" r:id="rId57" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
+    <hyperlink ref="D47" r:id="rId58" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
     <hyperlink ref="C79" r:id="rId59" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
-    <hyperlink ref="C48" r:id="rId60" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
-    <hyperlink ref="D36" r:id="rId61" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
-    <hyperlink ref="D19" r:id="rId62" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
-    <hyperlink ref="C26" r:id="rId63" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="D13" r:id="rId64" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C55" r:id="rId65" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D16" r:id="rId66" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="C42" r:id="rId60" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
+    <hyperlink ref="D31" r:id="rId61" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
+    <hyperlink ref="D18" r:id="rId62" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
+    <hyperlink ref="C24" r:id="rId63" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
+    <hyperlink ref="D12" r:id="rId64" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C52" r:id="rId65" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
+    <hyperlink ref="D15" r:id="rId66" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
     <hyperlink ref="C83" r:id="rId67" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
-    <hyperlink ref="D11" r:id="rId68" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C46" r:id="rId69" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
-    <hyperlink ref="D29" r:id="rId70" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
+    <hyperlink ref="D10" r:id="rId68" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
+    <hyperlink ref="C38" r:id="rId69" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="D68" r:id="rId70" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
     <hyperlink ref="C2" r:id="rId71" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D20" r:id="rId72" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="D19" r:id="rId72" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
     <hyperlink ref="D79" r:id="rId73" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
-    <hyperlink ref="C24" r:id="rId74" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/04/scottish-natural-capital-accounts-2022/documents/scottish-natural-capital-accounts-2022-reference-tables/scottish-natural-capital-accounts-2022-reference-tables/govscot%3Adocument/scottish-natural-capital-accounts-2022-reference-tables.xlsx" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
+    <hyperlink ref="C22" r:id="rId74" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2022/04/scottish-natural-capital-accounts-2022/documents/scottish-natural-capital-accounts-2022-reference-tables/scottish-natural-capital-accounts-2022-reference-tables/govscot%3Adocument/scottish-natural-capital-accounts-2022-reference-tables.xlsx" xr:uid="{B41F83ED-1C07-4EE9-8443-D5574B6AAE3B}"/>
     <hyperlink ref="D81" r:id="rId75" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
     <hyperlink ref="D83" r:id="rId76" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
-    <hyperlink ref="C10" r:id="rId77" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D31" r:id="rId78" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D45" r:id="rId79" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C31" r:id="rId80" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C35" r:id="rId81" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C30" r:id="rId82" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C17" r:id="rId83" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C58" r:id="rId77" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
+    <hyperlink ref="D26" r:id="rId78" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D37" r:id="rId79" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C26" r:id="rId80" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C30" r:id="rId81" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C25" r:id="rId82" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C16" r:id="rId83" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
     <hyperlink ref="C5" r:id="rId84" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="C14" r:id="rId85" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
-    <hyperlink ref="D21" r:id="rId86" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
+    <hyperlink ref="C13" r:id="rId85" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
+    <hyperlink ref="D20" r:id="rId86" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
     <hyperlink ref="C6" r:id="rId87" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
-    <hyperlink ref="D34" r:id="rId88" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
-    <hyperlink ref="C36" r:id="rId89" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
-    <hyperlink ref="C33" r:id="rId90" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
-    <hyperlink ref="C37" r:id="rId91" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
-    <hyperlink ref="D44" r:id="rId92" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
-    <hyperlink ref="C44" r:id="rId93" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
-    <hyperlink ref="C42" r:id="rId94" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
-    <hyperlink ref="C13" r:id="rId95" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
-    <hyperlink ref="C16" r:id="rId96" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
-    <hyperlink ref="C63" r:id="rId97" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
-    <hyperlink ref="C20" r:id="rId98" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
-    <hyperlink ref="C61" r:id="rId99" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
-    <hyperlink ref="C65" r:id="rId100" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
-    <hyperlink ref="D24" r:id="rId101" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
+    <hyperlink ref="D29" r:id="rId88" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
+    <hyperlink ref="C31" r:id="rId89" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
+    <hyperlink ref="C28" r:id="rId90" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
+    <hyperlink ref="C48" r:id="rId91" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
+    <hyperlink ref="D36" r:id="rId92" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
+    <hyperlink ref="C36" r:id="rId93" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
+    <hyperlink ref="C34" r:id="rId94" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
+    <hyperlink ref="C12" r:id="rId95" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
+    <hyperlink ref="C15" r:id="rId96" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
+    <hyperlink ref="C61" r:id="rId97" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
+    <hyperlink ref="C19" r:id="rId98" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
+    <hyperlink ref="C59" r:id="rId99" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
+    <hyperlink ref="C63" r:id="rId100" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
+    <hyperlink ref="D22" r:id="rId101" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId102"/>

</xml_diff>

<commit_message>
September quarterly (generation, capacity, pipeline, consumption)
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1239F907-21E9-4EF1-A9A2-79AC2BE03FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15ADAD87-7AFD-44FE-BC73-A6CCF7F9A464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -748,9 +748,6 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1107328/Renewable_electricity_by_local_authority_2014_-_2021.xlsx</t>
   </si>
   <si>
-    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1106843/subnational_total_final_energy_consumption_2020.xlsx</t>
-  </si>
-  <si>
     <t>https://www.gov.uk/government/statistics/electric-vehicle-charging-device-statistics-july-2022</t>
   </si>
   <si>
@@ -935,6 +932,9 @@
   </si>
   <si>
     <t>https://www.electralink.co.uk/2023/08/smart-installs-pass-21-million/</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1187087/Subnational_total_final_consumption_2005_2021.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1100,21 +1100,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1595,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1751,7 @@
         <v>233</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E6" s="8">
         <v>44743</v>
@@ -1777,7 +1775,7 @@
         <v>95</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>136</v>
@@ -1796,180 +1794,178 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41">
+      <c r="D8" s="36"/>
+      <c r="E8" s="37">
         <v>44652</v>
       </c>
-      <c r="F8" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="G8" s="41">
+      <c r="F8" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="37">
         <f>DATE(YEAR(E8)+1,MONTH(E8),DAY(E8))</f>
         <v>45017</v>
       </c>
-      <c r="H8" s="39" t="s">
+      <c r="H8" s="35" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+    <row r="9" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>277</v>
-      </c>
-      <c r="C9" s="43" t="s">
+      <c r="B9" s="35" t="s">
+        <v>276</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="37">
         <v>44743</v>
       </c>
-      <c r="F9" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="G9" s="41">
+      <c r="F9" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="37">
         <f>DATE(YEAR(E9)+1,MONTH(E9),DAY(E9))</f>
         <v>45108</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="35" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+    <row r="10" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="45" t="s">
-        <v>278</v>
-      </c>
-      <c r="C10" s="44" t="s">
+      <c r="B10" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="37">
         <v>44743</v>
       </c>
-      <c r="F10" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="G10" s="41">
+      <c r="F10" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="37">
         <f>DATE(YEAR(E10)+1,MONTH(E10),DAY(E10))</f>
         <v>45108</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="35" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="39" t="s">
-        <v>279</v>
-      </c>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="C11" s="40" t="s">
         <v>198</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="37">
         <v>44743</v>
       </c>
-      <c r="F11" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" s="41">
+      <c r="F11" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="37">
         <f>DATE(YEAR(E11)+1,MONTH(E11),DAY(E11))</f>
         <v>45108</v>
       </c>
-      <c r="H11" s="39" t="s">
+      <c r="H11" s="35" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+    <row r="12" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="C12" s="44" t="s">
+      <c r="B12" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="C12" s="40" t="s">
         <v>199</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="37">
         <v>44743</v>
       </c>
-      <c r="F12" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="G12" s="41">
+      <c r="F12" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="37">
         <f>DATE(YEAR(E12)+1,MONTH(E12),DAY(E12))</f>
         <v>45108</v>
       </c>
-      <c r="H12" s="39" t="s">
+      <c r="H12" s="35" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+    <row r="13" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="C13" s="44" t="s">
+      <c r="B13" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" s="40" t="s">
         <v>195</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="37">
         <v>44743</v>
       </c>
-      <c r="F13" s="42" t="s">
-        <v>124</v>
-      </c>
-      <c r="G13" s="41">
+      <c r="F13" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" s="37">
         <f>DATE(YEAR(E13)+1,MONTH(E13),DAY(E13))</f>
         <v>45108</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="35" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>259</v>
+        <v>53</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="1">
+        <v>54</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18">
         <v>45078</v>
       </c>
       <c r="F14" s="19" t="s">
@@ -1980,26 +1976,24 @@
         <v>45170</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="1">
+        <v>150</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18">
         <v>45078</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="16" t="s">
         <v>123</v>
       </c>
       <c r="G15" s="18">
@@ -2007,30 +2001,30 @@
         <v>45170</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>106</v>
+        <v>245</v>
       </c>
       <c r="E16" s="18">
-        <v>45078</v>
+        <v>44805</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G16" s="18">
-        <f>DATE(YEAR(E16),MONTH(E16)+3,DAY(E16))</f>
+        <f>DATE(YEAR(E16)+1,MONTH(E16),DAY(E16))</f>
         <v>45170</v>
       </c>
       <c r="H16" s="16" t="s">
@@ -2039,26 +2033,26 @@
     </row>
     <row r="17" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>225</v>
+        <v>16</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="1">
-        <v>45078</v>
+        <v>204</v>
+      </c>
+      <c r="E17" s="18">
+        <v>45170</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G17" s="18">
-        <f>DATE(YEAR(E17),MONTH(E17)+3,DAY(E17))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E17),MONTH(E17)+1,DAY(E17))</f>
+        <v>45200</v>
       </c>
       <c r="H17" s="16" t="s">
         <v>179</v>
@@ -2066,184 +2060,184 @@
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="B18" t="s">
-        <v>268</v>
+        <v>38</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>231</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>106</v>
+        <v>303</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="E18" s="18">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G18" s="18">
-        <f>DATE(YEAR(E18),MONTH(E18)+3,DAY(E18))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E18),MONTH(E18)+1,DAY(E18))</f>
+        <v>45200</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="B19" s="46" t="s">
-        <v>275</v>
+      <c r="A19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" s="37">
-        <v>45078</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="G19" s="37">
-        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
-        <v>45170</v>
-      </c>
-      <c r="H19" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="18">
+        <v>45200</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="18">
+        <f>DATE(YEAR(E19),MONTH(E19)+1,DAY(E19))</f>
+        <v>45231</v>
+      </c>
+      <c r="H19" s="16" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>268</v>
+        <v>85</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>106</v>
+        <v>240</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>232</v>
       </c>
       <c r="E20" s="18">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="18">
         <f>DATE(YEAR(E20),MONTH(E20)+3,DAY(E20))</f>
-        <v>45170</v>
-      </c>
-      <c r="H20" s="36" t="s">
-        <v>179</v>
+        <v>45200</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="D21" s="17"/>
       <c r="E21" s="18">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="F21" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G21" s="18">
         <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
-        <v>45170</v>
-      </c>
-      <c r="H21" s="36" t="s">
+        <v>45200</v>
+      </c>
+      <c r="H21" s="16" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>151</v>
+      <c r="A22" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>294</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="18">
-        <v>45078</v>
-      </c>
-      <c r="F22" s="36" t="s">
+        <v>45108</v>
+      </c>
+      <c r="F22" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G22" s="18">
         <f>DATE(YEAR(E22),MONTH(E22)+3,DAY(E22))</f>
-        <v>45170</v>
-      </c>
-      <c r="H22" s="36" t="s">
-        <v>184</v>
+        <v>45200</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>212</v>
+        <v>65</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>251</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="E23" s="18">
-        <v>45078</v>
+        <v>44866</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G23" s="18">
-        <f>DATE(YEAR(E23),MONTH(E23)+3,DAY(E23))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E23)+1,MONTH(E23),DAY(E23))</f>
+        <v>45231</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="E24" s="18">
-        <v>45078</v>
+        <v>44866</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G24" s="18">
-        <f>DATE(YEAR(E24),MONTH(E24)+3,DAY(E24))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E24)+1,MONTH(E24),DAY(E24))</f>
+        <v>45231</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>179</v>
@@ -2251,26 +2245,26 @@
     </row>
     <row r="25" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>239</v>
+        <v>269</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="18">
-        <v>45078</v>
+        <v>100</v>
+      </c>
+      <c r="E25" s="1">
+        <v>45170</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G25" s="18">
         <f>DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>179</v>
@@ -2278,26 +2272,26 @@
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="E26" s="18">
-        <v>44805</v>
+        <v>100</v>
+      </c>
+      <c r="E26" s="1">
+        <v>45170</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G26" s="18">
-        <f>DATE(YEAR(E26)+1,MONTH(E26),DAY(E26))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E26),MONTH(E26)+3,DAY(E26))</f>
+        <v>45261</v>
       </c>
       <c r="H26" s="16" t="s">
         <v>179</v>
@@ -2305,26 +2299,26 @@
     </row>
     <row r="27" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="18">
-        <v>44805</v>
+        <v>100</v>
+      </c>
+      <c r="E27" s="1">
+        <v>45170</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G27" s="18">
-        <f>DATE(YEAR(E27)+1,MONTH(E27),DAY(E27))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E27),MONTH(E27)+3,DAY(E27))</f>
+        <v>45261</v>
       </c>
       <c r="H27" s="16" t="s">
         <v>179</v>
@@ -2332,26 +2326,26 @@
     </row>
     <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>159</v>
+        <v>255</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>103</v>
       </c>
       <c r="E28" s="18">
-        <v>44805</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>124</v>
+        <v>45170</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="G28" s="18">
-        <f>DATE(YEAR(E28)+1,MONTH(E28),DAY(E28))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E28),MONTH(E28)+3,DAY(E28))</f>
+        <v>45261</v>
       </c>
       <c r="H28" s="16" t="s">
         <v>179</v>
@@ -2359,26 +2353,26 @@
     </row>
     <row r="29" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E29" s="18">
-        <v>44805</v>
+        <v>45170</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G29" s="18">
-        <f>DATE(YEAR(E29)+1,MONTH(E29),DAY(E29))</f>
-        <v>45170</v>
+        <f>DATE(YEAR(E29),MONTH(E29)+3,DAY(E29))</f>
+        <v>45261</v>
       </c>
       <c r="H29" s="16" t="s">
         <v>179</v>
@@ -2386,26 +2380,26 @@
     </row>
     <row r="30" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
-        <v>224</v>
+        <v>25</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="1">
-        <v>45078</v>
+        <v>106</v>
+      </c>
+      <c r="E30" s="18">
+        <v>45170</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G30" s="18">
         <f>DATE(YEAR(E30),MONTH(E30)+3,DAY(E30))</f>
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>179</v>
@@ -2413,26 +2407,26 @@
     </row>
     <row r="31" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>213</v>
+        <v>258</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>220</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>100</v>
       </c>
       <c r="E31" s="1">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="F31" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G31" s="18">
         <f>DATE(YEAR(E31),MONTH(E31)+3,DAY(E31))</f>
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>179</v>
@@ -2440,26 +2434,26 @@
     </row>
     <row r="32" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>214</v>
+        <v>260</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>219</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>100</v>
       </c>
       <c r="E32" s="1">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G32" s="18">
         <f>DATE(YEAR(E32),MONTH(E32)+3,DAY(E32))</f>
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>179</v>
@@ -2467,26 +2461,26 @@
     </row>
     <row r="33" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="E33" s="18">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G33" s="18">
         <f>DATE(YEAR(E33),MONTH(E33)+3,DAY(E33))</f>
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>179</v>
@@ -2494,26 +2488,26 @@
     </row>
     <row r="34" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>25</v>
+        <v>225</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="18">
-        <v>45078</v>
+        <v>100</v>
+      </c>
+      <c r="E34" s="1">
+        <v>45170</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G34" s="18">
         <f>DATE(YEAR(E34),MONTH(E34)+3,DAY(E34))</f>
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H34" s="16" t="s">
         <v>179</v>
@@ -2521,26 +2515,26 @@
     </row>
     <row r="35" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>204</v>
+        <v>230</v>
+      </c>
+      <c r="B35" t="s">
+        <v>267</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>106</v>
       </c>
       <c r="E35" s="18">
         <v>45170</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G35" s="18">
-        <f>DATE(YEAR(E35),MONTH(E35)+1,DAY(E35))</f>
-        <v>45200</v>
+        <f>DATE(YEAR(E35),MONTH(E35)+3,DAY(E35))</f>
+        <v>45261</v>
       </c>
       <c r="H35" s="16" t="s">
         <v>179</v>
@@ -2548,53 +2542,53 @@
     </row>
     <row r="36" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>39</v>
+        <v>229</v>
+      </c>
+      <c r="B36" t="s">
+        <v>274</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>304</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>137</v>
+        <v>228</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>106</v>
       </c>
       <c r="E36" s="18">
         <v>45170</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G36" s="18">
-        <f>DATE(YEAR(E36),MONTH(E36)+1,DAY(E36))</f>
-        <v>45200</v>
+        <f>DATE(YEAR(E36),MONTH(E36)+3,DAY(E36))</f>
+        <v>45261</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B37" s="16" t="s">
         <v>267</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>105</v>
+        <v>201</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="E37" s="18">
         <v>45170</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G37" s="18">
-        <f>DATE(YEAR(E37),MONTH(E37)+1,DAY(E37))</f>
-        <v>45200</v>
+        <f>DATE(YEAR(E37),MONTH(E37)+3,DAY(E37))</f>
+        <v>45261</v>
       </c>
       <c r="H37" s="16" t="s">
         <v>179</v>
@@ -2602,147 +2596,151 @@
     </row>
     <row r="38" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="D38" s="33" t="s">
-        <v>232</v>
+        <v>256</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>107</v>
       </c>
       <c r="E38" s="18">
-        <v>45108</v>
+        <v>45170</v>
       </c>
       <c r="F38" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G38" s="18">
         <f>DATE(YEAR(E38),MONTH(E38)+3,DAY(E38))</f>
-        <v>45200</v>
+        <v>45261</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D39" s="17"/>
+        <v>257</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="E39" s="18">
-        <v>45108</v>
+        <v>45170</v>
       </c>
       <c r="F39" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G39" s="18">
         <f>DATE(YEAR(E39),MONTH(E39)+3,DAY(E39))</f>
-        <v>45200</v>
+        <v>45261</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>295</v>
-      </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="18">
-        <v>45108</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="G40" s="18">
-        <f>DATE(YEAR(E40),MONTH(E40)+3,DAY(E40))</f>
-        <v>45200</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>183</v>
+      <c r="A40" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="43">
+        <v>44896</v>
+      </c>
+      <c r="F40" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="43">
+        <f>DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
+        <v>45261</v>
+      </c>
+      <c r="H40" s="41" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="36" t="s">
-        <v>65</v>
+      <c r="A41" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>261</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>252</v>
+        <v>215</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" s="37">
-        <v>44866</v>
-      </c>
-      <c r="F41" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="G41" s="37">
+        <v>104</v>
+      </c>
+      <c r="E41" s="43">
+        <v>44896</v>
+      </c>
+      <c r="F41" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="G41" s="43">
         <f>DATE(YEAR(E41)+1,MONTH(E41),DAY(E41))</f>
-        <v>45231</v>
-      </c>
-      <c r="H41" s="36" t="s">
-        <v>180</v>
+        <v>45261</v>
+      </c>
+      <c r="H41" s="41" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>114</v>
+        <v>259</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="E42" s="18">
-        <v>44866</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="G42" s="37">
+        <v>44896</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="43">
         <f>DATE(YEAR(E42)+1,MONTH(E42),DAY(E42))</f>
-        <v>45231</v>
-      </c>
-      <c r="H42" s="36" t="s">
+        <v>45261</v>
+      </c>
+      <c r="H42" s="41" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="E43" s="22">
         <v>44896</v>
@@ -2759,22 +2757,22 @@
       </c>
     </row>
     <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>215</v>
+      <c r="A44" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="C44" s="31" t="s">
+        <v>248</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E44" s="18">
         <v>44896</v>
       </c>
-      <c r="F44" s="38" t="s">
+      <c r="F44" s="44" t="s">
         <v>124</v>
       </c>
       <c r="G44" s="22">
@@ -2787,21 +2785,21 @@
     </row>
     <row r="45" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>260</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>159</v>
+        <v>289</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>113</v>
       </c>
       <c r="E45" s="18">
         <v>44896</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G45" s="18">
@@ -2814,97 +2812,97 @@
     </row>
     <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>255</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>102</v>
+        <v>48</v>
+      </c>
+      <c r="C46" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>139</v>
       </c>
       <c r="E46" s="18">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="F46" s="27" t="s">
         <v>124</v>
       </c>
       <c r="G46" s="18">
         <f>DATE(YEAR(E46)+1,MONTH(E46),DAY(E46))</f>
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>289</v>
+        <v>78</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>249</v>
+        <v>293</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>110</v>
+        <v>252</v>
       </c>
       <c r="E47" s="18">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="F47" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G47" s="18">
         <f>DATE(YEAR(E47)+1,MONTH(E47),DAY(E47))</f>
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>211</v>
+        <v>41</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="E48" s="18">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="F48" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G48" s="18">
-        <f>DATE(YEAR(E48)+1,MONTH(E48),DAY(E48))</f>
-        <v>45261</v>
+        <f>DATE(YEAR(E48),MONTH(E48)+12,DAY(E48))</f>
+        <v>45292</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>139</v>
+        <v>81</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>252</v>
       </c>
       <c r="E49" s="18">
         <v>44927</v>
@@ -2917,111 +2915,111 @@
         <v>45292</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>78</v>
+        <v>263</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>294</v>
+        <v>250</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>253</v>
+        <v>109</v>
       </c>
       <c r="E50" s="18">
-        <v>44927</v>
+        <v>45200</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G50" s="18">
-        <f>DATE(YEAR(E50)+1,MONTH(E50),DAY(E50))</f>
-        <v>45292</v>
+        <f>DATE(YEAR(E50),MONTH(E50)+4,DAY(E50))</f>
+        <v>45323</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>40</v>
+        <v>169</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>42</v>
+        <v>170</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="E51" s="18">
-        <v>44927</v>
+        <v>45200</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G51" s="18">
-        <f>DATE(YEAR(E51),MONTH(E51)+12,DAY(E51))</f>
-        <v>45292</v>
+        <f>DATE(YEAR(E51),MONTH(E51)+4,DAY(E51))</f>
+        <v>45323</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>254</v>
+        <v>162</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>243</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>253</v>
+        <v>163</v>
       </c>
       <c r="E52" s="18">
-        <v>44927</v>
+        <v>45139</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
       <c r="G52" s="18">
-        <f>DATE(YEAR(E52)+1,MONTH(E52),DAY(E52))</f>
-        <v>45292</v>
+        <f>DATE(YEAR(E52),MONTH(E52)+6,DAY(E52))</f>
+        <v>45323</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="B53" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="C53" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>109</v>
+      <c r="C53" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="E53" s="18">
-        <v>45200</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>123</v>
+        <v>44958</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="G53" s="18">
-        <f>DATE(YEAR(E53),MONTH(E53)+4,DAY(E53))</f>
+        <f>DATE(YEAR(E53)+1,MONTH(E53),DAY(E53))</f>
         <v>45323</v>
       </c>
       <c r="H53" s="16" t="s">
@@ -3030,181 +3028,181 @@
     </row>
     <row r="54" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="C54" s="32" t="s">
-        <v>250</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>222</v>
+        <v>44</v>
+      </c>
+      <c r="C54" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>247</v>
       </c>
       <c r="E54" s="18">
-        <v>45200</v>
+        <v>44986</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G54" s="18">
-        <f>DATE(YEAR(E54),MONTH(E54)+4,DAY(E54))</f>
-        <v>45323</v>
+        <f>DATE(YEAR(E54)+1,MONTH(E54),DAY(E54))</f>
+        <v>45352</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="D55" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="E55" s="18">
-        <v>45139</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>221</v>
+      <c r="A55" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E55" s="43">
+        <v>45017</v>
+      </c>
+      <c r="F55" s="44" t="s">
+        <v>124</v>
       </c>
       <c r="G55" s="18">
-        <f>DATE(YEAR(E55),MONTH(E55)+6,DAY(E55))</f>
-        <v>45323</v>
+        <f>DATE(YEAR(E55)+1,MONTH(E55),DAY(E55))</f>
+        <v>45383</v>
       </c>
       <c r="H55" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="C56" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="E56" s="18">
-        <v>44958</v>
-      </c>
-      <c r="F56" s="16" t="s">
+      <c r="A56" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="43">
+        <v>45047</v>
+      </c>
+      <c r="F56" s="44" t="s">
         <v>124</v>
       </c>
       <c r="G56" s="18">
         <f>DATE(YEAR(E56)+1,MONTH(E56),DAY(E56))</f>
-        <v>45323</v>
+        <v>45413</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="31" t="s">
-        <v>297</v>
-      </c>
-      <c r="D57" s="23" t="s">
-        <v>248</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="17"/>
       <c r="E57" s="18">
-        <v>44986</v>
-      </c>
-      <c r="F57" s="19" t="s">
+        <v>45078</v>
+      </c>
+      <c r="F57" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G57" s="18">
         <f>DATE(YEAR(E57)+1,MONTH(E57),DAY(E57))</f>
-        <v>45352</v>
+        <v>45444</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="E58" s="22">
-        <v>45017</v>
-      </c>
-      <c r="F58" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C58" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="D58" s="45" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" s="46">
+        <v>45078</v>
+      </c>
+      <c r="F58" s="21" t="s">
         <v>124</v>
       </c>
       <c r="G58" s="18">
         <f>DATE(YEAR(E58)+1,MONTH(E58),DAY(E58))</f>
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>203</v>
+        <v>69</v>
+      </c>
+      <c r="C59" s="31" t="s">
+        <v>237</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>203</v>
+        <v>236</v>
       </c>
       <c r="E59" s="18">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="F59" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G59" s="18">
         <f>DATE(YEAR(E59)+1,MONTH(E59),DAY(E59))</f>
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D60" s="17"/>
+        <v>237</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>236</v>
+      </c>
       <c r="E60" s="18">
         <v>45078</v>
       </c>
-      <c r="F60" s="16" t="s">
+      <c r="F60" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G60" s="18">
@@ -3212,23 +3210,23 @@
         <v>45444</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>142</v>
+        <v>192</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>143</v>
+        <v>275</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>303</v>
+        <v>235</v>
       </c>
       <c r="D61" s="33" t="s">
-        <v>302</v>
-      </c>
-      <c r="E61" s="34">
+        <v>234</v>
+      </c>
+      <c r="E61" s="18">
         <v>45078</v>
       </c>
       <c r="F61" s="16" t="s">
@@ -3239,21 +3237,21 @@
         <v>45444</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>236</v>
+        <v>300</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>140</v>
       </c>
       <c r="E62" s="18">
         <v>45078</v>
@@ -3266,21 +3264,21 @@
         <v>45444</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="D63" s="17" t="s">
-        <v>236</v>
+        <v>283</v>
+      </c>
+      <c r="C63" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="D63" s="31" t="s">
+        <v>298</v>
       </c>
       <c r="E63" s="18">
         <v>45078</v>
@@ -3293,85 +3291,85 @@
         <v>45444</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="C64" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="D64" s="33" t="s">
-        <v>234</v>
+        <v>189</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>118</v>
       </c>
       <c r="E64" s="18">
-        <v>45078</v>
+        <v>45139</v>
       </c>
       <c r="F64" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G64" s="18">
         <f>DATE(YEAR(E64)+1,MONTH(E64),DAY(E64))</f>
-        <v>45444</v>
+        <v>45505</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C65" s="31" t="s">
-        <v>301</v>
-      </c>
-      <c r="D65" s="23" t="s">
-        <v>140</v>
+        <v>73</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>118</v>
       </c>
       <c r="E65" s="18">
-        <v>45078</v>
+        <v>45139</v>
       </c>
       <c r="F65" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G65" s="18">
         <f>DATE(YEAR(E65)+1,MONTH(E65),DAY(E65))</f>
-        <v>45444</v>
+        <v>45505</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="C66" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D66" s="31" t="s">
-        <v>299</v>
+        <v>282</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>112</v>
       </c>
       <c r="E66" s="18">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="F66" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G66" s="18">
         <f>DATE(YEAR(E66)+1,MONTH(E66),DAY(E66))</f>
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="H66" s="16" t="s">
         <v>179</v>
@@ -3379,56 +3377,56 @@
     </row>
     <row r="67" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
-        <v>188</v>
+        <v>30</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C67" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="D67" s="23" t="s">
-        <v>118</v>
+        <v>285</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>111</v>
       </c>
       <c r="E67" s="18">
-        <v>45139</v>
-      </c>
-      <c r="F67" s="16" t="s">
+        <v>45170</v>
+      </c>
+      <c r="F67" s="19" t="s">
         <v>124</v>
       </c>
       <c r="G67" s="18">
         <f>DATE(YEAR(E67)+1,MONTH(E67),DAY(E67))</f>
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>118</v>
+        <v>284</v>
+      </c>
+      <c r="C68" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="E68" s="18">
-        <v>45139</v>
-      </c>
-      <c r="F68" s="19" t="s">
+        <v>45170</v>
+      </c>
+      <c r="F68" s="16" t="s">
         <v>124</v>
       </c>
       <c r="G68" s="18">
         <f>DATE(YEAR(E68)+1,MONTH(E68),DAY(E68))</f>
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3494,7 +3492,7 @@
         <v>15</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
@@ -3588,7 +3586,7 @@
         <v>12</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>13</v>
@@ -3680,7 +3678,7 @@
         <v>141</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>135</v>
@@ -3731,7 +3729,7 @@
         <v>67</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D82" s="17" t="s">
         <v>116</v>
@@ -3811,114 +3809,116 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D51" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C49" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C39" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C60" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D48" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C46" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C21" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C57" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
     <hyperlink ref="C71" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
     <hyperlink ref="C81" r:id="rId7" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
     <hyperlink ref="D74" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C58" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D31" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D32" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C55" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D26" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
     <hyperlink ref="D9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="D23" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D28" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
     <hyperlink ref="D10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D44" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D47" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D27" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="D48" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D42" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D15" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D14" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D41" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="D38" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D44" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D67" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D66" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="D45" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="D24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="D32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
     <hyperlink ref="D4" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
     <hyperlink ref="D5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
     <hyperlink ref="D82" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
     <hyperlink ref="D71" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="D46" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D16" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="D41" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D29" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D43" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D23" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
     <hyperlink ref="D78" r:id="rId33" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
     <hyperlink ref="D70" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
     <hyperlink ref="C70" r:id="rId35" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
     <hyperlink ref="D12" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
     <hyperlink ref="D13" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C32" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D37" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C27" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D19" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
     <hyperlink ref="D7" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D36" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C51" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="D49" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D65" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D58" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D68" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="D18" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C48" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="D62" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D55" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D65" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
     <hyperlink ref="C80" r:id="rId47" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
     <hyperlink ref="C84" r:id="rId48" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
-    <hyperlink ref="D56" r:id="rId49" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
-    <hyperlink ref="C22" r:id="rId50" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
+    <hyperlink ref="D53" r:id="rId49" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
+    <hyperlink ref="C15" r:id="rId50" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
     <hyperlink ref="D75" r:id="rId51" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
     <hyperlink ref="C75" r:id="rId52" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
     <hyperlink ref="D73" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
     <hyperlink ref="C73" r:id="rId54" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
     <hyperlink ref="C78" r:id="rId55" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
-    <hyperlink ref="D45" r:id="rId56" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
-    <hyperlink ref="D28" r:id="rId57" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
-    <hyperlink ref="D55" r:id="rId58" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
+    <hyperlink ref="D42" r:id="rId56" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
+    <hyperlink ref="D68" r:id="rId57" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
+    <hyperlink ref="D52" r:id="rId58" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
     <hyperlink ref="C79" r:id="rId59" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
     <hyperlink ref="C9" r:id="rId60" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
-    <hyperlink ref="D20" r:id="rId61" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
-    <hyperlink ref="D34" r:id="rId62" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
-    <hyperlink ref="C68" r:id="rId63" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="D53" r:id="rId64" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C27" r:id="rId65" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D35" r:id="rId66" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="D37" r:id="rId61" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
+    <hyperlink ref="D30" r:id="rId62" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
+    <hyperlink ref="C65" r:id="rId63" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
+    <hyperlink ref="D50" r:id="rId64" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C66" r:id="rId65" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
+    <hyperlink ref="D17" r:id="rId66" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
     <hyperlink ref="C83" r:id="rId67" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
-    <hyperlink ref="D43" r:id="rId68" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C31" r:id="rId69" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
-    <hyperlink ref="D59" r:id="rId70" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
+    <hyperlink ref="D40" r:id="rId68" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
+    <hyperlink ref="C26" r:id="rId69" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="D56" r:id="rId70" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
     <hyperlink ref="C2" r:id="rId71" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D54" r:id="rId72" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="D51" r:id="rId72" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
     <hyperlink ref="D79" r:id="rId73" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
     <hyperlink ref="D81" r:id="rId74" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
     <hyperlink ref="D83" r:id="rId75" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
-    <hyperlink ref="C44" r:id="rId76" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D17" r:id="rId77" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D30" r:id="rId78" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C17" r:id="rId79" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C16" r:id="rId80" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C18" r:id="rId81" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C37" r:id="rId82" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C41" r:id="rId76" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
+    <hyperlink ref="D34" r:id="rId77" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D25" r:id="rId78" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C34" r:id="rId79" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C33" r:id="rId80" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C35" r:id="rId81" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C19" r:id="rId82" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
     <hyperlink ref="C5" r:id="rId83" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="C56" r:id="rId84" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
-    <hyperlink ref="D38" r:id="rId85" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
+    <hyperlink ref="C53" r:id="rId84" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
+    <hyperlink ref="D20" r:id="rId85" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
     <hyperlink ref="C6" r:id="rId86" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
-    <hyperlink ref="D19" r:id="rId87" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
-    <hyperlink ref="C20" r:id="rId88" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
-    <hyperlink ref="C15" r:id="rId89" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
-    <hyperlink ref="C23" r:id="rId90" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
-    <hyperlink ref="D64" r:id="rId91" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
-    <hyperlink ref="C64" r:id="rId92" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
-    <hyperlink ref="C62" r:id="rId93" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
-    <hyperlink ref="C53" r:id="rId94" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
-    <hyperlink ref="C35" r:id="rId95" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
-    <hyperlink ref="C47" r:id="rId96" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
-    <hyperlink ref="C54" r:id="rId97" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
-    <hyperlink ref="C45" r:id="rId98" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
-    <hyperlink ref="C50" r:id="rId99" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
-    <hyperlink ref="D61" r:id="rId100" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
-    <hyperlink ref="D66" r:id="rId101" xr:uid="{6F00F671-AF53-4F92-BB47-E9B0FDCBC1D9}"/>
-    <hyperlink ref="C40" r:id="rId102" xr:uid="{7FE65590-98DE-4007-9308-9C1A738E8F44}"/>
-    <hyperlink ref="C65" r:id="rId103" xr:uid="{9E939E47-ECE0-46F0-82D1-02FE6E974157}"/>
+    <hyperlink ref="D36" r:id="rId87" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
+    <hyperlink ref="C37" r:id="rId88" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
+    <hyperlink ref="C32" r:id="rId89" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
+    <hyperlink ref="C28" r:id="rId90" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
+    <hyperlink ref="D61" r:id="rId91" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
+    <hyperlink ref="C61" r:id="rId92" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
+    <hyperlink ref="C59" r:id="rId93" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
+    <hyperlink ref="C50" r:id="rId94" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
+    <hyperlink ref="C17" r:id="rId95" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
+    <hyperlink ref="C44" r:id="rId96" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
+    <hyperlink ref="C51" r:id="rId97" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
+    <hyperlink ref="C42" r:id="rId98" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
+    <hyperlink ref="C47" r:id="rId99" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
+    <hyperlink ref="D58" r:id="rId100" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
+    <hyperlink ref="D63" r:id="rId101" xr:uid="{6F00F671-AF53-4F92-BB47-E9B0FDCBC1D9}"/>
+    <hyperlink ref="C22" r:id="rId102" xr:uid="{7FE65590-98DE-4007-9308-9C1A738E8F44}"/>
+    <hyperlink ref="C62" r:id="rId103" xr:uid="{9E939E47-ECE0-46F0-82D1-02FE6E974157}"/>
+    <hyperlink ref="C31" r:id="rId104" xr:uid="{0693917C-81AF-4242-A944-450CAD3D7797}"/>
+    <hyperlink ref="D35" r:id="rId105" xr:uid="{AD237274-5FC6-4AD7-A77A-83DD508576FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId104"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId106"/>
   <tableParts count="1">
-    <tablePart r:id="rId105"/>
+    <tablePart r:id="rId107"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
smart meters, rhi, daily demand, chp
</commit_message>
<xml_diff>
--- a/Structure/Sources.xlsx
+++ b/Structure/Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Energy Stats\Documents\Github\Scottish-Energy-Statistics-Hub\Structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588BF00D-5695-4972-B3A7-536B3882DC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DE77A3-9A00-4717-A013-1D2263BA58E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>Eurostat: Share of renewable energy in gross final energy consumption</t>
   </si>
   <si>
-    <t>https://appsso.eurostat.ec.europa.eu/nui/show.do?dataset=nrg_bal_c&amp;lang=en</t>
-  </si>
-  <si>
     <t>HMRCTrade</t>
   </si>
   <si>
@@ -754,12 +751,6 @@
     <t>https://www.ofgem.gov.uk/sites/default/files/2022-08/Default_tariff_cap_level_v1.13.xlsx</t>
   </si>
   <si>
-    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1107320/Combined_Heat_and_Power_in_the_regions_2021_-_data_tables.xlsx</t>
-  </si>
-  <si>
-    <t>https://www.gov.uk/government/statistics/energy-trends-september-2022-special-feature-article-combined-heat-and-power-in-the-regions</t>
-  </si>
-  <si>
     <t>https://www.gov.uk/government/statistics/household-energy-efficiency-statistics-headline-release-september-2022</t>
   </si>
   <si>
@@ -769,12 +760,6 @@
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1115149/subnational_electricity_consumption_statistics_2005-2020.xlsx</t>
   </si>
   <si>
-    <t>https://www.ofgem.gov.uk/publications/domestic-renewable-heat-incentive-drhi-quarterly-report-issue-34</t>
-  </si>
-  <si>
-    <t>https://www.gov.uk/government/statistics/rhi-monthly-deployment-data-september-2022-quarterly-edition</t>
-  </si>
-  <si>
     <t>https://oeuk.org.uk/wp-content/uploads/2022/11/OEUK-Workforce-Insight-2022.pdf</t>
   </si>
   <si>
@@ -935,6 +920,21 @@
   </si>
   <si>
     <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1187087/Subnational_total_final_consumption_2005_2021.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.ofgem.gov.uk/sites/default/files/2023-05/Domestic%20Renewable%20Heat%20Incentive%20%28DRHI%29%20Quarterly%20Report%20Issue%2036.pdf</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/statistics/rhi-monthly-deployment-data-march-2023-quarterly-edition</t>
+  </si>
+  <si>
+    <t>https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/1174226/DUKES_7.8.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.gov.uk/government/statistics/combined-heat-and-power-chapter-7-digest-of-united-kingdom-energy-statistics-dukes</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/eurostat/databrowser/view/nrg_bal_c__custom_8119843/default/table?lang=en</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1110,6 +1110,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1590,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,10 +1617,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
         <v>98</v>
-      </c>
-      <c r="D1" t="s">
-        <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1625,62 +1629,62 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="15">
         <v>43862</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G2" s="15">
         <f>DATE(YEAR(E2)+1,MONTH(E2),DAY(E2))</f>
         <v>44228</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>177</v>
-      </c>
       <c r="D3" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="25">
         <v>44197</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="18">
         <f>DATE(YEAR(E3)+1,MONTH(E3),DAY(E3))</f>
         <v>44562</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1688,26 +1692,26 @@
         <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="8">
         <v>44562</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G4" s="18">
         <f>DATE(YEAR(E4),MONTH(E4)+3,DAY(E4))</f>
         <v>44652</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1715,105 +1719,105 @@
         <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="8">
         <v>44562</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" s="18">
         <f>DATE(YEAR(E5),MONTH(E5)+3,DAY(E5))</f>
         <v>44652</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>172</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E6" s="8">
         <v>44743</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" s="8">
         <f>DATE(YEAR(E6),MONTH(E6)+3,DAY(E6))</f>
         <v>44835</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="8">
         <v>44743</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G7" s="8">
         <f>DATE(YEAR(E7),MONTH(E7)+3,DAY(E7))</f>
         <v>44835</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>131</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>132</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="37">
         <v>44652</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" s="37">
         <f t="shared" ref="G8:G13" si="0">DATE(YEAR(E8)+1,MONTH(E8),DAY(E8))</f>
         <v>45017</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -1821,26 +1825,26 @@
         <v>7</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="37">
         <v>44743</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G9" s="37">
         <f t="shared" si="0"/>
         <v>45108</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -1848,26 +1852,26 @@
         <v>19</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C10" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="D10" s="40" t="s">
         <v>193</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>194</v>
       </c>
       <c r="E10" s="37">
         <v>44743</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G10" s="37">
         <f t="shared" si="0"/>
         <v>45108</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -1875,26 +1879,26 @@
         <v>8</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" s="37">
         <v>44743</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G11" s="37">
         <f t="shared" si="0"/>
         <v>45108</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -1902,26 +1906,26 @@
         <v>9</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" s="37">
         <v>44743</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G12" s="37">
         <f t="shared" si="0"/>
         <v>45108</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
@@ -1929,342 +1933,342 @@
         <v>10</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="37">
         <v>44743</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G13" s="37">
         <f t="shared" si="0"/>
         <v>45108</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="C14" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="18">
         <v>45078</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G14" s="18">
         <f>DATE(YEAR(E14),MONTH(E14)+3,DAY(E14))</f>
         <v>45170</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>303</v>
+      </c>
+      <c r="E15" s="45">
+        <v>45200</v>
+      </c>
+      <c r="F15" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="45">
+        <f>DATE(YEAR(E15)+1,MONTH(E15),DAY(E15))</f>
+        <v>45566</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="E16" s="45">
         <v>45170</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="G15" s="18">
-        <f>DATE(YEAR(E15),MONTH(E15)+3,DAY(E15))</f>
-        <v>45261</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="E16" s="18">
-        <v>44805</v>
-      </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="G16" s="18">
-        <f>DATE(YEAR(E16)+1,MONTH(E16),DAY(E16))</f>
-        <v>45170</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>265</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" s="18">
-        <v>45170</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" s="18">
-        <f>DATE(YEAR(E17),MONTH(E17)+1,DAY(E17))</f>
+      <c r="G16" s="45">
+        <f>DATE(YEAR(E16),MONTH(E16)+1,DAY(E16))</f>
         <v>45200</v>
       </c>
-      <c r="H17" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>303</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" s="18">
-        <v>45170</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" s="18">
-        <f>DATE(YEAR(E18),MONTH(E18)+1,DAY(E18))</f>
+      <c r="H16" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="E17" s="45">
+        <v>45108</v>
+      </c>
+      <c r="F17" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="G17" s="45">
+        <f>DATE(YEAR(E17),MONTH(E17)+3,DAY(E17))</f>
         <v>45200</v>
       </c>
-      <c r="H18" s="16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>216</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" s="18">
+      <c r="H17" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45">
+        <v>45108</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="45">
+        <f>DATE(YEAR(E18),MONTH(E18)+3,DAY(E18))</f>
         <v>45200</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" s="18">
-        <f>DATE(YEAR(E19),MONTH(E19)+1,DAY(E19))</f>
-        <v>45231</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>179</v>
+      <c r="H18" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>289</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="45">
+        <v>45108</v>
+      </c>
+      <c r="F19" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="G19" s="45">
+        <f>DATE(YEAR(E19),MONTH(E19)+3,DAY(E19))</f>
+        <v>45200</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>232</v>
+        <v>298</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="E20" s="18">
-        <v>45108</v>
+        <v>45200</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G20" s="18">
-        <f>DATE(YEAR(E20),MONTH(E20)+3,DAY(E20))</f>
-        <v>45200</v>
+        <f>DATE(YEAR(E20),MONTH(E20)+1,DAY(E20))</f>
+        <v>45231</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D21" s="17"/>
+        <v>261</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>104</v>
+      </c>
       <c r="E21" s="18">
-        <v>45108</v>
+        <v>45200</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G21" s="18">
-        <f>DATE(YEAR(E21),MONTH(E21)+3,DAY(E21))</f>
-        <v>45200</v>
+        <f>DATE(YEAR(E21),MONTH(E21)+1,DAY(E21))</f>
+        <v>45231</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>294</v>
-      </c>
-      <c r="D22" s="17"/>
+        <v>64</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>125</v>
+      </c>
       <c r="E22" s="18">
-        <v>45108</v>
+        <v>44866</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>123</v>
       </c>
       <c r="G22" s="18">
-        <f>DATE(YEAR(E22),MONTH(E22)+3,DAY(E22))</f>
-        <v>45200</v>
+        <f>DATE(YEAR(E22)+1,MONTH(E22),DAY(E22))</f>
+        <v>45231</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>65</v>
+        <v>281</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>251</v>
+        <v>204</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="E23" s="18">
         <v>44866</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G23" s="18">
         <f>DATE(YEAR(E23)+1,MONTH(E23),DAY(E23))</f>
         <v>45231</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>33</v>
+        <v>148</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>114</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="17"/>
       <c r="E24" s="18">
-        <v>44866</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>124</v>
+        <v>45170</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="G24" s="18">
-        <f>DATE(YEAR(E24)+1,MONTH(E24),DAY(E24))</f>
-        <v>45231</v>
+        <f t="shared" ref="G24:G39" si="1">DATE(YEAR(E24),MONTH(E24)+3,DAY(E24))</f>
+        <v>45261</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E25" s="1">
         <v>45170</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G25" s="18">
-        <f t="shared" ref="G25:G39" si="1">DATE(YEAR(E25),MONTH(E25)+3,DAY(E25))</f>
+        <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2272,26 +2276,26 @@
         <v>4</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E26" s="1">
         <v>45170</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G26" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2299,26 +2303,26 @@
         <v>5</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E27" s="1">
         <v>45170</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G27" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2326,26 +2330,26 @@
         <v>17</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E28" s="18">
         <v>45170</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G28" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2353,26 +2357,26 @@
         <v>24</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E29" s="18">
         <v>45170</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G29" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2380,26 +2384,26 @@
         <v>25</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30" s="18">
         <v>45170</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G30" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2407,26 +2411,26 @@
         <v>35</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E31" s="1">
         <v>45170</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G31" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2434,26 +2438,26 @@
         <v>34</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E32" s="1">
         <v>45170</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G32" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2461,107 +2465,107 @@
         <v>22</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E33" s="18">
         <v>45170</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G33" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="B34" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>226</v>
-      </c>
       <c r="D34" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E34" s="1">
         <v>45170</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G34" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B35" t="s">
+        <v>262</v>
+      </c>
+      <c r="C35" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="B35" t="s">
-        <v>267</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>231</v>
-      </c>
       <c r="D35" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E35" s="18">
         <v>45170</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G35" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E36" s="18">
         <v>45170</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G36" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2569,26 +2573,26 @@
         <v>23</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E37" s="18">
         <v>45170</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G37" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2596,26 +2600,26 @@
         <v>26</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E38" s="18">
         <v>45170</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G38" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2623,26 +2627,26 @@
         <v>27</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E39" s="18">
         <v>45170</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G39" s="18">
         <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2650,26 +2654,26 @@
         <v>14</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E40" s="18">
         <v>44896</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G40" s="18">
         <f t="shared" ref="G40:G47" si="2">DATE(YEAR(E40)+1,MONTH(E40),DAY(E40))</f>
         <v>45261</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2677,53 +2681,53 @@
         <v>20</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" s="18">
         <v>44896</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G41" s="18">
         <f t="shared" si="2"/>
         <v>45261</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D42" s="23" t="s">
         <v>158</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>259</v>
-      </c>
-      <c r="C42" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>159</v>
       </c>
       <c r="E42" s="18">
         <v>44896</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G42" s="18">
         <f t="shared" si="2"/>
         <v>45261</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -2731,26 +2735,26 @@
         <v>11</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E43" s="22">
         <v>44896</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G43" s="22">
         <f t="shared" si="2"/>
         <v>45261</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2758,26 +2762,26 @@
         <v>29</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E44" s="18">
         <v>44896</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G44" s="22">
         <f t="shared" si="2"/>
         <v>45261</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2785,26 +2789,26 @@
         <v>32</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E45" s="18">
         <v>44896</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G45" s="18">
         <f t="shared" si="2"/>
         <v>45261</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2815,50 +2819,50 @@
         <v>48</v>
       </c>
       <c r="C46" s="41" t="s">
-        <v>49</v>
+        <v>304</v>
       </c>
       <c r="D46" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E46" s="18">
         <v>44927</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G46" s="18">
         <f t="shared" si="2"/>
         <v>45292</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="C47" s="31" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E47" s="18">
         <v>44927</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G47" s="18">
         <f t="shared" si="2"/>
         <v>45292</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2869,7 +2873,7 @@
         <v>41</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>42</v>
@@ -2878,41 +2882,41 @@
         <v>44927</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G48" s="18">
         <f>DATE(YEAR(E48),MONTH(E48)+12,DAY(E48))</f>
         <v>45292</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>81</v>
-      </c>
       <c r="C49" s="17" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E49" s="18">
         <v>44927</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G49" s="18">
         <f>DATE(YEAR(E49)+1,MONTH(E49),DAY(E49))</f>
         <v>45292</v>
       </c>
       <c r="H49" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2920,107 +2924,107 @@
         <v>28</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E50" s="18">
         <v>45200</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G50" s="18">
         <f>DATE(YEAR(E50),MONTH(E50)+4,DAY(E50))</f>
         <v>45323</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="16" t="s">
-        <v>170</v>
-      </c>
       <c r="C51" s="32" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E51" s="18">
         <v>45200</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G51" s="18">
         <f>DATE(YEAR(E51),MONTH(E51)+4,DAY(E51))</f>
         <v>45323</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="C52" s="33" t="s">
+        <v>242</v>
+      </c>
+      <c r="D52" s="23" t="s">
         <v>162</v>
-      </c>
-      <c r="C52" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>163</v>
       </c>
       <c r="E52" s="18">
         <v>45139</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G52" s="18">
         <f>DATE(YEAR(E52),MONTH(E52)+6,DAY(E52))</f>
         <v>45323</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C53" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B53" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="C53" s="32" t="s">
-        <v>148</v>
-      </c>
       <c r="D53" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E53" s="18">
         <v>44958</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G53" s="18">
         <f t="shared" ref="G53:G68" si="3">DATE(YEAR(E53)+1,MONTH(E53),DAY(E53))</f>
         <v>45323</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3031,50 +3035,50 @@
         <v>44</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E54" s="18">
         <v>44986</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G54" s="18">
         <f t="shared" si="3"/>
         <v>45352</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B55" s="16" t="s">
-        <v>97</v>
-      </c>
       <c r="C55" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E55" s="18">
         <v>45017</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G55" s="18">
         <f t="shared" si="3"/>
         <v>45383</v>
       </c>
       <c r="H55" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3085,183 +3089,183 @@
         <v>46</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E56" s="18">
         <v>45047</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G56" s="18">
         <f t="shared" si="3"/>
         <v>45413</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="C57" s="17" t="s">
         <v>62</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="D57" s="17"/>
       <c r="E57" s="18">
         <v>45078</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G57" s="18">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B58" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="21" t="s">
-        <v>143</v>
-      </c>
       <c r="C58" s="42" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D58" s="42" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E58" s="43">
         <v>45078</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G58" s="18">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B59" s="16" t="s">
-        <v>69</v>
-      </c>
       <c r="C59" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E59" s="18">
         <v>45078</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G59" s="18">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H59" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B60" s="16" t="s">
-        <v>71</v>
-      </c>
       <c r="C60" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E60" s="18">
         <v>45078</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G60" s="18">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H60" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C61" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D61" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E61" s="18">
         <v>45078</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G61" s="18">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H61" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="16" t="s">
-        <v>60</v>
-      </c>
       <c r="C62" s="31" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E62" s="18">
         <v>45078</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G62" s="18">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3269,80 +3273,80 @@
         <v>18</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E63" s="18">
         <v>45078</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G63" s="18">
         <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H63" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="C64" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="C64" s="23" t="s">
-        <v>190</v>
-      </c>
       <c r="D64" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E64" s="18">
         <v>45139</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G64" s="18">
         <f t="shared" si="3"/>
         <v>45505</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="C65" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E65" s="18">
         <v>45139</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G65" s="18">
         <f t="shared" si="3"/>
         <v>45505</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3350,26 +3354,26 @@
         <v>31</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E66" s="18">
         <v>45170</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G66" s="18">
         <f t="shared" si="3"/>
         <v>45536</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3377,53 +3381,53 @@
         <v>30</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E67" s="18">
         <v>45170</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G67" s="18">
         <f t="shared" si="3"/>
         <v>45536</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E68" s="18">
         <v>45170</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G68" s="18">
         <f t="shared" si="3"/>
         <v>45536</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3438,50 +3442,50 @@
     </row>
     <row r="70" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D70" s="20" t="s">
         <v>127</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>128</v>
       </c>
       <c r="E70" s="18">
         <v>43435</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G70" s="18"/>
       <c r="H70" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="C71" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C71" s="17" t="s">
-        <v>76</v>
-      </c>
       <c r="D71" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E71" s="18">
         <v>43447</v>
       </c>
       <c r="F71" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3489,7 +3493,7 @@
         <v>15</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>13</v>
@@ -3499,7 +3503,7 @@
         <v>43466</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G72" s="8"/>
       <c r="H72" s="4" t="s">
@@ -3508,46 +3512,46 @@
     </row>
     <row r="73" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C73" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E73" s="15">
         <v>43831</v>
       </c>
       <c r="F73" s="29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C74" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E74" s="18">
         <v>43831</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="16" t="s">
@@ -3556,26 +3560,26 @@
     </row>
     <row r="75" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="C75" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D75" s="14" t="s">
         <v>153</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>154</v>
       </c>
       <c r="E75" s="15">
         <v>43908</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3583,7 +3587,7 @@
         <v>12</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>13</v>
@@ -3593,7 +3597,7 @@
         <v>43916</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="4" t="s">
@@ -3602,10 +3606,10 @@
     </row>
     <row r="77" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="16" t="s">
         <v>86</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>87</v>
       </c>
       <c r="C77" s="17" t="s">
         <v>13</v>
@@ -3615,7 +3619,7 @@
         <v>43950</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G77" s="18"/>
       <c r="H77" s="16" t="s">
@@ -3624,136 +3628,136 @@
     </row>
     <row r="78" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>91</v>
-      </c>
       <c r="C78" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E78" s="18">
         <v>43950</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G78" s="18"/>
       <c r="H78" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="C79" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="D79" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E79" s="8">
         <v>44044</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G79" s="8"/>
       <c r="H79" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E80" s="8">
         <v>44166</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G80" s="8"/>
       <c r="H80" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="16" t="s">
-        <v>89</v>
-      </c>
       <c r="C81" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E81" s="18">
         <v>44166</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G81" s="18"/>
       <c r="H81" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>67</v>
-      </c>
       <c r="C82" s="17" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E82" s="18">
         <v>44986</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G82" s="18"/>
       <c r="H82" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="C83" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D83" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>208</v>
       </c>
       <c r="E83" s="8">
         <v>44256</v>
@@ -3761,33 +3765,33 @@
       <c r="F83" s="4"/>
       <c r="G83" s="8"/>
       <c r="H83" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8"/>
       <c r="F84" s="4"/>
       <c r="G84" s="8"/>
       <c r="H84" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>13</v>
@@ -3807,115 +3811,112 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D48" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C46" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C21" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C57" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C71" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C81" r:id="rId7" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D74" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C55" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="D26" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="D27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="D9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="D28" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="D10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="D41" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="D38" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="D39" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="D44" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="D67" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="D66" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="D45" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="D24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="D32" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="D31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="D4" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="D5" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="D82" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="D71" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="D29" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="D43" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="D23" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="D78" r:id="rId33" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="D70" r:id="rId34" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C70" r:id="rId35" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="D12" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="D13" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C27" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="D19" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="D7" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="D18" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C48" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="D46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="D62" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="D55" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="D65" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="C80" r:id="rId47" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
-    <hyperlink ref="C84" r:id="rId48" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
-    <hyperlink ref="D53" r:id="rId49" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
-    <hyperlink ref="C15" r:id="rId50" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
-    <hyperlink ref="D75" r:id="rId51" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
-    <hyperlink ref="C75" r:id="rId52" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
-    <hyperlink ref="D73" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C73" r:id="rId54" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
-    <hyperlink ref="C78" r:id="rId55" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
-    <hyperlink ref="D42" r:id="rId56" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
-    <hyperlink ref="D68" r:id="rId57" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
-    <hyperlink ref="D52" r:id="rId58" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
-    <hyperlink ref="C79" r:id="rId59" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
-    <hyperlink ref="C9" r:id="rId60" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
-    <hyperlink ref="D37" r:id="rId61" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
-    <hyperlink ref="D30" r:id="rId62" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
-    <hyperlink ref="C65" r:id="rId63" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
-    <hyperlink ref="D50" r:id="rId64" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
-    <hyperlink ref="C66" r:id="rId65" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
-    <hyperlink ref="D17" r:id="rId66" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
-    <hyperlink ref="C83" r:id="rId67" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
-    <hyperlink ref="D40" r:id="rId68" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
-    <hyperlink ref="C26" r:id="rId69" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
-    <hyperlink ref="D56" r:id="rId70" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
-    <hyperlink ref="C2" r:id="rId71" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
-    <hyperlink ref="D51" r:id="rId72" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
-    <hyperlink ref="D79" r:id="rId73" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
-    <hyperlink ref="D81" r:id="rId74" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
-    <hyperlink ref="D83" r:id="rId75" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
-    <hyperlink ref="C41" r:id="rId76" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
-    <hyperlink ref="D34" r:id="rId77" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
-    <hyperlink ref="D25" r:id="rId78" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
-    <hyperlink ref="C34" r:id="rId79" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
-    <hyperlink ref="C33" r:id="rId80" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
-    <hyperlink ref="C35" r:id="rId81" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
-    <hyperlink ref="C19" r:id="rId82" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
-    <hyperlink ref="C5" r:id="rId83" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
-    <hyperlink ref="C53" r:id="rId84" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
-    <hyperlink ref="D20" r:id="rId85" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
-    <hyperlink ref="C6" r:id="rId86" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
-    <hyperlink ref="D36" r:id="rId87" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
-    <hyperlink ref="C37" r:id="rId88" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
-    <hyperlink ref="C32" r:id="rId89" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
-    <hyperlink ref="C28" r:id="rId90" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
-    <hyperlink ref="D61" r:id="rId91" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
-    <hyperlink ref="C61" r:id="rId92" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
-    <hyperlink ref="C59" r:id="rId93" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
-    <hyperlink ref="C50" r:id="rId94" xr:uid="{00BB129D-D5A2-40B8-82DE-D729F07874E2}"/>
-    <hyperlink ref="C17" r:id="rId95" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
-    <hyperlink ref="C44" r:id="rId96" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
-    <hyperlink ref="C51" r:id="rId97" xr:uid="{61BEAFD6-8542-4172-94BF-7ACCDCB0C9AB}"/>
-    <hyperlink ref="C42" r:id="rId98" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
-    <hyperlink ref="C47" r:id="rId99" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
-    <hyperlink ref="D58" r:id="rId100" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
-    <hyperlink ref="D63" r:id="rId101" xr:uid="{6F00F671-AF53-4F92-BB47-E9B0FDCBC1D9}"/>
-    <hyperlink ref="C22" r:id="rId102" xr:uid="{7FE65590-98DE-4007-9308-9C1A738E8F44}"/>
-    <hyperlink ref="C62" r:id="rId103" xr:uid="{9E939E47-ECE0-46F0-82D1-02FE6E974157}"/>
-    <hyperlink ref="C31" r:id="rId104" xr:uid="{0693917C-81AF-4242-A944-450CAD3D7797}"/>
-    <hyperlink ref="D35" r:id="rId105" xr:uid="{AD237274-5FC6-4AD7-A77A-83DD508576FF}"/>
+    <hyperlink ref="C14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C57" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C71" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C81" r:id="rId6" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/12/scottish-house-condition-survey-2019-key-findings/documents/scottish-house-condition-survey-2019-key-findings-tables-figures/scottish-house-condition-survey-2019-key-findings-tables-figures/govscot%3Adocument/scottish-house-condition-survey-2019-key-findings-tables-figures.xlsx" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D74" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C55" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="D26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="D27" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="D9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="D28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="D10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="D41" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="D38" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="D39" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="D44" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="D67" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="D66" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="D45" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="D23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="D32" r:id="rId22" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="D31" r:id="rId23" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="D4" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="D5" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="D82" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="D71" r:id="rId27" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="D43" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="D22" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="D78" r:id="rId32" location="thescottishnationalaccountsprogramme(snap)" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="D70" r:id="rId33" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C70" r:id="rId34" display="https://www.gov.scot/binaries/content/documents/govscot/publications/research-and-analysis/2018/12/scotlands-non-domestic-energy-efficiency-baseline/documents/scotlands-non-domestic-energy-efficiency-baseline/scotlands-non-domestic-energy-efficiency-baseline/govscot%3Adocument/00544110.pdf?forceDownload=true" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="D12" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="D13" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C27" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="D21" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="D7" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="D20" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C48" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="D46" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="D62" r:id="rId43" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="D55" r:id="rId44" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="D65" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="C80" r:id="rId46" xr:uid="{52E842E9-D247-4F78-88A0-217490DB26DC}"/>
+    <hyperlink ref="C84" r:id="rId47" xr:uid="{74E28334-8574-4123-8AF4-3B16A49B29E4}"/>
+    <hyperlink ref="D53" r:id="rId48" xr:uid="{FEB7188F-6069-4320-A732-0D5E6CE94251}"/>
+    <hyperlink ref="C24" r:id="rId49" location="thumbchart-c23042756505310535-n95432" display="https://www.ofgem.gov.uk/data-portal/retail-market-indicators - thumbchart-c23042756505310535-n95432" xr:uid="{B9F0501D-AFB8-4B4D-953F-E3BC7D924F18}"/>
+    <hyperlink ref="D75" r:id="rId50" xr:uid="{C4988921-2E24-4390-A3C9-361CEE63651F}"/>
+    <hyperlink ref="C75" r:id="rId51" xr:uid="{CE0718F8-A335-45DA-B5B6-2421993AC8CB}"/>
+    <hyperlink ref="D73" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C73" r:id="rId53" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2019/05/scottish-national-accounts-programme-whole-of-scotland-economic-accounts-project/documents/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/development-of-supply--use-satellite-accounts-for-extra-regio-economic-activities/govscot%3Adocument/Development%2Bof%2BSupply%2B%2526%2BUse%2BSatellite%2BAccounts%2Bfor%2BExtra-Regio%2BEconomic%2BActivities.xlsx" xr:uid="{1E1171F7-3FA7-4DA0-AF12-73B304849A8E}"/>
+    <hyperlink ref="C78" r:id="rId54" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2020/04/gdp-quarterly-national-accounts-for-scotland-2019-q4/documents/other-quarterly-national-accounts-summary-tables%5B2%5D/other-quarterly-national-accounts-summary-tables/govscot%3Adocument/%25282%2529%2BQNAS%2B2019%2BQ4%2B--%2BOther%2BNational%2BAccounts%2BSummary%2BTables.xlsx" xr:uid="{0C8A3909-BDB7-4B5E-8E78-079038DEBB87}"/>
+    <hyperlink ref="D42" r:id="rId55" xr:uid="{E22CB7C1-666E-4646-9C00-4EF366985FA6}"/>
+    <hyperlink ref="D68" r:id="rId56" xr:uid="{C15CAB16-DAA4-4A78-A179-22DF9AF423CA}"/>
+    <hyperlink ref="D52" r:id="rId57" xr:uid="{8B65AF1A-CD33-4F88-B1C9-E10EB9EE5FF4}"/>
+    <hyperlink ref="C79" r:id="rId58" xr:uid="{3583A0F4-B6F6-49D3-A2BB-E1CDFB8779A8}"/>
+    <hyperlink ref="C9" r:id="rId59" xr:uid="{34113D8D-8455-4C83-A88E-E572A167879B}"/>
+    <hyperlink ref="D37" r:id="rId60" xr:uid="{C42D263B-7A21-4C4F-AAFE-41FDFE76DA53}"/>
+    <hyperlink ref="D30" r:id="rId61" xr:uid="{4EFECAF4-5CA2-4557-92F4-F13F0A656C5D}"/>
+    <hyperlink ref="C65" r:id="rId62" xr:uid="{C1166389-9A68-4C55-83E9-EB5BD8DADF18}"/>
+    <hyperlink ref="D50" r:id="rId63" xr:uid="{C3B710A7-8E88-451D-9260-4AA730AA1243}"/>
+    <hyperlink ref="C66" r:id="rId64" xr:uid="{BB13BC3C-E626-484C-AA42-B69F61990E6E}"/>
+    <hyperlink ref="D16" r:id="rId65" xr:uid="{73FBBA2B-41BE-4232-BC94-02C4A2A4337B}"/>
+    <hyperlink ref="C83" r:id="rId66" xr:uid="{A927D557-DFDB-4AEC-9C52-943C822A7BE5}"/>
+    <hyperlink ref="D40" r:id="rId67" xr:uid="{5E427227-A3F5-46D0-8ECB-B66F05FAEBD8}"/>
+    <hyperlink ref="C26" r:id="rId68" xr:uid="{6DB047C4-8112-4490-900E-290196538556}"/>
+    <hyperlink ref="D56" r:id="rId69" xr:uid="{67D6AD3A-CFA5-47C4-810A-48270F828F99}"/>
+    <hyperlink ref="C2" r:id="rId70" xr:uid="{4C72A6B4-2143-4394-ACD1-16D3C6165A5F}"/>
+    <hyperlink ref="D51" r:id="rId71" xr:uid="{EA182F35-D107-4521-B8E4-9E0E60BC090E}"/>
+    <hyperlink ref="D79" r:id="rId72" xr:uid="{A67B8192-CA33-4287-8573-5F8945F7CDF9}"/>
+    <hyperlink ref="D81" r:id="rId73" xr:uid="{A4ADEDF4-32C7-4488-98D2-687C6E9BF5A8}"/>
+    <hyperlink ref="D83" r:id="rId74" xr:uid="{DCF7F52D-E031-45FE-92A8-99FFA2843EDB}"/>
+    <hyperlink ref="C41" r:id="rId75" xr:uid="{11A5D28F-2D00-4B9D-9605-5F4934D79928}"/>
+    <hyperlink ref="D34" r:id="rId76" xr:uid="{827D302C-F2CA-4368-96E2-7C5D378EBAE6}"/>
+    <hyperlink ref="D25" r:id="rId77" xr:uid="{CE79BA0C-757C-4235-AD05-E6F068C48C54}"/>
+    <hyperlink ref="C34" r:id="rId78" xr:uid="{BA76B832-6529-4B09-839B-7DA26362F7E2}"/>
+    <hyperlink ref="C33" r:id="rId79" xr:uid="{ECC5282C-1FA2-4F19-91E4-CD4CFCB06235}"/>
+    <hyperlink ref="C35" r:id="rId80" xr:uid="{46D15876-509D-4040-8ACA-A1265F19D3E1}"/>
+    <hyperlink ref="C21" r:id="rId81" xr:uid="{AC152226-69FF-4698-8A05-D7FE289A723A}"/>
+    <hyperlink ref="C5" r:id="rId82" xr:uid="{3000F582-61CB-4173-A59B-870C4FE2AB75}"/>
+    <hyperlink ref="C53" r:id="rId83" xr:uid="{37CFE1F4-0E77-4820-B8D8-DF572D5ECBB2}"/>
+    <hyperlink ref="D17" r:id="rId84" location="quarterlygrossdomesticproduct(gdp)" xr:uid="{74C8EEDC-6067-426A-AE0B-7402E4DFA196}"/>
+    <hyperlink ref="C6" r:id="rId85" xr:uid="{EBBB8C92-CAE7-4603-AEA2-0D438D30DD02}"/>
+    <hyperlink ref="D36" r:id="rId86" xr:uid="{47A29FD3-E1FE-4255-B416-F01539F6BDFE}"/>
+    <hyperlink ref="C37" r:id="rId87" xr:uid="{B54C112E-597A-4409-B9BF-5C0D471D20C6}"/>
+    <hyperlink ref="C32" r:id="rId88" xr:uid="{9629372E-78CB-4510-8C81-0128E1BFBF53}"/>
+    <hyperlink ref="C28" r:id="rId89" xr:uid="{5238C2C1-4095-4C31-BF6E-25170A443699}"/>
+    <hyperlink ref="D61" r:id="rId90" xr:uid="{B0D73686-B77C-4FE1-8404-4CC045E5C7F1}"/>
+    <hyperlink ref="C61" r:id="rId91" xr:uid="{27A6FF43-926C-44C6-897E-8B125E5AD7FA}"/>
+    <hyperlink ref="C59" r:id="rId92" xr:uid="{F58B7D0B-35FB-4A94-A1E6-AF8EB6FB21BF}"/>
+    <hyperlink ref="C16" r:id="rId93" xr:uid="{697F69A6-80B5-43A3-B48F-4C6250BA39A2}"/>
+    <hyperlink ref="C44" r:id="rId94" xr:uid="{5B6E2066-FB6E-45C7-8042-6748245C029E}"/>
+    <hyperlink ref="C42" r:id="rId95" xr:uid="{B920E25B-4454-4410-BB00-101F50B92D85}"/>
+    <hyperlink ref="C47" r:id="rId96" display="https://www.gov.scot/binaries/content/documents/govscot/publications/statistics/2023/01/oil-and-gas-production-statistics/documents/oil-and-gas-physical-commodity-balances-1998-2021/oil-and-gas-physical-commodity-balances-1998-2021/govscot%3Adocument/Oil%2Band%2BGas%2BPhysical%2BCommodity%2BBalances%2B1998-2021.xlsx" xr:uid="{90BD01A2-8C2E-486E-A841-A90C2D18C89F}"/>
+    <hyperlink ref="D58" r:id="rId97" xr:uid="{0E1A9E40-DD7A-451D-8162-15B332F5BFF3}"/>
+    <hyperlink ref="D63" r:id="rId98" xr:uid="{6F00F671-AF53-4F92-BB47-E9B0FDCBC1D9}"/>
+    <hyperlink ref="C19" r:id="rId99" xr:uid="{7FE65590-98DE-4007-9308-9C1A738E8F44}"/>
+    <hyperlink ref="C62" r:id="rId100" xr:uid="{9E939E47-ECE0-46F0-82D1-02FE6E974157}"/>
+    <hyperlink ref="C31" r:id="rId101" xr:uid="{0693917C-81AF-4242-A944-450CAD3D7797}"/>
+    <hyperlink ref="D35" r:id="rId102" xr:uid="{AD237274-5FC6-4AD7-A77A-83DD508576FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId106"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId103"/>
   <tableParts count="1">
-    <tablePart r:id="rId107"/>
+    <tablePart r:id="rId104"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>